<commit_message>
Update Dicionário | Update modelo-fisico
</commit_message>
<xml_diff>
--- a/dicionario_tabelas/dicionario.xlsx
+++ b/dicionario_tabelas/dicionario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC do Brunooo\Documents\Github\Sistema-de-Manutencao-de-Veiculos\dicionario_tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8F9E568-5371-4A31-B0E5-7626F9881BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A139B56-70B0-46F0-9610-B7D568220A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="4185" windowWidth="24345" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="161">
   <si>
     <t>Tabela</t>
   </si>
   <si>
-    <t>Clientes</t>
-  </si>
-  <si>
     <t>Descrição</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Idx_clientes_cpf</t>
   </si>
   <si>
-    <t>Seguros</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os dados dos seguros.</t>
   </si>
   <si>
@@ -154,42 +148,15 @@
     <t>Nome da seguradora</t>
   </si>
   <si>
-    <t>data_inicio</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>0001-01-01 – 9999-12-31</t>
-  </si>
-  <si>
-    <t>Data de início da cobertura do seguro</t>
-  </si>
-  <si>
-    <t>data_fim</t>
-  </si>
-  <si>
-    <t>Data de fim da cobertura do seguro</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>0 – 1</t>
-  </si>
-  <si>
     <t>Idx_seguros_nm_seguradora</t>
   </si>
   <si>
-    <t>Idx_seguros_data_inicio_data_fim</t>
-  </si>
-  <si>
-    <t>data_inicio, data_fim</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os dados dos funcionários cadastrados no sistema.</t>
   </si>
   <si>
@@ -274,12 +241,6 @@
     <t>Código do status do funcionario</t>
   </si>
   <si>
-    <t>Agendamento</t>
-  </si>
-  <si>
-    <t>Status_agendamento</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os dados dos agendamentos.</t>
   </si>
   <si>
@@ -352,9 +313,6 @@
     <t xml:space="preserve">Código do status do agendamento                                </t>
   </si>
   <si>
-    <t>Alas</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os dados da alas cadastradas no sistema</t>
   </si>
   <si>
@@ -397,15 +355,9 @@
     <t>Descrição do tipo de manutenção</t>
   </si>
   <si>
-    <t>descrição</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os possíveis status dos seguros.</t>
   </si>
   <si>
-    <t>cd_statusSeguros</t>
-  </si>
-  <si>
     <t>1 –  2.147.483.647</t>
   </si>
   <si>
@@ -415,9 +367,6 @@
     <t>Descrição do Status (Ativo, Inativo)</t>
   </si>
   <si>
-    <t>Idx_statusSeguros_descricao</t>
-  </si>
-  <si>
     <t>Estado atual do seguro</t>
   </si>
   <si>
@@ -427,15 +376,6 @@
     <t>Código do Status de Manutenção</t>
   </si>
   <si>
-    <t>Descrição do Status (Em progresso, Concluída)</t>
-  </si>
-  <si>
-    <t>Idx_statusManutencao_descricao</t>
-  </si>
-  <si>
-    <t>Status_seguros</t>
-  </si>
-  <si>
     <t>Veiculos</t>
   </si>
   <si>
@@ -457,21 +397,6 @@
     <t>ano</t>
   </si>
   <si>
-    <t>Veículos</t>
-  </si>
-  <si>
-    <t>Status_funcionario</t>
-  </si>
-  <si>
-    <t>Funcionarios</t>
-  </si>
-  <si>
-    <t>Manutencao</t>
-  </si>
-  <si>
-    <t>Tipos_manutecao</t>
-  </si>
-  <si>
     <t>Tabela responsável por armazenar os dados dos veículos cadastrados no sistema</t>
   </si>
   <si>
@@ -505,20 +430,86 @@
     <t>Código da ala</t>
   </si>
   <si>
-    <t>cd_statusManutencao</t>
-  </si>
-  <si>
-    <t>cd_statusFuncionario</t>
-  </si>
-  <si>
-    <t>Status_manutencao</t>
+    <t>1 – 7</t>
+  </si>
+  <si>
+    <t>clientes</t>
+  </si>
+  <si>
+    <t>seguros</t>
+  </si>
+  <si>
+    <t>funcionarios</t>
+  </si>
+  <si>
+    <t>veiculos</t>
+  </si>
+  <si>
+    <t>status_seguros</t>
+  </si>
+  <si>
+    <t>1 – 1</t>
+  </si>
+  <si>
+    <t>Descrição do Status (Em progresso, Concluída, Cancelada)</t>
+  </si>
+  <si>
+    <t>vl_manutencao</t>
+  </si>
+  <si>
+    <t>float(5,2)</t>
+  </si>
+  <si>
+    <t>0 – 3.402823466 E + 38</t>
+  </si>
+  <si>
+    <t>Valor cobrado pela manutenção</t>
+  </si>
+  <si>
+    <t>Status da manutenção</t>
+  </si>
+  <si>
+    <t>cd_status_manutencao</t>
+  </si>
+  <si>
+    <t>cd_status_seguros</t>
+  </si>
+  <si>
+    <t>agendamentos</t>
+  </si>
+  <si>
+    <t>manutencoes</t>
+  </si>
+  <si>
+    <t>tipos_manutencao</t>
+  </si>
+  <si>
+    <t>ala</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>status_funcionarios</t>
+  </si>
+  <si>
+    <t>cd_status_funcionarios</t>
+  </si>
+  <si>
+    <t>status_agendamentos</t>
+  </si>
+  <si>
+    <t>status_manutencoes</t>
+  </si>
+  <si>
+    <t>cd_status_manutencoes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,26 +562,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="0.14999847407452621"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.14999847407452621"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,20 +582,8 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -717,49 +678,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -815,80 +739,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -896,25 +747,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -933,20 +771,56 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1164,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1002"/>
+  <dimension ref="A1:P1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1185,22 +1059,23 @@
     <col min="13" max="13" width="20.42578125" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.140625" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="44"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1212,17 +1087,17 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1233,16 +1108,16 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1253,27 +1128,27 @@
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="44"/>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -1285,25 +1160,25 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1315,23 +1190,23 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="44"/>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1343,23 +1218,23 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1371,23 +1246,23 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1399,16 +1274,16 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
+      <c r="A9" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1419,24 +1294,24 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="44"/>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1447,20 +1322,20 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="24"/>
+      <c r="A11" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="44"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+      <c r="F11" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1471,22 +1346,22 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="24"/>
+      <c r="A12" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="44"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+        <v>14</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="43"/>
+      <c r="H12" s="44"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1497,8 +1372,8 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
@@ -1518,317 +1393,274 @@
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
+      <c r="B14" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="44"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="68" t="s">
-        <v>137</v>
-      </c>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="68"/>
+      <c r="K14" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="68"/>
+      <c r="J15" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="69" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="K17" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="1" t="s">
+      <c r="L17" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="M17" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="N17" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="O17" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="K17" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="M17" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="N17" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="O17" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="P17" s="67" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="24"/>
+      <c r="P17" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="44"/>
       <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="K18" s="68" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="M18" s="68" t="s">
+      <c r="J18" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="N18" s="68" t="s">
-        <v>15</v>
-      </c>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="24"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="44"/>
       <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="K19" s="68" t="s">
+      <c r="K19" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="L19" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="M19" s="68" t="s">
+      <c r="M19" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="55" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="68" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="H20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="44"/>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="43"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="72"/>
-      <c r="O20" s="72"/>
-      <c r="P20" s="73"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="K21" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" s="47"/>
-      <c r="P21" s="47"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="49"/>
-      <c r="L22" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="M22" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="N22" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="24"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="43"/>
+      <c r="H23" s="44"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1839,24 +1671,6 @@
       <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1867,20 +1681,18 @@
       <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="44"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -1891,20 +1703,18 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="44"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1915,289 +1725,321 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="44"/>
       <c r="I27" s="13"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
+      <c r="A28" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="44"/>
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K28" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="24"/>
+      <c r="K28" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="44"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="24"/>
+      <c r="A29" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="44"/>
+      <c r="C29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="I29" s="2"/>
       <c r="J29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K29" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="44"/>
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="24"/>
+      <c r="A30" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="44"/>
+      <c r="C30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="24"/>
+      <c r="J30" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="44"/>
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>2</v>
+      <c r="A31" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="44"/>
+      <c r="C31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="1" t="s">
+      <c r="L31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O31" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="P31" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="24"/>
+      <c r="A32" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="44"/>
       <c r="C32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="5" t="s">
-        <v>59</v>
+      <c r="H32" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L32" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M32" s="5" t="s">
+      <c r="N32" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="N32" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="O32" s="5"/>
       <c r="P32" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="E33" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="24"/>
+      <c r="A34" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="44"/>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" s="24"/>
+      <c r="A35" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="44"/>
       <c r="C35" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="14" t="s">
-        <v>71</v>
+      <c r="H35" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="24"/>
+      <c r="A36" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="44"/>
       <c r="C36" s="5" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="24"/>
+      <c r="A37" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="44"/>
       <c r="C37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
       <c r="H37" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="9"/>
@@ -2209,24 +2051,14 @@
       <c r="P37" s="9"/>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
       <c r="I38" s="2"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
@@ -2237,24 +2069,18 @@
       <c r="P38" s="9"/>
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5" t="s">
-        <v>82</v>
-      </c>
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="44"/>
       <c r="I39" s="2"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
@@ -2265,26 +2091,18 @@
       <c r="P39" s="9"/>
     </row>
     <row r="40" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="44"/>
       <c r="I40" s="2"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
@@ -2295,14 +2113,16 @@
       <c r="P40" s="9"/>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="A41" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="44"/>
       <c r="I41" s="2"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
@@ -2313,71 +2133,97 @@
       <c r="P41" s="9"/>
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="24"/>
+      <c r="A42" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="44"/>
+      <c r="C42" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="I42" s="2"/>
       <c r="J42" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K42" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="24"/>
+      <c r="K42" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="44"/>
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="23"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="24"/>
+      <c r="A43" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="44"/>
+      <c r="C43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="I43" s="2"/>
       <c r="J43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K43" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="L43" s="23"/>
-      <c r="M43" s="23"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="K43" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+      <c r="P43" s="44"/>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="24"/>
+      <c r="A44" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="44"/>
+      <c r="C44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="I44" s="3"/>
       <c r="J44" s="17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K44" s="17"/>
       <c r="L44" s="17"/>
@@ -2387,149 +2233,147 @@
       <c r="P44" s="17"/>
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>2</v>
+      <c r="A45" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="44"/>
+      <c r="C45" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="P45" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="B46" s="24"/>
+      <c r="A46" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="53"/>
       <c r="C46" s="5" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="5" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="K46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L46" s="5" t="s">
+      <c r="M46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M46" s="5" t="s">
+      <c r="N46" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="O46" s="5"/>
       <c r="P46" s="5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" s="24"/>
+      <c r="A47" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="44"/>
       <c r="C47" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5" t="s">
-        <v>93</v>
+      <c r="H47" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="5"/>
       <c r="P47" s="5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>73</v>
+      <c r="A48" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="44"/>
+      <c r="C48" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="E48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5" t="s">
-        <v>97</v>
+      <c r="H48" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="9"/>
@@ -2541,23 +2385,25 @@
       <c r="P48" s="9"/>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="30"/>
+      <c r="A49" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="44"/>
       <c r="C49" s="5" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="E49" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5" t="s">
-        <v>101</v>
+      <c r="H49" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="9"/>
@@ -2569,25 +2415,25 @@
       <c r="P49" s="9"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="24"/>
+      <c r="A50" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="44"/>
       <c r="C50" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="14"/>
+      <c r="G50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>102</v>
+      <c r="H50" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="I50" s="12"/>
       <c r="J50" s="18"/>
@@ -2599,26 +2445,6 @@
       <c r="P50" s="18"/>
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H51" s="14" t="s">
-        <v>106</v>
-      </c>
       <c r="I51" s="15"/>
       <c r="J51" s="16"/>
       <c r="K51" s="16"/>
@@ -2629,26 +2455,18 @@
       <c r="P51" s="16"/>
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>108</v>
-      </c>
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="44"/>
       <c r="I52" s="15"/>
       <c r="J52" s="16"/>
       <c r="K52" s="16"/>
@@ -2659,26 +2477,18 @@
       <c r="P52" s="16"/>
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" s="14"/>
-      <c r="G53" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>109</v>
-      </c>
+      <c r="A53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="44"/>
       <c r="I53" s="15"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
@@ -2689,6 +2499,16 @@
       <c r="P53" s="16"/>
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="44"/>
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
       <c r="K54" s="13"/>
@@ -2699,18 +2519,28 @@
       <c r="P54" s="13"/>
     </row>
     <row r="55" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="24"/>
+      <c r="A55" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="44"/>
+      <c r="C55" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -2721,18 +2551,26 @@
       <c r="P55" s="2"/>
     </row>
     <row r="56" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23"/>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="24"/>
+      <c r="A56" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="44"/>
+      <c r="C56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -2743,16 +2581,24 @@
       <c r="P56" s="2"/>
     </row>
     <row r="57" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="23"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="23"/>
-      <c r="F57" s="23"/>
-      <c r="G57" s="23"/>
-      <c r="H57" s="24"/>
+      <c r="A57" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="44"/>
+      <c r="C57" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2763,27 +2609,23 @@
       <c r="P57" s="3"/>
     </row>
     <row r="58" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="24"/>
-      <c r="C58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>2</v>
+      <c r="A58" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="44"/>
+      <c r="C58" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -2795,26 +2637,16 @@
       <c r="P58" s="4"/>
     </row>
     <row r="59" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5" t="s">
-        <v>113</v>
-      </c>
+      <c r="A59" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="43"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="44"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -2825,24 +2657,24 @@
       <c r="P59" s="2"/>
     </row>
     <row r="60" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="A60" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="44"/>
+      <c r="C60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="43"/>
+      <c r="H60" s="44"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -2853,24 +2685,14 @@
       <c r="P60" s="2"/>
     </row>
     <row r="61" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="A61" s="47"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="44"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -2881,16 +2703,14 @@
       <c r="P61" s="2"/>
     </row>
     <row r="62" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B62" s="23"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="23"/>
-      <c r="H62" s="24"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="44"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -2901,24 +2721,6 @@
       <c r="P62" s="4"/>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F63" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" s="23"/>
-      <c r="H63" s="24"/>
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -2929,14 +2731,18 @@
       <c r="P63" s="4"/>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="23"/>
-      <c r="H64" s="24"/>
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="44"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -2946,15 +2752,19 @@
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
     </row>
-    <row r="65" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="23"/>
-      <c r="H65" s="24"/>
+    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="44"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -2964,7 +2774,17 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="43"/>
+      <c r="C66" s="43"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="43"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="44"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
       <c r="K66" s="13"/>
@@ -2974,809 +2794,763 @@
       <c r="O66" s="13"/>
       <c r="P66" s="13"/>
     </row>
-    <row r="67" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="44"/>
+      <c r="C67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I67" s="2"/>
+      <c r="J67" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B67" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="23"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="K67" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="L67" s="36"/>
-      <c r="M67" s="36"/>
-      <c r="N67" s="36"/>
-      <c r="O67" s="36"/>
-      <c r="P67" s="36"/>
-      <c r="Q67" s="37"/>
-    </row>
-    <row r="68" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C68" s="23"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
-      <c r="F68" s="23"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="24"/>
+      <c r="K67" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="L67" s="54"/>
+      <c r="M67" s="54"/>
+      <c r="N67" s="54"/>
+      <c r="O67" s="54"/>
+      <c r="P67" s="54"/>
+    </row>
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="B68" s="44"/>
+      <c r="C68" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="I68" s="2"/>
-      <c r="J68" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="K68" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="L68" s="36"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="36"/>
-      <c r="O68" s="36"/>
-      <c r="P68" s="36"/>
-      <c r="Q68" s="37"/>
-    </row>
-    <row r="69" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
+      <c r="J68" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K68" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="L68" s="54"/>
+      <c r="M68" s="54"/>
+      <c r="N68" s="54"/>
+      <c r="O68" s="54"/>
+      <c r="P68" s="54"/>
+    </row>
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69" s="44"/>
+      <c r="C69" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" s="3"/>
+      <c r="J69" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+      <c r="N69" s="36"/>
+      <c r="O69" s="36"/>
+      <c r="P69" s="36"/>
+    </row>
+    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B70" s="44"/>
+      <c r="C70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="J70" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="K69" s="39"/>
-      <c r="L69" s="39"/>
-      <c r="M69" s="39"/>
-      <c r="N69" s="39"/>
-      <c r="O69" s="39"/>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="40"/>
-    </row>
-    <row r="70" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="26" t="s">
+      <c r="K70" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="1" t="s">
+      <c r="L70" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="M70" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="N70" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="O70" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G70" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I70" s="4"/>
-      <c r="J70" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="K70" s="42"/>
-      <c r="L70" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="M70" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="N70" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="O70" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="P70" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q70" s="34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B71" s="24"/>
+      <c r="P70" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B71" s="44"/>
       <c r="C71" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E71" s="5" t="s">
+      <c r="F71" s="5"/>
+      <c r="G71" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F71" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G71" s="5"/>
       <c r="H71" s="5" t="s">
-        <v>16</v>
+        <v>134</v>
       </c>
       <c r="I71" s="2"/>
-      <c r="J71" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="K71" s="37"/>
-      <c r="L71" s="43" t="s">
+      <c r="J71" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="K71" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="L71" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="M71" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N71" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="O71" s="34"/>
+      <c r="P71" s="55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="44"/>
+      <c r="C72" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M71" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="N71" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="O71" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="P71" s="43"/>
-      <c r="Q71" s="43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B72" s="24"/>
-      <c r="C72" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="E72" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="I72" s="2"/>
-      <c r="J72" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="K72" s="44"/>
-      <c r="L72" s="43" t="s">
+      <c r="J72" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="K72" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L72" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="M72" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="N72" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="O72" s="43"/>
-      <c r="P72" s="43"/>
-      <c r="Q72" s="43" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M72" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N72" s="34"/>
+      <c r="O72" s="34"/>
+      <c r="P72" s="55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B73" s="24"/>
+        <v>144</v>
+      </c>
+      <c r="B73" s="20"/>
       <c r="C73" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+    </row>
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="44"/>
+      <c r="C74" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I73" s="2"/>
-      <c r="J73" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="K73" s="46"/>
-      <c r="L73" s="46"/>
-      <c r="M73" s="46"/>
-      <c r="N73" s="46"/>
-      <c r="O73" s="46"/>
-      <c r="P73" s="46"/>
-      <c r="Q73" s="46"/>
-    </row>
-    <row r="74" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I74" s="2"/>
-      <c r="J74" s="46" t="s">
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+    </row>
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+    </row>
+    <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" s="44"/>
+      <c r="C76" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K74" s="46"/>
-      <c r="L74" s="47" t="s">
+      <c r="D76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M74" s="47" t="s">
+      <c r="E76" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N74" s="47" t="s">
+      <c r="F76" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="O74" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="P74" s="46"/>
-      <c r="Q74" s="46"/>
-    </row>
-    <row r="75" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="I75" s="2"/>
-      <c r="J75" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="K75" s="48"/>
-      <c r="L75" s="49"/>
-      <c r="M75" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="N75" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="O75" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="P75" s="48"/>
-      <c r="Q75" s="48"/>
-    </row>
-    <row r="76" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B76" s="23"/>
-      <c r="C76" s="23"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
-      <c r="F76" s="23"/>
-      <c r="G76" s="23"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-    </row>
-    <row r="77" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F77" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G77" s="23"/>
-      <c r="H77" s="24"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-    </row>
-    <row r="78" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="25"/>
-      <c r="B78" s="24"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+    </row>
+    <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="47"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+    </row>
+    <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="47"/>
+      <c r="B78" s="44"/>
       <c r="C78" s="7"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="23"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="2"/>
-      <c r="J78" s="2"/>
-      <c r="K78" s="2"/>
-      <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2"/>
-      <c r="O78" s="2"/>
-      <c r="P78" s="2"/>
-    </row>
-    <row r="79" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="23"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="2"/>
-      <c r="K79" s="2"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="2"/>
-      <c r="O79" s="2"/>
-      <c r="P79" s="2"/>
-    </row>
-    <row r="80" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="21"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="63"/>
-      <c r="D80" s="64"/>
-      <c r="E80" s="64"/>
-      <c r="F80" s="64"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="20"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="43"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="30"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
+      <c r="G80" s="43"/>
+      <c r="H80" s="44"/>
       <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-      <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
-      <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="2"/>
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="B81" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
+      <c r="G81" s="43"/>
+      <c r="H81" s="44"/>
       <c r="I81" s="2"/>
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B82" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
-      <c r="F82" s="23"/>
-      <c r="G82" s="23"/>
-      <c r="H82" s="24"/>
+      <c r="A82" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82" s="43"/>
+      <c r="C82" s="43"/>
+      <c r="D82" s="43"/>
+      <c r="E82" s="43"/>
+      <c r="F82" s="43"/>
+      <c r="G82" s="43"/>
+      <c r="H82" s="44"/>
       <c r="I82" s="2"/>
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="27" t="s">
+      <c r="A83" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B83" s="23"/>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23"/>
-      <c r="F83" s="23"/>
-      <c r="G83" s="23"/>
-      <c r="H83" s="24"/>
-      <c r="I83" s="3"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I84" s="4"/>
+      <c r="A84" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="44"/>
+      <c r="C84" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I84" s="2"/>
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="B85" s="24"/>
+      <c r="A85" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" s="44"/>
       <c r="C85" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D85" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E85" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I85" s="2"/>
+        <v>110</v>
+      </c>
+      <c r="I85" s="3"/>
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B86" s="24"/>
-      <c r="C86" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="5"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I86" s="2"/>
+      <c r="A86" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86" s="43"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="26" t="s">
+      <c r="A87" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B87" s="23"/>
-      <c r="C87" s="23"/>
-      <c r="D87" s="23"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="23"/>
-      <c r="H87" s="24"/>
-      <c r="I87" s="4"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F87" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87" s="43"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B88" s="24"/>
-      <c r="C88" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F88" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G88" s="23"/>
-      <c r="H88" s="24"/>
-      <c r="I88" s="4"/>
+      <c r="A88" s="47"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="43"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="24"/>
+      <c r="A89" s="47"/>
+      <c r="B89" s="44"/>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
-      <c r="F89" s="25"/>
-      <c r="G89" s="23"/>
-      <c r="H89" s="24"/>
-      <c r="I89" s="2"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="43"/>
+      <c r="H89" s="44"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="25"/>
-      <c r="G90" s="23"/>
-      <c r="H90" s="24"/>
-      <c r="I90" s="2"/>
+      <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I91" s="13"/>
+      <c r="A91" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D91" s="38"/>
+      <c r="E91" s="38"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="2"/>
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B92" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="C92" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="D92" s="55"/>
-      <c r="E92" s="55"/>
-      <c r="F92" s="55"/>
-      <c r="G92" s="55"/>
-      <c r="H92" s="55"/>
-      <c r="I92" s="51"/>
-      <c r="J92" s="51"/>
-      <c r="K92" s="51"/>
+      <c r="A92" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="2"/>
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="54" t="s">
-        <v>150</v>
-      </c>
-      <c r="C93" s="55"/>
-      <c r="D93" s="55"/>
-      <c r="E93" s="55"/>
-      <c r="F93" s="55"/>
-      <c r="G93" s="55"/>
-      <c r="H93" s="55"/>
-      <c r="I93" s="51"/>
+      <c r="A93" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="38"/>
+      <c r="C93" s="38"/>
+      <c r="D93" s="38"/>
+      <c r="E93" s="38"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="13"/>
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="56" t="s">
-        <v>4</v>
-      </c>
-      <c r="B94" s="55"/>
-      <c r="C94" s="55"/>
-      <c r="D94" s="55"/>
-      <c r="E94" s="55"/>
-      <c r="F94" s="55"/>
-      <c r="G94" s="55"/>
-      <c r="H94" s="55"/>
-      <c r="I94" s="51"/>
+      <c r="A94" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" s="38"/>
+      <c r="C94" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G94" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H94" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I94" s="23"/>
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="B95" s="55"/>
-      <c r="C95" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="D95" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="E95" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="F95" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="53" t="s">
+      <c r="A95" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" s="38"/>
+      <c r="C95" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E95" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="25"/>
+      <c r="H95" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="I95" s="23"/>
+    </row>
+    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="H95" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="I95" s="52"/>
-    </row>
-    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="B96" s="55"/>
-      <c r="C96" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="D96" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="E96" s="58" t="s">
+      <c r="B96" s="38"/>
+      <c r="C96" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="25"/>
+      <c r="G96" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="I96" s="52"/>
+      <c r="H96" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="I96" s="23"/>
     </row>
     <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="54" t="s">
+      <c r="A97" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B97" s="38"/>
+      <c r="C97" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E97" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="25"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I97" s="23"/>
+    </row>
+    <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B98" s="38"/>
+      <c r="C98" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F98" s="25"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="I98" s="23"/>
+    </row>
+    <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B99" s="38"/>
+      <c r="C99" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F99" s="25"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="I99" s="23"/>
+    </row>
+    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B100" s="38"/>
+      <c r="C100" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B97" s="55"/>
-      <c r="C97" s="65" t="s">
+      <c r="D100" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D97" s="59" t="s">
+      <c r="E100" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E97" s="58" t="s">
+      <c r="F100" s="28"/>
+      <c r="G100" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F97" s="58"/>
-      <c r="G97" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="H97" s="58" t="s">
-        <v>153</v>
-      </c>
-      <c r="I97" s="52"/>
-    </row>
-    <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B98" s="55"/>
-      <c r="C98" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D98" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="E98" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="I98" s="52"/>
-    </row>
-    <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="B99" s="55"/>
-      <c r="C99" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D99" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="E99" s="58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99" s="58"/>
-      <c r="G99" s="58"/>
-      <c r="H99" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="I99" s="52"/>
-    </row>
-    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="60" t="s">
-        <v>144</v>
-      </c>
-      <c r="B100" s="55"/>
-      <c r="C100" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="D100" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="E100" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="58"/>
-      <c r="G100" s="58"/>
-      <c r="H100" s="58" t="s">
-        <v>157</v>
-      </c>
-      <c r="I100" s="52"/>
+      <c r="H100" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="I100" s="23"/>
     </row>
     <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="B101" s="55"/>
-      <c r="C101" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="D101" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="E101" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" s="61"/>
-      <c r="G101" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="H101" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="I101" s="52"/>
+      <c r="I101" s="23"/>
     </row>
     <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I102" s="13"/>
+      <c r="I102" s="23"/>
     </row>
     <row r="103" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I103" s="13"/>
+      <c r="I103" s="23"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I104" s="13"/>
@@ -6475,31 +6249,81 @@
     <row r="1002" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1002" s="13"/>
     </row>
+    <row r="1003" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1003" s="13"/>
+    </row>
+    <row r="1004" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1004" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="129">
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="J20:P20"/>
-    <mergeCell ref="B93:H93"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="B92:H92"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="O75:Q75"/>
-    <mergeCell ref="K67:Q67"/>
-    <mergeCell ref="K68:Q68"/>
-    <mergeCell ref="J69:Q69"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J72:K72"/>
-    <mergeCell ref="J73:Q73"/>
-    <mergeCell ref="J74:K74"/>
-    <mergeCell ref="O74:Q74"/>
+  <mergeCells count="117">
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="K67:P67"/>
+    <mergeCell ref="K68:P68"/>
+    <mergeCell ref="J69:P69"/>
+    <mergeCell ref="B81:H81"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F89:H89"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A86:H86"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A82:H82"/>
+    <mergeCell ref="B65:H65"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A54:H54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="K29:P29"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="K42:P42"/>
+    <mergeCell ref="K43:P43"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="B39:H39"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -6516,96 +6340,40 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:H75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="B92:H92"/>
+    <mergeCell ref="A93:H93"/>
+    <mergeCell ref="B91:H91"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F23:H23"/>
     <mergeCell ref="K28:P28"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="K29:P29"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="K42:P42"/>
-    <mergeCell ref="K43:P43"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="A44:H44"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:H76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="A69:H69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B82:H82"/>
-    <mergeCell ref="B81:H81"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="F89:H89"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A87:H87"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A83:H83"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Fazendo os inserts nas tabelas
Tive que arrumar alguns inserts, mas coisa de uma palavra no plural e umas vírgulas meio soltas.
</commit_message>
<xml_diff>
--- a/dicionario_tabelas/dicionario.xlsx
+++ b/dicionario_tabelas/dicionario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kazam\Desktop\Sistema-de-Manutencao-de-Veiculos\dicionario_tabelas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142100AE-892B-4223-8ACA-12D61BDD5006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF8EE30-0869-455F-A419-6F8763A47AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="2655" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="166">
   <si>
     <t>Tabela</t>
   </si>
@@ -331,9 +331,6 @@
     <t>descricao</t>
   </si>
   <si>
-    <t>0 – 100</t>
-  </si>
-  <si>
     <t>Descrição das alas</t>
   </si>
   <si>
@@ -515,6 +512,12 @@
   </si>
   <si>
     <t>Idx_cd_status_agendamento</t>
+  </si>
+  <si>
+    <t>1 – 100</t>
+  </si>
+  <si>
+    <t>0 – 200</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -885,88 +888,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -976,23 +897,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1010,12 +920,103 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,19 +1235,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1029"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K120" sqref="K120"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="72" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="4.85546875" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="58.140625" style="72" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
     <col min="11" max="11" width="23.140625" customWidth="1"/>
@@ -1262,15 +1262,15 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1284,15 +1284,15 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1303,16 +1303,16 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1323,11 +1323,11 @@
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="70" t="s">
+      <c r="B4" s="56"/>
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1342,7 +1342,7 @@
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="70" t="s">
+      <c r="H4" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
@@ -1355,10 +1355,10 @@
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1385,10 +1385,10 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
@@ -1413,10 +1413,10 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
@@ -1441,10 +1441,10 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
@@ -1469,16 +1469,16 @@
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1489,11 +1489,11 @@
       <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="70" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1502,11 +1502,11 @@
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="56"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1517,20 +1517,20 @@
       <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="82"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="56"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1541,22 +1541,22 @@
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="82"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="56"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1567,14 +1567,14 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -1585,14 +1585,14 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
+      <c r="A14" s="76"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1603,14 +1603,14 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
+      <c r="A15" s="76"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1621,14 +1621,14 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1642,21 +1642,21 @@
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="56"/>
       <c r="I17" s="2"/>
       <c r="J17" s="26" t="s">
         <v>0</v>
       </c>
       <c r="K17" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
@@ -1668,21 +1668,21 @@
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="2"/>
       <c r="J18" s="26" t="s">
         <v>1</v>
       </c>
       <c r="K18" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L18" s="27"/>
       <c r="M18" s="27"/>
@@ -1691,33 +1691,33 @@
       <c r="P18" s="27"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="60" t="s">
+      <c r="J19" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="70" t="s">
+      <c r="B20" s="56"/>
+      <c r="C20" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1732,7 +1732,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="70" t="s">
+      <c r="H20" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I20" s="4"/>
@@ -1759,10 +1759,10 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="11" t="s">
         <v>11</v>
       </c>
@@ -1781,13 +1781,13 @@
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K21" s="27" t="s">
         <v>11</v>
       </c>
       <c r="L21" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M21" s="27" t="s">
         <v>13</v>
@@ -1797,14 +1797,14 @@
       </c>
       <c r="O21" s="27"/>
       <c r="P21" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="38"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="11" t="s">
         <v>17</v>
       </c>
@@ -1835,19 +1835,19 @@
       <c r="N22" s="27"/>
       <c r="O22" s="27"/>
       <c r="P22" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="B23" s="38"/>
+      <c r="A23" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="56"/>
       <c r="C23" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>13</v>
@@ -1857,29 +1857,29 @@
         <v>14</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="38"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="56"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="70" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1888,30 +1888,30 @@
       <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="41" t="s">
+      <c r="F25" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="38"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="56"/>
       <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="82"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="38"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="56"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -1924,12 +1924,12 @@
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="31"/>
-      <c r="C27" s="83"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="31"/>
-      <c r="H27" s="71"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -1942,12 +1942,12 @@
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="31"/>
-      <c r="C28" s="83"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="31"/>
-      <c r="H28" s="71"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1960,12 +1960,12 @@
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="31"/>
-      <c r="C29" s="83"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="31"/>
-      <c r="H29" s="71"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -1989,15 +1989,15 @@
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="38"/>
+      <c r="B31" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="56"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2011,15 +2011,15 @@
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="38"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="56"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -2030,24 +2030,24 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="38"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="56"/>
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="70" t="s">
+      <c r="B34" s="56"/>
+      <c r="C34" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2062,28 +2062,28 @@
       <c r="G34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="70" t="s">
+      <c r="H34" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
+      <c r="K34" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="11" t="s">
         <v>11</v>
       </c>
@@ -2104,21 +2104,21 @@
       <c r="J35" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="43" t="s">
+      <c r="K35" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="11" t="s">
         <v>52</v>
       </c>
@@ -2134,22 +2134,22 @@
         <v>54</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="65" t="s">
+      <c r="J36" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="74"/>
+      <c r="M36" s="74"/>
+      <c r="N36" s="74"/>
+      <c r="O36" s="74"/>
+      <c r="P36" s="74"/>
+      <c r="Q36" s="74"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="11" t="s">
         <v>21</v>
       </c>
@@ -2183,16 +2183,16 @@
       <c r="O37" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="P37" s="47" t="s">
+      <c r="P37" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="Q37" s="47"/>
+      <c r="Q37" s="51"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="39" t="s">
+      <c r="A38" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="38"/>
+      <c r="B38" s="56"/>
       <c r="C38" s="11" t="s">
         <v>26</v>
       </c>
@@ -2204,12 +2204,12 @@
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="73" t="s">
+      <c r="H38" s="14" t="s">
         <v>60</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>11</v>
@@ -2224,16 +2224,16 @@
         <v>14</v>
       </c>
       <c r="O38" s="19"/>
-      <c r="P38" s="43" t="s">
+      <c r="P38" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="Q38" s="43"/>
+      <c r="Q38" s="49"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="56"/>
       <c r="C39" s="11" t="s">
         <v>42</v>
       </c>
@@ -2263,16 +2263,16 @@
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="19"/>
-      <c r="P39" s="43" t="s">
+      <c r="P39" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="Q39" s="43"/>
+      <c r="Q39" s="49"/>
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="56"/>
       <c r="C40" s="11" t="s">
         <v>42</v>
       </c>
@@ -2288,22 +2288,22 @@
         <v>65</v>
       </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="41" t="s">
+      <c r="J40" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="37"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="37"/>
-      <c r="P40" s="67"/>
-      <c r="Q40" s="63"/>
+      <c r="K40" s="53"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="53"/>
+      <c r="P40" s="54"/>
+      <c r="Q40" s="55"/>
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="39" t="s">
+      <c r="A41" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="38"/>
+      <c r="B41" s="56"/>
       <c r="C41" s="11" t="s">
         <v>42</v>
       </c>
@@ -2319,10 +2319,10 @@
         <v>67</v>
       </c>
       <c r="I41" s="15"/>
-      <c r="J41" s="41" t="s">
+      <c r="J41" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K41" s="38"/>
+      <c r="K41" s="56"/>
       <c r="L41" s="1" t="s">
         <v>31</v>
       </c>
@@ -2332,17 +2332,17 @@
       <c r="N41" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="41" t="s">
+      <c r="O41" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="P41" s="37"/>
-      <c r="Q41" s="38"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="56"/>
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="38"/>
+      <c r="B42" s="56"/>
       <c r="C42" s="11" t="s">
         <v>69</v>
       </c>
@@ -2358,10 +2358,10 @@
         <v>71</v>
       </c>
       <c r="I42" s="2"/>
-      <c r="J42" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="K42" s="38"/>
+      <c r="J42" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="K42" s="56"/>
       <c r="L42" s="7" t="s">
         <v>14</v>
       </c>
@@ -2369,17 +2369,17 @@
       <c r="N42" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="O42" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="P42" s="37"/>
-      <c r="Q42" s="38"/>
+      <c r="O42" s="58" t="s">
+        <v>156</v>
+      </c>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="56"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="38"/>
+      <c r="B43" s="56"/>
       <c r="C43" s="11" t="s">
         <v>11</v>
       </c>
@@ -2406,16 +2406,16 @@
       <c r="P43" s="9"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="37"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="53"/>
+      <c r="H44" s="56"/>
       <c r="I44" s="2"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
@@ -2426,11 +2426,11 @@
       <c r="P44" s="9"/>
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="70" t="s">
+      <c r="B45" s="56"/>
+      <c r="C45" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="1" t="s">
@@ -2439,37 +2439,37 @@
       <c r="E45" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="41" t="s">
+      <c r="F45" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G45" s="37"/>
-      <c r="H45" s="38"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="56"/>
       <c r="I45" s="2"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
       <c r="L45" s="10"/>
       <c r="M45" s="9"/>
-      <c r="N45" s="68"/>
+      <c r="N45" s="36"/>
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" s="38"/>
-      <c r="C46" s="84" t="s">
+      <c r="A46" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" s="56"/>
+      <c r="C46" s="45" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="G46" s="37"/>
-      <c r="H46" s="38"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="56"/>
       <c r="I46" s="2"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
@@ -2482,12 +2482,12 @@
     <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="31"/>
-      <c r="C47" s="83"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="2"/>
       <c r="E47" s="34"/>
       <c r="F47" s="2"/>
       <c r="G47" s="31"/>
-      <c r="H47" s="71"/>
+      <c r="H47" s="31"/>
       <c r="I47" s="2"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
@@ -2500,12 +2500,12 @@
     <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="31"/>
-      <c r="C48" s="83"/>
+      <c r="C48" s="44"/>
       <c r="D48" s="2"/>
       <c r="E48" s="34"/>
       <c r="F48" s="2"/>
       <c r="G48" s="31"/>
-      <c r="H48" s="74"/>
+      <c r="H48" s="39"/>
       <c r="I48" s="2"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
@@ -2518,12 +2518,12 @@
     <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="31"/>
-      <c r="C49" s="83"/>
+      <c r="C49" s="44"/>
       <c r="D49" s="2"/>
       <c r="E49" s="34"/>
       <c r="F49" s="2"/>
       <c r="G49" s="31"/>
-      <c r="H49" s="71"/>
+      <c r="H49" s="31"/>
       <c r="I49" s="2"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
@@ -2534,8 +2534,8 @@
       <c r="P49" s="9"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="58"/>
-      <c r="B50" s="59"/>
+      <c r="A50" s="71"/>
+      <c r="B50" s="72"/>
       <c r="C50" s="17"/>
       <c r="D50" s="10"/>
       <c r="E50" s="9"/>
@@ -2555,15 +2555,15 @@
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="38"/>
+      <c r="B51" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="56"/>
       <c r="I51" s="2"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
@@ -2577,15 +2577,15 @@
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="38"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="56"/>
       <c r="I52" s="2"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
@@ -2596,16 +2596,16 @@
       <c r="P52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="40" t="s">
+      <c r="A53" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="38"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="56"/>
       <c r="I53" s="2"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -2616,11 +2616,11 @@
       <c r="P53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="38"/>
-      <c r="C54" s="70" t="s">
+      <c r="B54" s="56"/>
+      <c r="C54" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="1" t="s">
@@ -2635,28 +2635,28 @@
       <c r="G54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H54" s="70" t="s">
+      <c r="H54" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="K54" s="43" t="s">
-        <v>158</v>
-      </c>
-      <c r="L54" s="43"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
-      <c r="P54" s="43"/>
-      <c r="Q54" s="43"/>
+      <c r="K54" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
     </row>
     <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="B55" s="38"/>
+      <c r="B55" s="56"/>
       <c r="C55" s="11" t="s">
         <v>11</v>
       </c>
@@ -2677,21 +2677,21 @@
       <c r="J55" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="K55" s="43" t="s">
+      <c r="K55" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+      <c r="O55" s="49"/>
+      <c r="P55" s="49"/>
+      <c r="Q55" s="49"/>
     </row>
     <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="38"/>
+      <c r="B56" s="56"/>
       <c r="C56" s="11" t="s">
         <v>42</v>
       </c>
@@ -2707,22 +2707,22 @@
         <v>80</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="46" t="s">
+      <c r="J56" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="46"/>
-      <c r="O56" s="46"/>
-      <c r="P56" s="46"/>
-      <c r="Q56" s="46"/>
+      <c r="K56" s="50"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
     </row>
     <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="38"/>
+      <c r="B57" s="56"/>
       <c r="C57" s="11" t="s">
         <v>42</v>
       </c>
@@ -2756,16 +2756,16 @@
       <c r="O57" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="P57" s="47" t="s">
+      <c r="P57" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="Q57" s="47"/>
+      <c r="Q57" s="51"/>
     </row>
     <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="62" t="s">
+      <c r="A58" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="63"/>
+      <c r="B58" s="55"/>
       <c r="C58" s="11" t="s">
         <v>86</v>
       </c>
@@ -2797,16 +2797,16 @@
         <v>14</v>
       </c>
       <c r="O58" s="22"/>
-      <c r="P58" s="43" t="s">
+      <c r="P58" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="Q58" s="43"/>
+      <c r="Q58" s="49"/>
     </row>
     <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
+      <c r="A59" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="38"/>
+      <c r="B59" s="56"/>
       <c r="C59" s="11" t="s">
         <v>11</v>
       </c>
@@ -2838,17 +2838,17 @@
       </c>
       <c r="N59" s="22"/>
       <c r="O59" s="22"/>
-      <c r="P59" s="43" t="s">
+      <c r="P59" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="Q59" s="43"/>
+      <c r="Q59" s="49"/>
     </row>
     <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="61" t="s">
+      <c r="A60" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="73" t="s">
+      <c r="B60" s="56"/>
+      <c r="C60" s="14" t="s">
         <v>91</v>
       </c>
       <c r="D60" s="14" t="s">
@@ -2861,26 +2861,26 @@
       <c r="G60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="73" t="s">
+      <c r="H60" s="14" t="s">
         <v>93</v>
       </c>
       <c r="I60" s="2"/>
-      <c r="J60" s="41" t="s">
+      <c r="J60" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K60" s="37"/>
-      <c r="L60" s="37"/>
-      <c r="M60" s="37"/>
-      <c r="N60" s="37"/>
-      <c r="O60" s="37"/>
-      <c r="P60" s="67"/>
-      <c r="Q60" s="63"/>
+      <c r="K60" s="53"/>
+      <c r="L60" s="53"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="53"/>
+      <c r="O60" s="53"/>
+      <c r="P60" s="54"/>
+      <c r="Q60" s="55"/>
     </row>
     <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="61" t="s">
+      <c r="A61" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="38"/>
+      <c r="B61" s="56"/>
       <c r="C61" s="11" t="s">
         <v>11</v>
       </c>
@@ -2894,14 +2894,14 @@
       <c r="G61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H61" s="73" t="s">
+      <c r="H61" s="14" t="s">
         <v>95</v>
       </c>
       <c r="I61" s="2"/>
-      <c r="J61" s="41" t="s">
+      <c r="J61" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K61" s="38"/>
+      <c r="K61" s="56"/>
       <c r="L61" s="1" t="s">
         <v>31</v>
       </c>
@@ -2911,17 +2911,17 @@
       <c r="N61" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O61" s="41" t="s">
+      <c r="O61" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="P61" s="37"/>
-      <c r="Q61" s="38"/>
+      <c r="P61" s="53"/>
+      <c r="Q61" s="56"/>
     </row>
     <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
+      <c r="A62" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="38"/>
+      <c r="B62" s="56"/>
       <c r="C62" s="11" t="s">
         <v>11</v>
       </c>
@@ -2935,14 +2935,14 @@
       <c r="G62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="73" t="s">
+      <c r="H62" s="14" t="s">
         <v>96</v>
       </c>
       <c r="I62" s="12"/>
-      <c r="J62" s="42" t="s">
-        <v>164</v>
-      </c>
-      <c r="K62" s="38"/>
+      <c r="J62" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="K62" s="56"/>
       <c r="L62" s="7" t="s">
         <v>14</v>
       </c>
@@ -2950,23 +2950,23 @@
       <c r="N62" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="O62" s="36" t="s">
+      <c r="O62" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="P62" s="37"/>
-      <c r="Q62" s="38"/>
+      <c r="P62" s="53"/>
+      <c r="Q62" s="56"/>
     </row>
     <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="38"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="56"/>
       <c r="I63" s="12"/>
       <c r="J63" s="17"/>
       <c r="K63" s="17"/>
@@ -2977,11 +2977,11 @@
       <c r="P63" s="17"/>
     </row>
     <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="38"/>
-      <c r="C64" s="70" t="s">
+      <c r="B64" s="56"/>
+      <c r="C64" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D64" s="1" t="s">
@@ -2990,11 +2990,11 @@
       <c r="E64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="41" t="s">
+      <c r="F64" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
+      <c r="G64" s="53"/>
+      <c r="H64" s="56"/>
       <c r="I64" s="12"/>
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
@@ -3005,20 +3005,20 @@
       <c r="P64" s="17"/>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="38"/>
-      <c r="C65" s="82" t="s">
+      <c r="A65" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="56"/>
+      <c r="C65" s="43" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="8"/>
-      <c r="F65" s="36" t="s">
+      <c r="F65" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="G65" s="37"/>
-      <c r="H65" s="38"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="56"/>
       <c r="I65" s="12"/>
       <c r="J65" s="17"/>
       <c r="K65" s="17"/>
@@ -3036,7 +3036,7 @@
       <c r="E66" s="9"/>
       <c r="F66" s="16"/>
       <c r="G66" s="9"/>
-      <c r="H66" s="75"/>
+      <c r="H66" s="16"/>
       <c r="I66" s="12"/>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
@@ -3054,7 +3054,7 @@
       <c r="E67" s="9"/>
       <c r="F67" s="16"/>
       <c r="G67" s="9"/>
-      <c r="H67" s="75"/>
+      <c r="H67" s="16"/>
       <c r="I67" s="12"/>
       <c r="J67" s="17"/>
       <c r="K67" s="17"/>
@@ -3068,7 +3068,7 @@
       <c r="I68" s="15"/>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
-      <c r="L68" s="81"/>
+      <c r="L68" s="42"/>
       <c r="M68" s="16"/>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
@@ -3078,15 +3078,15 @@
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="39" t="s">
+      <c r="B69" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="38"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="56"/>
       <c r="I69" s="15"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
@@ -3100,15 +3100,15 @@
       <c r="A70" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B70" s="39" t="s">
+      <c r="B70" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="37"/>
-      <c r="H70" s="38"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="56"/>
       <c r="I70" s="15"/>
       <c r="J70" s="16"/>
       <c r="K70" s="16"/>
@@ -3119,16 +3119,16 @@
       <c r="P70" s="16"/>
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="40" t="s">
+      <c r="A71" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="38"/>
+      <c r="B71" s="53"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="53"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
+      <c r="H71" s="56"/>
       <c r="I71" s="13"/>
       <c r="J71" s="13"/>
       <c r="K71" s="13"/>
@@ -3139,11 +3139,11 @@
       <c r="P71" s="13"/>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B72" s="38"/>
-      <c r="C72" s="70" t="s">
+      <c r="B72" s="56"/>
+      <c r="C72" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -3158,7 +3158,7 @@
       <c r="G72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H72" s="70" t="s">
+      <c r="H72" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I72" s="2"/>
@@ -3171,10 +3171,10 @@
       <c r="P72" s="2"/>
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="39" t="s">
+      <c r="A73" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="B73" s="38"/>
+      <c r="B73" s="56"/>
       <c r="C73" s="11" t="s">
         <v>11</v>
       </c>
@@ -3201,22 +3201,22 @@
       <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
+      <c r="A74" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="56"/>
+      <c r="C74" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="38"/>
-      <c r="C74" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="D74" s="6" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
-      <c r="H74" s="11" t="s">
+      <c r="H74" s="86" t="s">
         <v>101</v>
       </c>
       <c r="I74" s="3"/>
@@ -3229,15 +3229,15 @@
       <c r="P74" s="3"/>
     </row>
     <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="39" t="s">
+      <c r="A75" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="B75" s="38"/>
+      <c r="B75" s="56"/>
       <c r="C75" s="11" t="s">
-        <v>155</v>
+        <v>52</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>23</v>
@@ -3245,28 +3245,28 @@
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="69"/>
+      <c r="M75" s="37"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
     </row>
     <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="38"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="53"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="56"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -3277,11 +3277,11 @@
       <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B77" s="38"/>
-      <c r="C77" s="70" t="s">
+      <c r="B77" s="56"/>
+      <c r="C77" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3290,11 +3290,11 @@
       <c r="E77" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F77" s="41" t="s">
+      <c r="F77" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G77" s="37"/>
-      <c r="H77" s="38"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="56"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
@@ -3305,14 +3305,14 @@
       <c r="P77" s="2"/>
     </row>
     <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="36"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="82"/>
+      <c r="A78" s="58"/>
+      <c r="B78" s="56"/>
+      <c r="C78" s="43"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="38"/>
+      <c r="F78" s="58"/>
+      <c r="G78" s="53"/>
+      <c r="H78" s="56"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -3323,14 +3323,14 @@
       <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="36"/>
-      <c r="B79" s="38"/>
-      <c r="C79" s="82"/>
+      <c r="A79" s="58"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="43"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
-      <c r="F79" s="87"/>
-      <c r="G79" s="88"/>
-      <c r="H79" s="89"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="66"/>
+      <c r="H79" s="67"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
@@ -3343,12 +3343,12 @@
     <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="31"/>
-      <c r="C80" s="83"/>
+      <c r="C80" s="44"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="31"/>
-      <c r="H80" s="71"/>
+      <c r="H80" s="31"/>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
@@ -3361,12 +3361,12 @@
     <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="31"/>
-      <c r="C81" s="83"/>
+      <c r="C81" s="44"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="31"/>
-      <c r="H81" s="71"/>
+      <c r="H81" s="31"/>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
@@ -3390,15 +3390,15 @@
       <c r="A83" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B83" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="38"/>
+      <c r="B83" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C83" s="53"/>
+      <c r="D83" s="53"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="53"/>
+      <c r="G83" s="53"/>
+      <c r="H83" s="56"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -3412,15 +3412,15 @@
       <c r="A84" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B84" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="38"/>
+      <c r="B84" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="C84" s="53"/>
+      <c r="D84" s="53"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="53"/>
+      <c r="G84" s="53"/>
+      <c r="H84" s="56"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -3431,16 +3431,16 @@
       <c r="P84" s="2"/>
     </row>
     <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="40" t="s">
+      <c r="A85" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="37"/>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="37"/>
-      <c r="H85" s="38"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="53"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="56"/>
       <c r="I85" s="13"/>
       <c r="J85" s="13"/>
       <c r="K85" s="13"/>
@@ -3451,11 +3451,11 @@
       <c r="P85" s="13"/>
     </row>
     <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="41" t="s">
+      <c r="A86" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B86" s="38"/>
-      <c r="C86" s="70" t="s">
+      <c r="B86" s="56"/>
+      <c r="C86" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -3470,28 +3470,28 @@
       <c r="G86" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H86" s="70" t="s">
+      <c r="H86" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="K86" s="64" t="s">
-        <v>159</v>
-      </c>
-      <c r="L86" s="64"/>
-      <c r="M86" s="64"/>
-      <c r="N86" s="64"/>
-      <c r="O86" s="64"/>
-      <c r="P86" s="64"/>
-      <c r="Q86" s="64"/>
+      <c r="K86" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="L86" s="59"/>
+      <c r="M86" s="59"/>
+      <c r="N86" s="59"/>
+      <c r="O86" s="59"/>
+      <c r="P86" s="59"/>
+      <c r="Q86" s="59"/>
     </row>
     <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="B87" s="38"/>
+      <c r="A87" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="56"/>
       <c r="C87" s="11" t="s">
         <v>11</v>
       </c>
@@ -3512,21 +3512,21 @@
       <c r="J87" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="K87" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="L87" s="64"/>
-      <c r="M87" s="64"/>
-      <c r="N87" s="64"/>
-      <c r="O87" s="64"/>
-      <c r="P87" s="64"/>
-      <c r="Q87" s="64"/>
+      <c r="K87" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="L87" s="59"/>
+      <c r="M87" s="59"/>
+      <c r="N87" s="59"/>
+      <c r="O87" s="59"/>
+      <c r="P87" s="59"/>
+      <c r="Q87" s="59"/>
     </row>
     <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="39" t="s">
+      <c r="A88" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="B88" s="38"/>
+      <c r="B88" s="56"/>
       <c r="C88" s="11" t="s">
         <v>17</v>
       </c>
@@ -3544,22 +3544,22 @@
         <v>19</v>
       </c>
       <c r="I88" s="3"/>
-      <c r="J88" s="60" t="s">
+      <c r="J88" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="K88" s="60"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="60"/>
-      <c r="N88" s="60"/>
-      <c r="O88" s="60"/>
-      <c r="P88" s="60"/>
-      <c r="Q88" s="60"/>
+      <c r="K88" s="62"/>
+      <c r="L88" s="62"/>
+      <c r="M88" s="62"/>
+      <c r="N88" s="62"/>
+      <c r="O88" s="62"/>
+      <c r="P88" s="62"/>
+      <c r="Q88" s="62"/>
     </row>
     <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="39" t="s">
+      <c r="A89" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B89" s="38"/>
+      <c r="B89" s="56"/>
       <c r="C89" s="11" t="s">
         <v>11</v>
       </c>
@@ -3595,16 +3595,16 @@
       <c r="O89" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="P89" s="79" t="s">
+      <c r="P89" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="Q89" s="79"/>
+      <c r="Q89" s="63"/>
     </row>
     <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B90" s="38"/>
+      <c r="A90" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90" s="56"/>
       <c r="C90" s="11" t="s">
         <v>11</v>
       </c>
@@ -3619,17 +3619,17 @@
         <v>14</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I90" s="2"/>
       <c r="J90" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K90" s="27" t="s">
         <v>11</v>
       </c>
       <c r="L90" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M90" s="27" t="s">
         <v>13</v>
@@ -3638,16 +3638,16 @@
         <v>14</v>
       </c>
       <c r="O90" s="27"/>
-      <c r="P90" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q90" s="80"/>
+      <c r="P90" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q90" s="64"/>
     </row>
     <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="39" t="s">
+      <c r="A91" s="60" t="s">
         <v>98</v>
       </c>
-      <c r="B91" s="38"/>
+      <c r="B91" s="56"/>
       <c r="C91" s="11" t="s">
         <v>11</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>14</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="27" t="s">
@@ -3679,21 +3679,21 @@
       </c>
       <c r="N91" s="27"/>
       <c r="O91" s="27"/>
-      <c r="P91" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q91" s="80"/>
+      <c r="P91" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q91" s="64"/>
     </row>
     <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B92" s="18"/>
       <c r="C92" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>23</v>
@@ -3701,7 +3701,7 @@
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
       <c r="H92" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I92" s="2"/>
       <c r="J92" s="4"/>
@@ -3713,10 +3713,10 @@
       <c r="P92" s="4"/>
     </row>
     <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B93" s="38"/>
+      <c r="A93" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="B93" s="56"/>
       <c r="C93" s="11" t="s">
         <v>11</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>14</v>
       </c>
       <c r="H93" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="4"/>
@@ -3743,16 +3743,16 @@
       <c r="P93" s="4"/>
     </row>
     <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="41" t="s">
+      <c r="A94" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B94" s="37"/>
-      <c r="C94" s="37"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="37"/>
-      <c r="H94" s="38"/>
+      <c r="B94" s="53"/>
+      <c r="C94" s="53"/>
+      <c r="D94" s="53"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="53"/>
+      <c r="G94" s="53"/>
+      <c r="H94" s="56"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -3763,11 +3763,11 @@
       <c r="P94" s="2"/>
     </row>
     <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="41" t="s">
+      <c r="A95" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B95" s="38"/>
-      <c r="C95" s="70" t="s">
+      <c r="B95" s="56"/>
+      <c r="C95" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -3776,11 +3776,11 @@
       <c r="E95" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F95" s="41" t="s">
+      <c r="F95" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G95" s="37"/>
-      <c r="H95" s="38"/>
+      <c r="G95" s="53"/>
+      <c r="H95" s="56"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
@@ -3791,14 +3791,14 @@
       <c r="P95" s="2"/>
     </row>
     <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="36"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="82"/>
+      <c r="A96" s="58"/>
+      <c r="B96" s="56"/>
+      <c r="C96" s="43"/>
       <c r="D96" s="8"/>
       <c r="E96" s="8"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="37"/>
-      <c r="H96" s="38"/>
+      <c r="F96" s="58"/>
+      <c r="G96" s="53"/>
+      <c r="H96" s="56"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -3809,109 +3809,109 @@
       <c r="P96" s="2"/>
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="36"/>
-      <c r="B97" s="38"/>
-      <c r="C97" s="82"/>
+      <c r="A97" s="58"/>
+      <c r="B97" s="56"/>
+      <c r="C97" s="43"/>
       <c r="D97" s="8"/>
       <c r="E97" s="8"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="37"/>
-      <c r="H97" s="38"/>
+      <c r="F97" s="58"/>
+      <c r="G97" s="53"/>
+      <c r="H97" s="56"/>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="48"/>
-      <c r="B98" s="49"/>
-      <c r="C98" s="49"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="49"/>
-      <c r="F98" s="49"/>
-      <c r="G98" s="49"/>
-      <c r="H98" s="50"/>
+      <c r="A98" s="80"/>
+      <c r="B98" s="75"/>
+      <c r="C98" s="75"/>
+      <c r="D98" s="75"/>
+      <c r="E98" s="75"/>
+      <c r="F98" s="75"/>
+      <c r="G98" s="75"/>
+      <c r="H98" s="81"/>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="51"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="52"/>
-      <c r="D99" s="52"/>
-      <c r="E99" s="52"/>
-      <c r="F99" s="52"/>
-      <c r="G99" s="52"/>
-      <c r="H99" s="53"/>
+      <c r="A99" s="82"/>
+      <c r="B99" s="76"/>
+      <c r="C99" s="76"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="83"/>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="51"/>
-      <c r="B100" s="52"/>
-      <c r="C100" s="52"/>
-      <c r="D100" s="52"/>
-      <c r="E100" s="52"/>
-      <c r="F100" s="52"/>
-      <c r="G100" s="52"/>
-      <c r="H100" s="53"/>
+      <c r="A100" s="82"/>
+      <c r="B100" s="76"/>
+      <c r="C100" s="76"/>
+      <c r="D100" s="76"/>
+      <c r="E100" s="76"/>
+      <c r="F100" s="76"/>
+      <c r="G100" s="76"/>
+      <c r="H100" s="83"/>
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="54"/>
-      <c r="B101" s="55"/>
-      <c r="C101" s="55"/>
-      <c r="D101" s="55"/>
-      <c r="E101" s="55"/>
-      <c r="F101" s="55"/>
-      <c r="G101" s="55"/>
-      <c r="H101" s="56"/>
+      <c r="A101" s="84"/>
+      <c r="B101" s="77"/>
+      <c r="C101" s="77"/>
+      <c r="D101" s="77"/>
+      <c r="E101" s="77"/>
+      <c r="F101" s="77"/>
+      <c r="G101" s="77"/>
+      <c r="H101" s="85"/>
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="C102" s="37"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="37"/>
-      <c r="F102" s="37"/>
-      <c r="G102" s="37"/>
-      <c r="H102" s="38"/>
+      <c r="B102" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="C102" s="53"/>
+      <c r="D102" s="53"/>
+      <c r="E102" s="53"/>
+      <c r="F102" s="53"/>
+      <c r="G102" s="53"/>
+      <c r="H102" s="56"/>
       <c r="I102" s="2"/>
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B103" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C103" s="37"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="37"/>
-      <c r="F103" s="37"/>
-      <c r="G103" s="37"/>
-      <c r="H103" s="38"/>
+      <c r="B103" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C103" s="53"/>
+      <c r="D103" s="53"/>
+      <c r="E103" s="53"/>
+      <c r="F103" s="53"/>
+      <c r="G103" s="53"/>
+      <c r="H103" s="56"/>
       <c r="I103" s="2"/>
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="40" t="s">
+      <c r="A104" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B104" s="37"/>
-      <c r="C104" s="37"/>
-      <c r="D104" s="37"/>
-      <c r="E104" s="37"/>
-      <c r="F104" s="37"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="38"/>
+      <c r="B104" s="53"/>
+      <c r="C104" s="53"/>
+      <c r="D104" s="53"/>
+      <c r="E104" s="53"/>
+      <c r="F104" s="53"/>
+      <c r="G104" s="53"/>
+      <c r="H104" s="56"/>
       <c r="I104" s="2"/>
     </row>
     <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="41" t="s">
+      <c r="A105" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B105" s="38"/>
-      <c r="C105" s="70" t="s">
+      <c r="B105" s="56"/>
+      <c r="C105" s="38" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -3926,16 +3926,16 @@
       <c r="G105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H105" s="70" t="s">
+      <c r="H105" s="38" t="s">
         <v>1</v>
       </c>
       <c r="I105" s="2"/>
     </row>
     <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="38"/>
+      <c r="A106" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="56"/>
       <c r="C106" s="11" t="s">
         <v>11</v>
       </c>
@@ -3950,15 +3950,15 @@
       </c>
       <c r="G106" s="5"/>
       <c r="H106" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I106" s="2"/>
     </row>
     <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="39" t="s">
+      <c r="A107" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="B107" s="38"/>
+      <c r="B107" s="56"/>
       <c r="C107" s="11" t="s">
         <v>17</v>
       </c>
@@ -3971,29 +3971,29 @@
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
       <c r="H107" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I107" s="3"/>
     </row>
     <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="41" t="s">
+      <c r="A108" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="B108" s="37"/>
-      <c r="C108" s="37"/>
-      <c r="D108" s="37"/>
-      <c r="E108" s="37"/>
-      <c r="F108" s="37"/>
-      <c r="G108" s="37"/>
-      <c r="H108" s="38"/>
+      <c r="B108" s="53"/>
+      <c r="C108" s="53"/>
+      <c r="D108" s="53"/>
+      <c r="E108" s="53"/>
+      <c r="F108" s="53"/>
+      <c r="G108" s="53"/>
+      <c r="H108" s="56"/>
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="41" t="s">
+      <c r="A109" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="B109" s="38"/>
-      <c r="C109" s="70" t="s">
+      <c r="B109" s="56"/>
+      <c r="C109" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -4002,33 +4002,33 @@
       <c r="E109" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F109" s="41" t="s">
+      <c r="F109" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G109" s="37"/>
-      <c r="H109" s="38"/>
+      <c r="G109" s="53"/>
+      <c r="H109" s="56"/>
       <c r="I109" s="2"/>
     </row>
     <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="36"/>
-      <c r="B110" s="38"/>
-      <c r="C110" s="82"/>
+      <c r="A110" s="58"/>
+      <c r="B110" s="56"/>
+      <c r="C110" s="43"/>
       <c r="D110" s="8"/>
       <c r="E110" s="8"/>
-      <c r="F110" s="36"/>
-      <c r="G110" s="37"/>
-      <c r="H110" s="38"/>
+      <c r="F110" s="58"/>
+      <c r="G110" s="53"/>
+      <c r="H110" s="56"/>
       <c r="I110" s="2"/>
     </row>
     <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="36"/>
-      <c r="B111" s="38"/>
-      <c r="C111" s="82"/>
+      <c r="A111" s="58"/>
+      <c r="B111" s="56"/>
+      <c r="C111" s="43"/>
       <c r="D111" s="8"/>
       <c r="E111" s="8"/>
-      <c r="F111" s="36"/>
-      <c r="G111" s="37"/>
-      <c r="H111" s="38"/>
+      <c r="F111" s="58"/>
+      <c r="G111" s="53"/>
+      <c r="H111" s="56"/>
       <c r="I111" s="4"/>
       <c r="J111" s="20"/>
       <c r="K111" s="20"/>
@@ -4036,12 +4036,12 @@
     <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="31"/>
-      <c r="C112" s="83"/>
+      <c r="C112" s="44"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="31"/>
-      <c r="H112" s="71"/>
+      <c r="H112" s="31"/>
       <c r="I112" s="4"/>
       <c r="J112" s="20"/>
       <c r="K112" s="20"/>
@@ -4049,12 +4049,12 @@
     <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="31"/>
-      <c r="C113" s="83"/>
+      <c r="C113" s="44"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="31"/>
-      <c r="H113" s="71"/>
+      <c r="H113" s="31"/>
       <c r="I113" s="4"/>
       <c r="J113" s="20"/>
       <c r="K113" s="20"/>
@@ -4062,12 +4062,12 @@
     <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="31"/>
-      <c r="C114" s="83"/>
+      <c r="C114" s="44"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="31"/>
-      <c r="H114" s="71"/>
+      <c r="H114" s="31"/>
       <c r="I114" s="4"/>
       <c r="J114" s="20"/>
       <c r="K114" s="20"/>
@@ -4079,57 +4079,57 @@
       <c r="A116" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B116" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="C116" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D116" s="44"/>
-      <c r="E116" s="44"/>
-      <c r="F116" s="44"/>
-      <c r="G116" s="44"/>
-      <c r="H116" s="44"/>
+      <c r="B116" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C116" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="D116" s="78"/>
+      <c r="E116" s="78"/>
+      <c r="F116" s="78"/>
+      <c r="G116" s="78"/>
+      <c r="H116" s="78"/>
       <c r="I116" s="2"/>
     </row>
     <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B117" s="43" t="s">
-        <v>125</v>
-      </c>
-      <c r="C117" s="44"/>
-      <c r="D117" s="44"/>
-      <c r="E117" s="44"/>
-      <c r="F117" s="44"/>
-      <c r="G117" s="44"/>
-      <c r="H117" s="44"/>
+      <c r="B117" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C117" s="78"/>
+      <c r="D117" s="78"/>
+      <c r="E117" s="78"/>
+      <c r="F117" s="78"/>
+      <c r="G117" s="78"/>
+      <c r="H117" s="78"/>
       <c r="I117" s="2"/>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="46" t="s">
+      <c r="A118" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B118" s="44"/>
-      <c r="C118" s="44"/>
-      <c r="D118" s="44"/>
-      <c r="E118" s="44"/>
-      <c r="F118" s="44"/>
-      <c r="G118" s="44"/>
-      <c r="H118" s="44"/>
+      <c r="B118" s="78"/>
+      <c r="C118" s="78"/>
+      <c r="D118" s="78"/>
+      <c r="E118" s="78"/>
+      <c r="F118" s="78"/>
+      <c r="G118" s="78"/>
+      <c r="H118" s="78"/>
       <c r="I118" s="13"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="47" t="s">
+      <c r="A119" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" s="78"/>
+      <c r="C119" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="B119" s="44"/>
-      <c r="C119" s="76" t="s">
+      <c r="D119" s="21" t="s">
         <v>120</v>
-      </c>
-      <c r="D119" s="21" t="s">
-        <v>121</v>
       </c>
       <c r="E119" s="21" t="s">
         <v>7</v>
@@ -4140,21 +4140,21 @@
       <c r="G119" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H119" s="76" t="s">
+      <c r="H119" s="40" t="s">
         <v>1</v>
       </c>
       <c r="I119" s="20"/>
     </row>
     <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="43" t="s">
+      <c r="A120" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B120" s="44"/>
-      <c r="C120" s="85" t="s">
+      <c r="B120" s="78"/>
+      <c r="C120" s="46" t="s">
         <v>91</v>
       </c>
       <c r="D120" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E120" s="22" t="s">
         <v>13</v>
@@ -4163,18 +4163,18 @@
         <v>14</v>
       </c>
       <c r="G120" s="22"/>
-      <c r="H120" s="77" t="s">
-        <v>126</v>
+      <c r="H120" s="41" t="s">
+        <v>125</v>
       </c>
       <c r="I120" s="20"/>
-      <c r="K120" s="90"/>
+      <c r="K120" s="48"/>
     </row>
     <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="43" t="s">
+      <c r="A121" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B121" s="44"/>
-      <c r="C121" s="85" t="s">
+      <c r="B121" s="78"/>
+      <c r="C121" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D121" s="24" t="s">
@@ -4187,17 +4187,17 @@
       <c r="G121" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H121" s="77" t="s">
-        <v>128</v>
+      <c r="H121" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="I121" s="20"/>
     </row>
     <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="B122" s="44"/>
-      <c r="C122" s="85" t="s">
+      <c r="A122" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" s="78"/>
+      <c r="C122" s="46" t="s">
         <v>26</v>
       </c>
       <c r="D122" s="22" t="s">
@@ -4208,17 +4208,17 @@
       </c>
       <c r="F122" s="22"/>
       <c r="G122" s="22"/>
-      <c r="H122" s="77" t="s">
-        <v>129</v>
+      <c r="H122" s="41" t="s">
+        <v>128</v>
       </c>
       <c r="I122" s="20"/>
     </row>
     <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B123" s="44"/>
-      <c r="C123" s="85" t="s">
+      <c r="A123" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" s="78"/>
+      <c r="C123" s="46" t="s">
         <v>26</v>
       </c>
       <c r="D123" s="24" t="s">
@@ -4229,38 +4229,38 @@
       </c>
       <c r="F123" s="22"/>
       <c r="G123" s="22"/>
-      <c r="H123" s="77" t="s">
-        <v>130</v>
+      <c r="H123" s="41" t="s">
+        <v>129</v>
       </c>
       <c r="I123" s="20"/>
     </row>
     <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="B124" s="44"/>
-      <c r="C124" s="86" t="s">
-        <v>127</v>
+      <c r="A124" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" s="78"/>
+      <c r="C124" s="47" t="s">
+        <v>126</v>
       </c>
       <c r="D124" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E124" s="25" t="s">
         <v>13</v>
       </c>
       <c r="F124" s="22"/>
       <c r="G124" s="22"/>
-      <c r="H124" s="77" t="s">
-        <v>132</v>
+      <c r="H124" s="41" t="s">
+        <v>131</v>
       </c>
       <c r="I124" s="20"/>
     </row>
     <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="45" t="s">
+      <c r="A125" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B125" s="44"/>
-      <c r="C125" s="86" t="s">
+      <c r="B125" s="78"/>
+      <c r="C125" s="47" t="s">
         <v>11</v>
       </c>
       <c r="D125" s="25" t="s">
@@ -4273,8 +4273,8 @@
       <c r="G125" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H125" s="78" t="s">
-        <v>131</v>
+      <c r="H125" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="I125" s="20"/>
     </row>
@@ -6992,16 +6992,123 @@
     </row>
   </sheetData>
   <mergeCells count="148">
-    <mergeCell ref="K55:Q55"/>
-    <mergeCell ref="J56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="J60:Q60"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="O61:Q61"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="O62:Q62"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:H94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="B117:H117"/>
+    <mergeCell ref="A118:H118"/>
+    <mergeCell ref="B116:H116"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A98:H101"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="K54:Q54"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="A53:H53"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="K34:Q34"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="A13:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="B51:H51"/>
+    <mergeCell ref="J40:Q40"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="O41:Q41"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="O42:Q42"/>
+    <mergeCell ref="J36:Q36"/>
+    <mergeCell ref="K35:Q35"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A63:H63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="A85:H85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A71:H71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="B83:H83"/>
     <mergeCell ref="K86:Q86"/>
     <mergeCell ref="B103:H103"/>
     <mergeCell ref="B102:H102"/>
@@ -7023,123 +7130,16 @@
     <mergeCell ref="P89:Q89"/>
     <mergeCell ref="P90:Q90"/>
     <mergeCell ref="P91:Q91"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="A85:H85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="B83:H83"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A63:H63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="J40:Q40"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="O41:Q41"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="O42:Q42"/>
-    <mergeCell ref="J36:Q36"/>
-    <mergeCell ref="K35:Q35"/>
-    <mergeCell ref="K34:Q34"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="A13:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="K54:Q54"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="B117:H117"/>
-    <mergeCell ref="A118:H118"/>
-    <mergeCell ref="B116:H116"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A98:H101"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="A53:H53"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="J56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="J60:Q60"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="O61:Q61"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="O62:Q62"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
atualização de tamanho das colunas
</commit_message>
<xml_diff>
--- a/dicionario_tabelas/dicionario.xlsx
+++ b/dicionario_tabelas/dicionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\APENAS MEU\Faculdade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0256EC59-7D8C-4465-A2B1-0971E64FBD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B68E84-96B9-4E4B-B457-61A33AC92094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1308,11 +1308,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1030"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
@@ -1331,7 +1331,7 @@
     <col min="17" max="17" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>3</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="55" t="s">
         <v>4</v>
       </c>
@@ -1427,7 +1427,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>10</v>
       </c>
@@ -1457,7 +1457,7 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>20</v>
       </c>
@@ -1513,7 +1513,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>29</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>30</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
         <v>162</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="57"/>
       <c r="B12" s="57"/>
       <c r="C12" s="57"/>
@@ -1633,7 +1633,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="57"/>
       <c r="B13" s="57"/>
       <c r="C13" s="57"/>
@@ -1651,7 +1651,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="57"/>
       <c r="B14" s="57"/>
       <c r="C14" s="57"/>
@@ -1669,7 +1669,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="57"/>
       <c r="B15" s="57"/>
       <c r="C15" s="57"/>
@@ -1687,7 +1687,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="P16" s="78"/>
       <c r="Q16" s="78"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1">
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>1</v>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="P17" s="78"/>
       <c r="Q17" s="78"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>3</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="P18" s="79"/>
       <c r="Q18" s="79"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="55" t="s">
         <v>4</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="Q19" s="79"/>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1">
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
         <v>36</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="Q20" s="83"/>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1">
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
         <v>38</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="Q21" s="83"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>143</v>
       </c>
@@ -1926,7 +1926,7 @@
       <c r="P22" s="84"/>
       <c r="Q22" s="85"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>29</v>
       </c>
@@ -1957,7 +1957,7 @@
       <c r="P23" s="62"/>
       <c r="Q23" s="62"/>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1">
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="55" t="s">
         <v>30</v>
       </c>
@@ -1994,7 +1994,7 @@
       <c r="P24" s="86"/>
       <c r="Q24" s="86"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="59" t="s">
         <v>161</v>
       </c>
@@ -2020,7 +2020,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="56"/>
       <c r="B26" s="56"/>
       <c r="C26" s="56"/>
@@ -2038,7 +2038,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="57"/>
       <c r="B27" s="57"/>
       <c r="C27" s="57"/>
@@ -2056,7 +2056,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="57"/>
       <c r="B28" s="57"/>
       <c r="C28" s="57"/>
@@ -2074,7 +2074,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="58"/>
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
@@ -2092,7 +2092,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -2119,7 +2119,7 @@
       <c r="P30" s="87"/>
       <c r="Q30" s="70"/>
     </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1">
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="P31" s="87"/>
       <c r="Q31" s="70"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="51" t="s">
         <v>3</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="P32" s="68"/>
       <c r="Q32" s="68"/>
     </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1">
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2216,7 @@
       </c>
       <c r="Q33" s="89"/>
     </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1">
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="71" t="s">
         <v>44</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="Q34" s="70"/>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1">
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
         <v>48</v>
       </c>
@@ -2298,7 +2298,7 @@
       </c>
       <c r="Q35" s="70"/>
     </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1">
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
         <v>20</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="P36" s="53"/>
       <c r="Q36" s="54"/>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1">
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
         <v>25</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="P37" s="49"/>
       <c r="Q37" s="50"/>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1">
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
         <v>58</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="P38" s="49"/>
       <c r="Q38" s="50"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1">
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
         <v>61</v>
       </c>
@@ -2433,7 +2433,7 @@
       <c r="O39" s="9"/>
       <c r="P39" s="9"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1">
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
         <v>63</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1">
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>65</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" customHeight="1">
+    <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48" t="s">
         <v>46</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" customHeight="1">
+    <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>29</v>
       </c>
@@ -2539,7 +2539,7 @@
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
     </row>
-    <row r="44" spans="1:17" ht="15.75" customHeight="1">
+    <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="55" t="s">
         <v>30</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
     </row>
-    <row r="45" spans="1:17" ht="15.75" customHeight="1">
+    <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="72" t="s">
         <v>155</v>
       </c>
@@ -2593,7 +2593,7 @@
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1">
+    <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="56"/>
       <c r="B46" s="56"/>
       <c r="C46" s="56"/>
@@ -2611,7 +2611,7 @@
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
     </row>
-    <row r="47" spans="1:17" ht="15.75" customHeight="1">
+    <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="57"/>
       <c r="B47" s="57"/>
       <c r="C47" s="57"/>
@@ -2629,7 +2629,7 @@
       <c r="O47" s="9"/>
       <c r="P47" s="9"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" customHeight="1">
+    <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="57"/>
       <c r="B48" s="57"/>
       <c r="C48" s="57"/>
@@ -2647,7 +2647,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
     </row>
-    <row r="49" spans="1:17" ht="15.75" customHeight="1">
+    <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="58"/>
       <c r="B49" s="58"/>
       <c r="C49" s="58"/>
@@ -2665,7 +2665,7 @@
       <c r="O49" s="9"/>
       <c r="P49" s="9"/>
     </row>
-    <row r="50" spans="1:17" ht="15.75" customHeight="1">
+    <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="P50" s="60"/>
       <c r="Q50" s="60"/>
     </row>
-    <row r="51" spans="1:17" ht="27.75" customHeight="1">
+    <row r="51" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
@@ -2719,7 +2719,7 @@
       <c r="P51" s="60"/>
       <c r="Q51" s="60"/>
     </row>
-    <row r="52" spans="1:17" ht="15.75" customHeight="1">
+    <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="51" t="s">
         <v>3</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="P52" s="62"/>
       <c r="Q52" s="62"/>
     </row>
-    <row r="53" spans="1:17" ht="15.75" customHeight="1">
+    <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="55" t="s">
         <v>4</v>
       </c>
@@ -2789,7 +2789,7 @@
       </c>
       <c r="Q53" s="82"/>
     </row>
-    <row r="54" spans="1:17" ht="15.75" customHeight="1">
+    <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
         <v>72</v>
       </c>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="Q54" s="60"/>
     </row>
-    <row r="55" spans="1:17" ht="15.75" customHeight="1">
+    <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
         <v>76</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="Q55" s="60"/>
     </row>
-    <row r="56" spans="1:17" ht="15.75" customHeight="1">
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>80</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="P56" s="53"/>
       <c r="Q56" s="54"/>
     </row>
-    <row r="57" spans="1:17" ht="15.75" customHeight="1">
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="74" t="s">
         <v>82</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="P57" s="49"/>
       <c r="Q57" s="50"/>
     </row>
-    <row r="58" spans="1:17" ht="15.75" customHeight="1">
+    <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
         <v>44</v>
       </c>
@@ -2980,7 +2980,7 @@
       <c r="P58" s="49"/>
       <c r="Q58" s="50"/>
     </row>
-    <row r="59" spans="1:17" ht="15.75" customHeight="1">
+    <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="73" t="s">
         <v>87</v>
       </c>
@@ -3010,7 +3010,7 @@
       <c r="O59" s="17"/>
       <c r="P59" s="17"/>
     </row>
-    <row r="60" spans="1:17" ht="15.75" customHeight="1">
+    <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="73" t="s">
         <v>91</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="O60" s="17"/>
       <c r="P60" s="17"/>
     </row>
-    <row r="61" spans="1:17" ht="15.75" customHeight="1">
+    <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
         <v>74</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="O61" s="17"/>
       <c r="P61" s="17"/>
     </row>
-    <row r="62" spans="1:17" ht="15.75" customHeight="1">
+    <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="55" t="s">
         <v>29</v>
       </c>
@@ -3090,7 +3090,7 @@
       <c r="O62" s="17"/>
       <c r="P62" s="17"/>
     </row>
-    <row r="63" spans="1:17" ht="15.75" customHeight="1">
+    <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="55" t="s">
         <v>30</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="O63" s="17"/>
       <c r="P63" s="17"/>
     </row>
-    <row r="64" spans="1:17" ht="15.75" customHeight="1">
+    <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="59" t="s">
         <v>154</v>
       </c>
@@ -3142,7 +3142,7 @@
       <c r="O64" s="16"/>
       <c r="P64" s="16"/>
     </row>
-    <row r="65" spans="1:16" ht="15.75" customHeight="1">
+    <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56"/>
       <c r="B65" s="56"/>
       <c r="C65" s="56"/>
@@ -3160,7 +3160,7 @@
       <c r="O65" s="16"/>
       <c r="P65" s="16"/>
     </row>
-    <row r="66" spans="1:16" ht="15.75" customHeight="1">
+    <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="57"/>
       <c r="B66" s="57"/>
       <c r="C66" s="57"/>
@@ -3178,7 +3178,7 @@
       <c r="O66" s="16"/>
       <c r="P66" s="16"/>
     </row>
-    <row r="67" spans="1:16" ht="15.75" customHeight="1">
+    <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="57"/>
       <c r="B67" s="57"/>
       <c r="C67" s="57"/>
@@ -3196,7 +3196,7 @@
       <c r="O67" s="16"/>
       <c r="P67" s="16"/>
     </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1">
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="58"/>
       <c r="B68" s="58"/>
       <c r="C68" s="58"/>
@@ -3214,7 +3214,7 @@
       <c r="O68" s="13"/>
       <c r="P68" s="13"/>
     </row>
-    <row r="69" spans="1:16" ht="15.75" customHeight="1">
+    <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3236,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="1:16" ht="15.75" customHeight="1">
+    <row r="70" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>1</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" ht="15.75" customHeight="1">
+    <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="51" t="s">
         <v>3</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
-    <row r="72" spans="1:16" ht="15.75" customHeight="1">
+    <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="55" t="s">
         <v>4</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="O72" s="4"/>
       <c r="P72" s="4"/>
     </row>
-    <row r="73" spans="1:16" ht="15.75" customHeight="1">
+    <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
         <v>95</v>
       </c>
@@ -3340,7 +3340,7 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" ht="15.75" customHeight="1">
+    <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
         <v>147</v>
       </c>
@@ -3368,7 +3368,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" ht="15.75" customHeight="1">
+    <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
         <v>99</v>
       </c>
@@ -3396,7 +3396,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" ht="15.75" customHeight="1">
+    <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="55" t="s">
         <v>29</v>
       </c>
@@ -3416,7 +3416,7 @@
       <c r="O76" s="4"/>
       <c r="P76" s="4"/>
     </row>
-    <row r="77" spans="1:16" ht="15.75" customHeight="1">
+    <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="55" t="s">
         <v>30</v>
       </c>
@@ -3444,7 +3444,7 @@
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
     </row>
-    <row r="78" spans="1:16" ht="15.75" customHeight="1">
+    <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="59" t="s">
         <v>166</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="O78" s="4"/>
       <c r="P78" s="4"/>
     </row>
-    <row r="79" spans="1:16" ht="15.75" customHeight="1">
+    <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="59"/>
       <c r="B79" s="50"/>
       <c r="C79" s="39"/>
@@ -3486,7 +3486,7 @@
       <c r="O79" s="4"/>
       <c r="P79" s="4"/>
     </row>
-    <row r="80" spans="1:16" ht="15.75" customHeight="1">
+    <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="56"/>
       <c r="B80" s="56"/>
       <c r="C80" s="56"/>
@@ -3504,7 +3504,7 @@
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="1:17" ht="15.75" customHeight="1">
+    <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="57"/>
       <c r="B81" s="57"/>
       <c r="C81" s="57"/>
@@ -3522,7 +3522,7 @@
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="1:17" ht="15.75" customHeight="1">
+    <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="57"/>
       <c r="B82" s="57"/>
       <c r="C82" s="57"/>
@@ -3540,7 +3540,7 @@
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="1:17" ht="15.75" customHeight="1">
+    <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="58"/>
       <c r="B83" s="58"/>
       <c r="C83" s="58"/>
@@ -3558,7 +3558,7 @@
       <c r="O83" s="13"/>
       <c r="P83" s="13"/>
     </row>
-    <row r="84" spans="1:17" ht="15.75" customHeight="1">
+    <row r="84" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -3585,7 +3585,7 @@
       <c r="P84" s="78"/>
       <c r="Q84" s="78"/>
     </row>
-    <row r="85" spans="1:17" ht="15.75" customHeight="1">
+    <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>1</v>
       </c>
@@ -3612,7 +3612,7 @@
       <c r="P85" s="78"/>
       <c r="Q85" s="78"/>
     </row>
-    <row r="86" spans="1:17" ht="15.75" customHeight="1">
+    <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="51" t="s">
         <v>3</v>
       </c>
@@ -3635,7 +3635,7 @@
       <c r="P86" s="79"/>
       <c r="Q86" s="79"/>
     </row>
-    <row r="87" spans="1:17" ht="15.75" customHeight="1">
+    <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="55" t="s">
         <v>4</v>
       </c>
@@ -3682,7 +3682,7 @@
       </c>
       <c r="Q87" s="80"/>
     </row>
-    <row r="88" spans="1:17" ht="15.75" customHeight="1">
+    <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
         <v>102</v>
       </c>
@@ -3725,16 +3725,16 @@
       </c>
       <c r="Q88" s="81"/>
     </row>
-    <row r="89" spans="1:17" ht="15.75" customHeight="1">
+    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
         <v>87</v>
       </c>
       <c r="B89" s="50"/>
       <c r="C89" s="11" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>13</v>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="Q89" s="81"/>
     </row>
-    <row r="90" spans="1:17" ht="15.75" customHeight="1">
+    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="48" t="s">
         <v>44</v>
       </c>
@@ -3799,7 +3799,7 @@
       <c r="P90" s="53"/>
       <c r="Q90" s="54"/>
     </row>
-    <row r="91" spans="1:17" ht="15.75" customHeight="1">
+    <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
         <v>103</v>
       </c>
@@ -3840,7 +3840,7 @@
       <c r="P91" s="49"/>
       <c r="Q91" s="50"/>
     </row>
-    <row r="92" spans="1:17" ht="15.75" customHeight="1">
+    <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
         <v>95</v>
       </c>
@@ -3879,7 +3879,7 @@
       <c r="P92" s="49"/>
       <c r="Q92" s="50"/>
     </row>
-    <row r="93" spans="1:17" ht="15.75" customHeight="1">
+    <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="19" t="s">
         <v>139</v>
       </c>
@@ -3907,7 +3907,7 @@
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
     </row>
-    <row r="94" spans="1:17" ht="15.75" customHeight="1">
+    <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="48" t="s">
         <v>142</v>
       </c>
@@ -3937,7 +3937,7 @@
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
     </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1">
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="55" t="s">
         <v>29</v>
       </c>
@@ -3950,7 +3950,7 @@
       <c r="H95" s="50"/>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:17" ht="15.75" customHeight="1">
+    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="55" t="s">
         <v>30</v>
       </c>
@@ -3971,7 +3971,7 @@
       <c r="H96" s="50"/>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:11" ht="15.75" customHeight="1">
+    <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="59" t="s">
         <v>167</v>
       </c>
@@ -3988,7 +3988,7 @@
       <c r="H97" s="50"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:11" ht="15.75" customHeight="1">
+    <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="59"/>
       <c r="B98" s="50"/>
       <c r="C98" s="39"/>
@@ -3999,7 +3999,7 @@
       <c r="H98" s="50"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:11" ht="15.75" customHeight="1">
+    <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="63"/>
       <c r="B99" s="56"/>
       <c r="C99" s="56"/>
@@ -4010,7 +4010,7 @@
       <c r="H99" s="56"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:11" ht="15.75" customHeight="1">
+    <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="64"/>
       <c r="B100" s="57"/>
       <c r="C100" s="57"/>
@@ -4021,7 +4021,7 @@
       <c r="H100" s="57"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:11" ht="15.75" customHeight="1">
+    <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="64"/>
       <c r="B101" s="57"/>
       <c r="C101" s="57"/>
@@ -4032,7 +4032,7 @@
       <c r="H101" s="57"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:11" ht="15.75" customHeight="1">
+    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="65"/>
       <c r="B102" s="58"/>
       <c r="C102" s="58"/>
@@ -4043,7 +4043,7 @@
       <c r="H102" s="58"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:11" ht="15.75" customHeight="1">
+    <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="H103" s="50"/>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:11" ht="15.75" customHeight="1">
+    <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>1</v>
       </c>
@@ -4073,7 +4073,7 @@
       <c r="H104" s="50"/>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:11" ht="15.75" customHeight="1">
+    <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="51" t="s">
         <v>3</v>
       </c>
@@ -4086,7 +4086,7 @@
       <c r="H105" s="50"/>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:11" ht="15.75" customHeight="1">
+    <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="55" t="s">
         <v>4</v>
       </c>
@@ -4111,7 +4111,7 @@
       </c>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:11" ht="15.75" customHeight="1">
+    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="48" t="s">
         <v>103</v>
       </c>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:11" ht="15.75" customHeight="1">
+    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="48" t="s">
         <v>99</v>
       </c>
@@ -4155,7 +4155,7 @@
       </c>
       <c r="I108" s="3"/>
     </row>
-    <row r="109" spans="1:11" ht="15.75" customHeight="1">
+    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="55" t="s">
         <v>29</v>
       </c>
@@ -4170,7 +4170,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" ht="15.75" customHeight="1">
+    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
         <v>30</v>
       </c>
@@ -4193,7 +4193,7 @@
       <c r="J110" s="20"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" ht="15.75" customHeight="1">
+    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="59" t="s">
         <v>164</v>
       </c>
@@ -4214,7 +4214,7 @@
       <c r="J111" s="20"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" ht="15.75" customHeight="1">
+    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="59" t="s">
         <v>165</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" ht="15.75" customHeight="1">
+    <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="56"/>
       <c r="B113" s="56"/>
       <c r="C113" s="56"/>
@@ -4244,7 +4244,7 @@
       <c r="H113" s="56"/>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" spans="1:11" ht="15.75" customHeight="1">
+    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="57"/>
       <c r="B114" s="57"/>
       <c r="C114" s="57"/>
@@ -4255,7 +4255,7 @@
       <c r="H114" s="57"/>
       <c r="I114" s="4"/>
     </row>
-    <row r="115" spans="1:11" ht="15.75" customHeight="1">
+    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="57"/>
       <c r="B115" s="57"/>
       <c r="C115" s="57"/>
@@ -4266,7 +4266,7 @@
       <c r="H115" s="57"/>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" spans="1:11" ht="15.75" customHeight="1">
+    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="66"/>
       <c r="B116" s="66"/>
       <c r="C116" s="66"/>
@@ -4277,7 +4277,7 @@
       <c r="H116" s="66"/>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" spans="1:11" ht="15.75" customHeight="1">
+    <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="21" t="s">
         <v>0</v>
       </c>
@@ -4294,7 +4294,7 @@
       <c r="H117" s="61"/>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:11" ht="15.75" customHeight="1">
+    <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="21" t="s">
         <v>1</v>
       </c>
@@ -4310,7 +4310,7 @@
       <c r="I118" s="2"/>
       <c r="K118" s="43"/>
     </row>
-    <row r="119" spans="1:11" ht="15.75" customHeight="1">
+    <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="62" t="s">
         <v>3</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="H119" s="61"/>
       <c r="I119" s="13"/>
     </row>
-    <row r="120" spans="1:11" ht="15.75" customHeight="1">
+    <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="82" t="s">
         <v>115</v>
       </c>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="I120" s="20"/>
     </row>
-    <row r="121" spans="1:11" ht="15.75" customHeight="1">
+    <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="60" t="s">
         <v>87</v>
       </c>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="I121" s="20"/>
     </row>
-    <row r="122" spans="1:11" ht="15.75" customHeight="1">
+    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="60" t="s">
         <v>10</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="I122" s="20"/>
     </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1">
+    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="60" t="s">
         <v>118</v>
       </c>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="I123" s="20"/>
     </row>
-    <row r="124" spans="1:11" ht="15.75" customHeight="1">
+    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="60" t="s">
         <v>119</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="I124" s="20"/>
     </row>
-    <row r="125" spans="1:11" ht="15.75" customHeight="1">
+    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="90" t="s">
         <v>120</v>
       </c>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="I125" s="20"/>
     </row>
-    <row r="126" spans="1:11" ht="15.75" customHeight="1">
+    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="90" t="s">
         <v>36</v>
       </c>
@@ -4480,7 +4480,7 @@
       </c>
       <c r="I126" s="20"/>
     </row>
-    <row r="127" spans="1:11" ht="15.75" customHeight="1">
+    <row r="127" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="55" t="s">
         <v>29</v>
       </c>
@@ -4493,7 +4493,7 @@
       <c r="H127" s="54"/>
       <c r="I127" s="20"/>
     </row>
-    <row r="128" spans="1:11" ht="15.75" customHeight="1">
+    <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="55" t="s">
         <v>30</v>
       </c>
@@ -4514,7 +4514,7 @@
       <c r="H128" s="50"/>
       <c r="I128" s="20"/>
     </row>
-    <row r="129" spans="1:9" ht="15.75" customHeight="1">
+    <row r="129" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="72"/>
       <c r="B129" s="50"/>
       <c r="C129" s="7"/>
@@ -4525,2707 +4525,2707 @@
       <c r="H129" s="50"/>
       <c r="I129" s="20"/>
     </row>
-    <row r="130" spans="1:9" ht="15.75" customHeight="1">
+    <row r="130" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I130" s="13"/>
     </row>
-    <row r="131" spans="1:9" ht="15.75" customHeight="1">
+    <row r="131" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I131" s="13"/>
     </row>
-    <row r="132" spans="1:9" ht="15.75" customHeight="1">
+    <row r="132" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I132" s="13"/>
     </row>
-    <row r="133" spans="1:9" ht="15.75" customHeight="1">
+    <row r="133" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I133" s="13"/>
     </row>
-    <row r="134" spans="1:9" ht="15.75" customHeight="1">
+    <row r="134" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I134" s="13"/>
     </row>
-    <row r="135" spans="1:9" ht="15.75" customHeight="1">
+    <row r="135" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I135" s="13"/>
     </row>
-    <row r="136" spans="1:9" ht="15.75" customHeight="1">
+    <row r="136" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I136" s="13"/>
     </row>
-    <row r="137" spans="1:9" ht="15.75" customHeight="1">
+    <row r="137" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I137" s="13"/>
     </row>
-    <row r="138" spans="1:9" ht="15.75" customHeight="1">
+    <row r="138" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I138" s="13"/>
     </row>
-    <row r="139" spans="1:9" ht="15.75" customHeight="1">
+    <row r="139" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I139" s="13"/>
     </row>
-    <row r="140" spans="1:9" ht="15.75" customHeight="1">
+    <row r="140" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I140" s="13"/>
     </row>
-    <row r="141" spans="1:9" ht="15.75" customHeight="1">
+    <row r="141" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I141" s="13"/>
     </row>
-    <row r="142" spans="1:9" ht="15.75" customHeight="1">
+    <row r="142" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I142" s="13"/>
     </row>
-    <row r="143" spans="1:9" ht="15.75" customHeight="1">
+    <row r="143" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I143" s="13"/>
     </row>
-    <row r="144" spans="1:9" ht="15.75" customHeight="1">
+    <row r="144" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I144" s="13"/>
     </row>
-    <row r="145" spans="9:9" ht="15.75" customHeight="1">
+    <row r="145" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I145" s="13"/>
     </row>
-    <row r="146" spans="9:9" ht="15.75" customHeight="1">
+    <row r="146" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I146" s="13"/>
     </row>
-    <row r="147" spans="9:9" ht="15.75" customHeight="1">
+    <row r="147" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I147" s="13"/>
     </row>
-    <row r="148" spans="9:9" ht="15.75" customHeight="1">
+    <row r="148" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I148" s="13"/>
     </row>
-    <row r="149" spans="9:9" ht="15.75" customHeight="1">
+    <row r="149" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I149" s="13"/>
     </row>
-    <row r="150" spans="9:9" ht="15.75" customHeight="1">
+    <row r="150" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I150" s="13"/>
     </row>
-    <row r="151" spans="9:9" ht="15.75" customHeight="1">
+    <row r="151" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I151" s="13"/>
     </row>
-    <row r="152" spans="9:9" ht="15.75" customHeight="1">
+    <row r="152" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I152" s="13"/>
     </row>
-    <row r="153" spans="9:9" ht="15.75" customHeight="1">
+    <row r="153" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I153" s="13"/>
     </row>
-    <row r="154" spans="9:9" ht="15.75" customHeight="1">
+    <row r="154" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I154" s="13"/>
     </row>
-    <row r="155" spans="9:9" ht="15.75" customHeight="1">
+    <row r="155" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I155" s="13"/>
     </row>
-    <row r="156" spans="9:9" ht="15.75" customHeight="1">
+    <row r="156" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I156" s="13"/>
     </row>
-    <row r="157" spans="9:9" ht="15.75" customHeight="1">
+    <row r="157" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I157" s="13"/>
     </row>
-    <row r="158" spans="9:9" ht="15.75" customHeight="1">
+    <row r="158" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I158" s="13"/>
     </row>
-    <row r="159" spans="9:9" ht="15.75" customHeight="1">
+    <row r="159" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I159" s="13"/>
     </row>
-    <row r="160" spans="9:9" ht="15.75" customHeight="1">
+    <row r="160" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I160" s="13"/>
     </row>
-    <row r="161" spans="9:9" ht="15.75" customHeight="1">
+    <row r="161" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I161" s="13"/>
     </row>
-    <row r="162" spans="9:9" ht="15.75" customHeight="1">
+    <row r="162" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I162" s="13"/>
     </row>
-    <row r="163" spans="9:9" ht="15.75" customHeight="1">
+    <row r="163" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I163" s="13"/>
     </row>
-    <row r="164" spans="9:9" ht="15.75" customHeight="1">
+    <row r="164" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I164" s="13"/>
     </row>
-    <row r="165" spans="9:9" ht="15.75" customHeight="1">
+    <row r="165" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I165" s="13"/>
     </row>
-    <row r="166" spans="9:9" ht="15.75" customHeight="1">
+    <row r="166" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I166" s="13"/>
     </row>
-    <row r="167" spans="9:9" ht="15.75" customHeight="1">
+    <row r="167" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I167" s="13"/>
     </row>
-    <row r="168" spans="9:9" ht="15.75" customHeight="1">
+    <row r="168" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I168" s="13"/>
     </row>
-    <row r="169" spans="9:9" ht="15.75" customHeight="1">
+    <row r="169" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I169" s="13"/>
     </row>
-    <row r="170" spans="9:9" ht="15.75" customHeight="1">
+    <row r="170" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I170" s="13"/>
     </row>
-    <row r="171" spans="9:9" ht="15.75" customHeight="1">
+    <row r="171" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I171" s="13"/>
     </row>
-    <row r="172" spans="9:9" ht="15.75" customHeight="1">
+    <row r="172" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I172" s="13"/>
     </row>
-    <row r="173" spans="9:9" ht="15.75" customHeight="1">
+    <row r="173" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I173" s="13"/>
     </row>
-    <row r="174" spans="9:9" ht="15.75" customHeight="1">
+    <row r="174" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I174" s="13"/>
     </row>
-    <row r="175" spans="9:9" ht="15.75" customHeight="1">
+    <row r="175" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I175" s="13"/>
     </row>
-    <row r="176" spans="9:9" ht="15.75" customHeight="1">
+    <row r="176" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I176" s="13"/>
     </row>
-    <row r="177" spans="9:9" ht="15.75" customHeight="1">
+    <row r="177" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I177" s="13"/>
     </row>
-    <row r="178" spans="9:9" ht="15.75" customHeight="1">
+    <row r="178" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I178" s="13"/>
     </row>
-    <row r="179" spans="9:9" ht="15.75" customHeight="1">
+    <row r="179" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I179" s="13"/>
     </row>
-    <row r="180" spans="9:9" ht="15.75" customHeight="1">
+    <row r="180" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I180" s="13"/>
     </row>
-    <row r="181" spans="9:9" ht="15.75" customHeight="1">
+    <row r="181" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I181" s="13"/>
     </row>
-    <row r="182" spans="9:9" ht="15.75" customHeight="1">
+    <row r="182" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I182" s="13"/>
     </row>
-    <row r="183" spans="9:9" ht="15.75" customHeight="1">
+    <row r="183" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I183" s="13"/>
     </row>
-    <row r="184" spans="9:9" ht="15.75" customHeight="1">
+    <row r="184" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I184" s="13"/>
     </row>
-    <row r="185" spans="9:9" ht="15.75" customHeight="1">
+    <row r="185" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I185" s="13"/>
     </row>
-    <row r="186" spans="9:9" ht="15.75" customHeight="1">
+    <row r="186" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I186" s="13"/>
     </row>
-    <row r="187" spans="9:9" ht="15.75" customHeight="1">
+    <row r="187" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I187" s="13"/>
     </row>
-    <row r="188" spans="9:9" ht="15.75" customHeight="1">
+    <row r="188" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I188" s="13"/>
     </row>
-    <row r="189" spans="9:9" ht="15.75" customHeight="1">
+    <row r="189" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I189" s="13"/>
     </row>
-    <row r="190" spans="9:9" ht="15.75" customHeight="1">
+    <row r="190" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I190" s="13"/>
     </row>
-    <row r="191" spans="9:9" ht="15.75" customHeight="1">
+    <row r="191" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I191" s="13"/>
     </row>
-    <row r="192" spans="9:9" ht="15.75" customHeight="1">
+    <row r="192" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I192" s="13"/>
     </row>
-    <row r="193" spans="9:9" ht="15.75" customHeight="1">
+    <row r="193" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I193" s="13"/>
     </row>
-    <row r="194" spans="9:9" ht="15.75" customHeight="1">
+    <row r="194" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I194" s="13"/>
     </row>
-    <row r="195" spans="9:9" ht="15.75" customHeight="1">
+    <row r="195" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I195" s="13"/>
     </row>
-    <row r="196" spans="9:9" ht="15.75" customHeight="1">
+    <row r="196" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I196" s="13"/>
     </row>
-    <row r="197" spans="9:9" ht="15.75" customHeight="1">
+    <row r="197" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I197" s="13"/>
     </row>
-    <row r="198" spans="9:9" ht="15.75" customHeight="1">
+    <row r="198" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I198" s="13"/>
     </row>
-    <row r="199" spans="9:9" ht="15.75" customHeight="1">
+    <row r="199" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I199" s="13"/>
     </row>
-    <row r="200" spans="9:9" ht="15.75" customHeight="1">
+    <row r="200" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I200" s="13"/>
     </row>
-    <row r="201" spans="9:9" ht="15.75" customHeight="1">
+    <row r="201" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I201" s="13"/>
     </row>
-    <row r="202" spans="9:9" ht="15.75" customHeight="1">
+    <row r="202" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I202" s="13"/>
     </row>
-    <row r="203" spans="9:9" ht="15.75" customHeight="1">
+    <row r="203" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I203" s="13"/>
     </row>
-    <row r="204" spans="9:9" ht="15.75" customHeight="1">
+    <row r="204" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I204" s="13"/>
     </row>
-    <row r="205" spans="9:9" ht="15.75" customHeight="1">
+    <row r="205" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I205" s="13"/>
     </row>
-    <row r="206" spans="9:9" ht="15.75" customHeight="1">
+    <row r="206" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I206" s="13"/>
     </row>
-    <row r="207" spans="9:9" ht="15.75" customHeight="1">
+    <row r="207" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I207" s="13"/>
     </row>
-    <row r="208" spans="9:9" ht="15.75" customHeight="1">
+    <row r="208" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I208" s="13"/>
     </row>
-    <row r="209" spans="9:9" ht="15.75" customHeight="1">
+    <row r="209" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I209" s="13"/>
     </row>
-    <row r="210" spans="9:9" ht="15.75" customHeight="1">
+    <row r="210" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I210" s="13"/>
     </row>
-    <row r="211" spans="9:9" ht="15.75" customHeight="1">
+    <row r="211" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I211" s="13"/>
     </row>
-    <row r="212" spans="9:9" ht="15.75" customHeight="1">
+    <row r="212" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I212" s="13"/>
     </row>
-    <row r="213" spans="9:9" ht="15.75" customHeight="1">
+    <row r="213" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I213" s="13"/>
     </row>
-    <row r="214" spans="9:9" ht="15.75" customHeight="1">
+    <row r="214" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I214" s="13"/>
     </row>
-    <row r="215" spans="9:9" ht="15.75" customHeight="1">
+    <row r="215" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I215" s="13"/>
     </row>
-    <row r="216" spans="9:9" ht="15.75" customHeight="1">
+    <row r="216" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I216" s="13"/>
     </row>
-    <row r="217" spans="9:9" ht="15.75" customHeight="1">
+    <row r="217" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I217" s="13"/>
     </row>
-    <row r="218" spans="9:9" ht="15.75" customHeight="1">
+    <row r="218" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I218" s="13"/>
     </row>
-    <row r="219" spans="9:9" ht="15.75" customHeight="1">
+    <row r="219" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I219" s="13"/>
     </row>
-    <row r="220" spans="9:9" ht="15.75" customHeight="1">
+    <row r="220" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I220" s="13"/>
     </row>
-    <row r="221" spans="9:9" ht="15.75" customHeight="1">
+    <row r="221" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I221" s="13"/>
     </row>
-    <row r="222" spans="9:9" ht="15.75" customHeight="1">
+    <row r="222" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I222" s="13"/>
     </row>
-    <row r="223" spans="9:9" ht="15.75" customHeight="1">
+    <row r="223" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I223" s="13"/>
     </row>
-    <row r="224" spans="9:9" ht="15.75" customHeight="1">
+    <row r="224" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I224" s="13"/>
     </row>
-    <row r="225" spans="9:9" ht="15.75" customHeight="1">
+    <row r="225" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I225" s="13"/>
     </row>
-    <row r="226" spans="9:9" ht="15.75" customHeight="1">
+    <row r="226" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I226" s="13"/>
     </row>
-    <row r="227" spans="9:9" ht="15.75" customHeight="1">
+    <row r="227" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I227" s="13"/>
     </row>
-    <row r="228" spans="9:9" ht="15.75" customHeight="1">
+    <row r="228" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I228" s="13"/>
     </row>
-    <row r="229" spans="9:9" ht="15.75" customHeight="1">
+    <row r="229" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I229" s="13"/>
     </row>
-    <row r="230" spans="9:9" ht="15.75" customHeight="1">
+    <row r="230" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I230" s="13"/>
     </row>
-    <row r="231" spans="9:9" ht="15.75" customHeight="1">
+    <row r="231" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I231" s="13"/>
     </row>
-    <row r="232" spans="9:9" ht="15.75" customHeight="1">
+    <row r="232" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I232" s="13"/>
     </row>
-    <row r="233" spans="9:9" ht="15.75" customHeight="1">
+    <row r="233" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I233" s="13"/>
     </row>
-    <row r="234" spans="9:9" ht="15.75" customHeight="1">
+    <row r="234" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I234" s="13"/>
     </row>
-    <row r="235" spans="9:9" ht="15.75" customHeight="1">
+    <row r="235" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I235" s="13"/>
     </row>
-    <row r="236" spans="9:9" ht="15.75" customHeight="1">
+    <row r="236" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I236" s="13"/>
     </row>
-    <row r="237" spans="9:9" ht="15.75" customHeight="1">
+    <row r="237" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I237" s="13"/>
     </row>
-    <row r="238" spans="9:9" ht="15.75" customHeight="1">
+    <row r="238" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I238" s="13"/>
     </row>
-    <row r="239" spans="9:9" ht="15.75" customHeight="1">
+    <row r="239" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I239" s="13"/>
     </row>
-    <row r="240" spans="9:9" ht="15.75" customHeight="1">
+    <row r="240" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I240" s="13"/>
     </row>
-    <row r="241" spans="9:9" ht="15.75" customHeight="1">
+    <row r="241" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I241" s="13"/>
     </row>
-    <row r="242" spans="9:9" ht="15.75" customHeight="1">
+    <row r="242" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I242" s="13"/>
     </row>
-    <row r="243" spans="9:9" ht="15.75" customHeight="1">
+    <row r="243" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I243" s="13"/>
     </row>
-    <row r="244" spans="9:9" ht="15.75" customHeight="1">
+    <row r="244" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I244" s="13"/>
     </row>
-    <row r="245" spans="9:9" ht="15.75" customHeight="1">
+    <row r="245" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I245" s="13"/>
     </row>
-    <row r="246" spans="9:9" ht="15.75" customHeight="1">
+    <row r="246" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I246" s="13"/>
     </row>
-    <row r="247" spans="9:9" ht="15.75" customHeight="1">
+    <row r="247" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I247" s="13"/>
     </row>
-    <row r="248" spans="9:9" ht="15.75" customHeight="1">
+    <row r="248" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I248" s="13"/>
     </row>
-    <row r="249" spans="9:9" ht="15.75" customHeight="1">
+    <row r="249" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I249" s="13"/>
     </row>
-    <row r="250" spans="9:9" ht="15.75" customHeight="1">
+    <row r="250" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I250" s="13"/>
     </row>
-    <row r="251" spans="9:9" ht="15.75" customHeight="1">
+    <row r="251" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I251" s="13"/>
     </row>
-    <row r="252" spans="9:9" ht="15.75" customHeight="1">
+    <row r="252" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I252" s="13"/>
     </row>
-    <row r="253" spans="9:9" ht="15.75" customHeight="1">
+    <row r="253" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I253" s="13"/>
     </row>
-    <row r="254" spans="9:9" ht="15.75" customHeight="1">
+    <row r="254" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I254" s="13"/>
     </row>
-    <row r="255" spans="9:9" ht="15.75" customHeight="1">
+    <row r="255" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I255" s="13"/>
     </row>
-    <row r="256" spans="9:9" ht="15.75" customHeight="1">
+    <row r="256" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I256" s="13"/>
     </row>
-    <row r="257" spans="9:9" ht="15.75" customHeight="1">
+    <row r="257" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I257" s="13"/>
     </row>
-    <row r="258" spans="9:9" ht="15.75" customHeight="1">
+    <row r="258" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I258" s="13"/>
     </row>
-    <row r="259" spans="9:9" ht="15.75" customHeight="1">
+    <row r="259" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I259" s="13"/>
     </row>
-    <row r="260" spans="9:9" ht="15.75" customHeight="1">
+    <row r="260" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I260" s="13"/>
     </row>
-    <row r="261" spans="9:9" ht="15.75" customHeight="1">
+    <row r="261" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I261" s="13"/>
     </row>
-    <row r="262" spans="9:9" ht="15.75" customHeight="1">
+    <row r="262" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I262" s="13"/>
     </row>
-    <row r="263" spans="9:9" ht="15.75" customHeight="1">
+    <row r="263" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I263" s="13"/>
     </row>
-    <row r="264" spans="9:9" ht="15.75" customHeight="1">
+    <row r="264" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I264" s="13"/>
     </row>
-    <row r="265" spans="9:9" ht="15.75" customHeight="1">
+    <row r="265" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I265" s="13"/>
     </row>
-    <row r="266" spans="9:9" ht="15.75" customHeight="1">
+    <row r="266" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I266" s="13"/>
     </row>
-    <row r="267" spans="9:9" ht="15.75" customHeight="1">
+    <row r="267" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I267" s="13"/>
     </row>
-    <row r="268" spans="9:9" ht="15.75" customHeight="1">
+    <row r="268" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I268" s="13"/>
     </row>
-    <row r="269" spans="9:9" ht="15.75" customHeight="1">
+    <row r="269" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I269" s="13"/>
     </row>
-    <row r="270" spans="9:9" ht="15.75" customHeight="1">
+    <row r="270" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I270" s="13"/>
     </row>
-    <row r="271" spans="9:9" ht="15.75" customHeight="1">
+    <row r="271" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I271" s="13"/>
     </row>
-    <row r="272" spans="9:9" ht="15.75" customHeight="1">
+    <row r="272" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I272" s="13"/>
     </row>
-    <row r="273" spans="9:9" ht="15.75" customHeight="1">
+    <row r="273" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I273" s="13"/>
     </row>
-    <row r="274" spans="9:9" ht="15.75" customHeight="1">
+    <row r="274" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I274" s="13"/>
     </row>
-    <row r="275" spans="9:9" ht="15.75" customHeight="1">
+    <row r="275" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I275" s="13"/>
     </row>
-    <row r="276" spans="9:9" ht="15.75" customHeight="1">
+    <row r="276" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I276" s="13"/>
     </row>
-    <row r="277" spans="9:9" ht="15.75" customHeight="1">
+    <row r="277" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I277" s="13"/>
     </row>
-    <row r="278" spans="9:9" ht="15.75" customHeight="1">
+    <row r="278" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I278" s="13"/>
     </row>
-    <row r="279" spans="9:9" ht="15.75" customHeight="1">
+    <row r="279" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I279" s="13"/>
     </row>
-    <row r="280" spans="9:9" ht="15.75" customHeight="1">
+    <row r="280" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I280" s="13"/>
     </row>
-    <row r="281" spans="9:9" ht="15.75" customHeight="1">
+    <row r="281" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I281" s="13"/>
     </row>
-    <row r="282" spans="9:9" ht="15.75" customHeight="1">
+    <row r="282" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I282" s="13"/>
     </row>
-    <row r="283" spans="9:9" ht="15.75" customHeight="1">
+    <row r="283" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I283" s="13"/>
     </row>
-    <row r="284" spans="9:9" ht="15.75" customHeight="1">
+    <row r="284" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I284" s="13"/>
     </row>
-    <row r="285" spans="9:9" ht="15.75" customHeight="1">
+    <row r="285" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I285" s="13"/>
     </row>
-    <row r="286" spans="9:9" ht="15.75" customHeight="1">
+    <row r="286" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I286" s="13"/>
     </row>
-    <row r="287" spans="9:9" ht="15.75" customHeight="1">
+    <row r="287" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I287" s="13"/>
     </row>
-    <row r="288" spans="9:9" ht="15.75" customHeight="1">
+    <row r="288" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I288" s="13"/>
     </row>
-    <row r="289" spans="9:9" ht="15.75" customHeight="1">
+    <row r="289" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I289" s="13"/>
     </row>
-    <row r="290" spans="9:9" ht="15.75" customHeight="1">
+    <row r="290" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I290" s="13"/>
     </row>
-    <row r="291" spans="9:9" ht="15.75" customHeight="1">
+    <row r="291" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I291" s="13"/>
     </row>
-    <row r="292" spans="9:9" ht="15.75" customHeight="1">
+    <row r="292" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I292" s="13"/>
     </row>
-    <row r="293" spans="9:9" ht="15.75" customHeight="1">
+    <row r="293" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I293" s="13"/>
     </row>
-    <row r="294" spans="9:9" ht="15.75" customHeight="1">
+    <row r="294" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I294" s="13"/>
     </row>
-    <row r="295" spans="9:9" ht="15.75" customHeight="1">
+    <row r="295" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I295" s="13"/>
     </row>
-    <row r="296" spans="9:9" ht="15.75" customHeight="1">
+    <row r="296" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I296" s="13"/>
     </row>
-    <row r="297" spans="9:9" ht="15.75" customHeight="1">
+    <row r="297" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I297" s="13"/>
     </row>
-    <row r="298" spans="9:9" ht="15.75" customHeight="1">
+    <row r="298" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I298" s="13"/>
     </row>
-    <row r="299" spans="9:9" ht="15.75" customHeight="1">
+    <row r="299" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I299" s="13"/>
     </row>
-    <row r="300" spans="9:9" ht="15.75" customHeight="1">
+    <row r="300" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I300" s="13"/>
     </row>
-    <row r="301" spans="9:9" ht="15.75" customHeight="1">
+    <row r="301" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I301" s="13"/>
     </row>
-    <row r="302" spans="9:9" ht="15.75" customHeight="1">
+    <row r="302" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I302" s="13"/>
     </row>
-    <row r="303" spans="9:9" ht="15.75" customHeight="1">
+    <row r="303" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I303" s="13"/>
     </row>
-    <row r="304" spans="9:9" ht="15.75" customHeight="1">
+    <row r="304" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I304" s="13"/>
     </row>
-    <row r="305" spans="9:9" ht="15.75" customHeight="1">
+    <row r="305" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I305" s="13"/>
     </row>
-    <row r="306" spans="9:9" ht="15.75" customHeight="1">
+    <row r="306" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I306" s="13"/>
     </row>
-    <row r="307" spans="9:9" ht="15.75" customHeight="1">
+    <row r="307" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I307" s="13"/>
     </row>
-    <row r="308" spans="9:9" ht="15.75" customHeight="1">
+    <row r="308" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I308" s="13"/>
     </row>
-    <row r="309" spans="9:9" ht="15.75" customHeight="1">
+    <row r="309" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I309" s="13"/>
     </row>
-    <row r="310" spans="9:9" ht="15.75" customHeight="1">
+    <row r="310" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I310" s="13"/>
     </row>
-    <row r="311" spans="9:9" ht="15.75" customHeight="1">
+    <row r="311" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I311" s="13"/>
     </row>
-    <row r="312" spans="9:9" ht="15.75" customHeight="1">
+    <row r="312" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I312" s="13"/>
     </row>
-    <row r="313" spans="9:9" ht="15.75" customHeight="1">
+    <row r="313" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I313" s="13"/>
     </row>
-    <row r="314" spans="9:9" ht="15.75" customHeight="1">
+    <row r="314" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I314" s="13"/>
     </row>
-    <row r="315" spans="9:9" ht="15.75" customHeight="1">
+    <row r="315" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I315" s="13"/>
     </row>
-    <row r="316" spans="9:9" ht="15.75" customHeight="1">
+    <row r="316" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I316" s="13"/>
     </row>
-    <row r="317" spans="9:9" ht="15.75" customHeight="1">
+    <row r="317" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I317" s="13"/>
     </row>
-    <row r="318" spans="9:9" ht="15.75" customHeight="1">
+    <row r="318" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I318" s="13"/>
     </row>
-    <row r="319" spans="9:9" ht="15.75" customHeight="1">
+    <row r="319" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I319" s="13"/>
     </row>
-    <row r="320" spans="9:9" ht="15.75" customHeight="1">
+    <row r="320" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I320" s="13"/>
     </row>
-    <row r="321" spans="9:9" ht="15.75" customHeight="1">
+    <row r="321" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I321" s="13"/>
     </row>
-    <row r="322" spans="9:9" ht="15.75" customHeight="1">
+    <row r="322" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I322" s="13"/>
     </row>
-    <row r="323" spans="9:9" ht="15.75" customHeight="1">
+    <row r="323" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I323" s="13"/>
     </row>
-    <row r="324" spans="9:9" ht="15.75" customHeight="1">
+    <row r="324" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I324" s="13"/>
     </row>
-    <row r="325" spans="9:9" ht="15.75" customHeight="1">
+    <row r="325" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I325" s="13"/>
     </row>
-    <row r="326" spans="9:9" ht="15.75" customHeight="1">
+    <row r="326" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I326" s="13"/>
     </row>
-    <row r="327" spans="9:9" ht="15.75" customHeight="1">
+    <row r="327" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I327" s="13"/>
     </row>
-    <row r="328" spans="9:9" ht="15.75" customHeight="1">
+    <row r="328" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I328" s="13"/>
     </row>
-    <row r="329" spans="9:9" ht="15.75" customHeight="1">
+    <row r="329" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I329" s="13"/>
     </row>
-    <row r="330" spans="9:9" ht="15.75" customHeight="1">
+    <row r="330" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I330" s="13"/>
     </row>
-    <row r="331" spans="9:9" ht="15.75" customHeight="1">
+    <row r="331" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I331" s="13"/>
     </row>
-    <row r="332" spans="9:9" ht="15.75" customHeight="1">
+    <row r="332" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I332" s="13"/>
     </row>
-    <row r="333" spans="9:9" ht="15.75" customHeight="1">
+    <row r="333" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I333" s="13"/>
     </row>
-    <row r="334" spans="9:9" ht="15.75" customHeight="1">
+    <row r="334" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I334" s="13"/>
     </row>
-    <row r="335" spans="9:9" ht="15.75" customHeight="1">
+    <row r="335" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I335" s="13"/>
     </row>
-    <row r="336" spans="9:9" ht="15.75" customHeight="1">
+    <row r="336" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I336" s="13"/>
     </row>
-    <row r="337" spans="9:9" ht="15.75" customHeight="1">
+    <row r="337" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I337" s="13"/>
     </row>
-    <row r="338" spans="9:9" ht="15.75" customHeight="1">
+    <row r="338" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I338" s="13"/>
     </row>
-    <row r="339" spans="9:9" ht="15.75" customHeight="1">
+    <row r="339" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I339" s="13"/>
     </row>
-    <row r="340" spans="9:9" ht="15.75" customHeight="1">
+    <row r="340" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I340" s="13"/>
     </row>
-    <row r="341" spans="9:9" ht="15.75" customHeight="1">
+    <row r="341" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I341" s="13"/>
     </row>
-    <row r="342" spans="9:9" ht="15.75" customHeight="1">
+    <row r="342" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I342" s="13"/>
     </row>
-    <row r="343" spans="9:9" ht="15.75" customHeight="1">
+    <row r="343" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I343" s="13"/>
     </row>
-    <row r="344" spans="9:9" ht="15.75" customHeight="1">
+    <row r="344" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I344" s="13"/>
     </row>
-    <row r="345" spans="9:9" ht="15.75" customHeight="1">
+    <row r="345" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I345" s="13"/>
     </row>
-    <row r="346" spans="9:9" ht="15.75" customHeight="1">
+    <row r="346" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I346" s="13"/>
     </row>
-    <row r="347" spans="9:9" ht="15.75" customHeight="1">
+    <row r="347" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I347" s="13"/>
     </row>
-    <row r="348" spans="9:9" ht="15.75" customHeight="1">
+    <row r="348" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I348" s="13"/>
     </row>
-    <row r="349" spans="9:9" ht="15.75" customHeight="1">
+    <row r="349" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I349" s="13"/>
     </row>
-    <row r="350" spans="9:9" ht="15.75" customHeight="1">
+    <row r="350" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I350" s="13"/>
     </row>
-    <row r="351" spans="9:9" ht="15.75" customHeight="1">
+    <row r="351" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I351" s="13"/>
     </row>
-    <row r="352" spans="9:9" ht="15.75" customHeight="1">
+    <row r="352" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I352" s="13"/>
     </row>
-    <row r="353" spans="9:9" ht="15.75" customHeight="1">
+    <row r="353" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I353" s="13"/>
     </row>
-    <row r="354" spans="9:9" ht="15.75" customHeight="1">
+    <row r="354" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I354" s="13"/>
     </row>
-    <row r="355" spans="9:9" ht="15.75" customHeight="1">
+    <row r="355" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I355" s="13"/>
     </row>
-    <row r="356" spans="9:9" ht="15.75" customHeight="1">
+    <row r="356" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I356" s="13"/>
     </row>
-    <row r="357" spans="9:9" ht="15.75" customHeight="1">
+    <row r="357" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I357" s="13"/>
     </row>
-    <row r="358" spans="9:9" ht="15.75" customHeight="1">
+    <row r="358" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I358" s="13"/>
     </row>
-    <row r="359" spans="9:9" ht="15.75" customHeight="1">
+    <row r="359" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I359" s="13"/>
     </row>
-    <row r="360" spans="9:9" ht="15.75" customHeight="1">
+    <row r="360" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I360" s="13"/>
     </row>
-    <row r="361" spans="9:9" ht="15.75" customHeight="1">
+    <row r="361" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I361" s="13"/>
     </row>
-    <row r="362" spans="9:9" ht="15.75" customHeight="1">
+    <row r="362" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I362" s="13"/>
     </row>
-    <row r="363" spans="9:9" ht="15.75" customHeight="1">
+    <row r="363" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I363" s="13"/>
     </row>
-    <row r="364" spans="9:9" ht="15.75" customHeight="1">
+    <row r="364" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I364" s="13"/>
     </row>
-    <row r="365" spans="9:9" ht="15.75" customHeight="1">
+    <row r="365" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I365" s="13"/>
     </row>
-    <row r="366" spans="9:9" ht="15.75" customHeight="1">
+    <row r="366" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I366" s="13"/>
     </row>
-    <row r="367" spans="9:9" ht="15.75" customHeight="1">
+    <row r="367" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I367" s="13"/>
     </row>
-    <row r="368" spans="9:9" ht="15.75" customHeight="1">
+    <row r="368" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I368" s="13"/>
     </row>
-    <row r="369" spans="9:9" ht="15.75" customHeight="1">
+    <row r="369" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I369" s="13"/>
     </row>
-    <row r="370" spans="9:9" ht="15.75" customHeight="1">
+    <row r="370" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I370" s="13"/>
     </row>
-    <row r="371" spans="9:9" ht="15.75" customHeight="1">
+    <row r="371" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I371" s="13"/>
     </row>
-    <row r="372" spans="9:9" ht="15.75" customHeight="1">
+    <row r="372" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I372" s="13"/>
     </row>
-    <row r="373" spans="9:9" ht="15.75" customHeight="1">
+    <row r="373" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I373" s="13"/>
     </row>
-    <row r="374" spans="9:9" ht="15.75" customHeight="1">
+    <row r="374" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I374" s="13"/>
     </row>
-    <row r="375" spans="9:9" ht="15.75" customHeight="1">
+    <row r="375" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I375" s="13"/>
     </row>
-    <row r="376" spans="9:9" ht="15.75" customHeight="1">
+    <row r="376" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I376" s="13"/>
     </row>
-    <row r="377" spans="9:9" ht="15.75" customHeight="1">
+    <row r="377" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I377" s="13"/>
     </row>
-    <row r="378" spans="9:9" ht="15.75" customHeight="1">
+    <row r="378" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I378" s="13"/>
     </row>
-    <row r="379" spans="9:9" ht="15.75" customHeight="1">
+    <row r="379" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I379" s="13"/>
     </row>
-    <row r="380" spans="9:9" ht="15.75" customHeight="1">
+    <row r="380" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I380" s="13"/>
     </row>
-    <row r="381" spans="9:9" ht="15.75" customHeight="1">
+    <row r="381" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I381" s="13"/>
     </row>
-    <row r="382" spans="9:9" ht="15.75" customHeight="1">
+    <row r="382" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I382" s="13"/>
     </row>
-    <row r="383" spans="9:9" ht="15.75" customHeight="1">
+    <row r="383" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I383" s="13"/>
     </row>
-    <row r="384" spans="9:9" ht="15.75" customHeight="1">
+    <row r="384" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I384" s="13"/>
     </row>
-    <row r="385" spans="9:9" ht="15.75" customHeight="1">
+    <row r="385" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I385" s="13"/>
     </row>
-    <row r="386" spans="9:9" ht="15.75" customHeight="1">
+    <row r="386" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I386" s="13"/>
     </row>
-    <row r="387" spans="9:9" ht="15.75" customHeight="1">
+    <row r="387" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I387" s="13"/>
     </row>
-    <row r="388" spans="9:9" ht="15.75" customHeight="1">
+    <row r="388" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I388" s="13"/>
     </row>
-    <row r="389" spans="9:9" ht="15.75" customHeight="1">
+    <row r="389" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I389" s="13"/>
     </row>
-    <row r="390" spans="9:9" ht="15.75" customHeight="1">
+    <row r="390" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I390" s="13"/>
     </row>
-    <row r="391" spans="9:9" ht="15.75" customHeight="1">
+    <row r="391" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I391" s="13"/>
     </row>
-    <row r="392" spans="9:9" ht="15.75" customHeight="1">
+    <row r="392" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I392" s="13"/>
     </row>
-    <row r="393" spans="9:9" ht="15.75" customHeight="1">
+    <row r="393" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I393" s="13"/>
     </row>
-    <row r="394" spans="9:9" ht="15.75" customHeight="1">
+    <row r="394" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I394" s="13"/>
     </row>
-    <row r="395" spans="9:9" ht="15.75" customHeight="1">
+    <row r="395" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I395" s="13"/>
     </row>
-    <row r="396" spans="9:9" ht="15.75" customHeight="1">
+    <row r="396" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I396" s="13"/>
     </row>
-    <row r="397" spans="9:9" ht="15.75" customHeight="1">
+    <row r="397" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I397" s="13"/>
     </row>
-    <row r="398" spans="9:9" ht="15.75" customHeight="1">
+    <row r="398" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I398" s="13"/>
     </row>
-    <row r="399" spans="9:9" ht="15.75" customHeight="1">
+    <row r="399" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I399" s="13"/>
     </row>
-    <row r="400" spans="9:9" ht="15.75" customHeight="1">
+    <row r="400" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I400" s="13"/>
     </row>
-    <row r="401" spans="9:9" ht="15.75" customHeight="1">
+    <row r="401" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I401" s="13"/>
     </row>
-    <row r="402" spans="9:9" ht="15.75" customHeight="1">
+    <row r="402" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I402" s="13"/>
     </row>
-    <row r="403" spans="9:9" ht="15.75" customHeight="1">
+    <row r="403" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I403" s="13"/>
     </row>
-    <row r="404" spans="9:9" ht="15.75" customHeight="1">
+    <row r="404" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I404" s="13"/>
     </row>
-    <row r="405" spans="9:9" ht="15.75" customHeight="1">
+    <row r="405" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I405" s="13"/>
     </row>
-    <row r="406" spans="9:9" ht="15.75" customHeight="1">
+    <row r="406" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I406" s="13"/>
     </row>
-    <row r="407" spans="9:9" ht="15.75" customHeight="1">
+    <row r="407" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I407" s="13"/>
     </row>
-    <row r="408" spans="9:9" ht="15.75" customHeight="1">
+    <row r="408" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I408" s="13"/>
     </row>
-    <row r="409" spans="9:9" ht="15.75" customHeight="1">
+    <row r="409" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I409" s="13"/>
     </row>
-    <row r="410" spans="9:9" ht="15.75" customHeight="1">
+    <row r="410" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I410" s="13"/>
     </row>
-    <row r="411" spans="9:9" ht="15.75" customHeight="1">
+    <row r="411" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I411" s="13"/>
     </row>
-    <row r="412" spans="9:9" ht="15.75" customHeight="1">
+    <row r="412" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I412" s="13"/>
     </row>
-    <row r="413" spans="9:9" ht="15.75" customHeight="1">
+    <row r="413" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I413" s="13"/>
     </row>
-    <row r="414" spans="9:9" ht="15.75" customHeight="1">
+    <row r="414" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I414" s="13"/>
     </row>
-    <row r="415" spans="9:9" ht="15.75" customHeight="1">
+    <row r="415" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I415" s="13"/>
     </row>
-    <row r="416" spans="9:9" ht="15.75" customHeight="1">
+    <row r="416" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I416" s="13"/>
     </row>
-    <row r="417" spans="9:9" ht="15.75" customHeight="1">
+    <row r="417" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I417" s="13"/>
     </row>
-    <row r="418" spans="9:9" ht="15.75" customHeight="1">
+    <row r="418" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I418" s="13"/>
     </row>
-    <row r="419" spans="9:9" ht="15.75" customHeight="1">
+    <row r="419" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I419" s="13"/>
     </row>
-    <row r="420" spans="9:9" ht="15.75" customHeight="1">
+    <row r="420" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I420" s="13"/>
     </row>
-    <row r="421" spans="9:9" ht="15.75" customHeight="1">
+    <row r="421" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I421" s="13"/>
     </row>
-    <row r="422" spans="9:9" ht="15.75" customHeight="1">
+    <row r="422" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I422" s="13"/>
     </row>
-    <row r="423" spans="9:9" ht="15.75" customHeight="1">
+    <row r="423" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I423" s="13"/>
     </row>
-    <row r="424" spans="9:9" ht="15.75" customHeight="1">
+    <row r="424" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I424" s="13"/>
     </row>
-    <row r="425" spans="9:9" ht="15.75" customHeight="1">
+    <row r="425" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I425" s="13"/>
     </row>
-    <row r="426" spans="9:9" ht="15.75" customHeight="1">
+    <row r="426" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I426" s="13"/>
     </row>
-    <row r="427" spans="9:9" ht="15.75" customHeight="1">
+    <row r="427" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I427" s="13"/>
     </row>
-    <row r="428" spans="9:9" ht="15.75" customHeight="1">
+    <row r="428" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I428" s="13"/>
     </row>
-    <row r="429" spans="9:9" ht="15.75" customHeight="1">
+    <row r="429" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I429" s="13"/>
     </row>
-    <row r="430" spans="9:9" ht="15.75" customHeight="1">
+    <row r="430" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I430" s="13"/>
     </row>
-    <row r="431" spans="9:9" ht="15.75" customHeight="1">
+    <row r="431" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I431" s="13"/>
     </row>
-    <row r="432" spans="9:9" ht="15.75" customHeight="1">
+    <row r="432" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I432" s="13"/>
     </row>
-    <row r="433" spans="9:9" ht="15.75" customHeight="1">
+    <row r="433" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I433" s="13"/>
     </row>
-    <row r="434" spans="9:9" ht="15.75" customHeight="1">
+    <row r="434" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I434" s="13"/>
     </row>
-    <row r="435" spans="9:9" ht="15.75" customHeight="1">
+    <row r="435" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I435" s="13"/>
     </row>
-    <row r="436" spans="9:9" ht="15.75" customHeight="1">
+    <row r="436" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I436" s="13"/>
     </row>
-    <row r="437" spans="9:9" ht="15.75" customHeight="1">
+    <row r="437" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I437" s="13"/>
     </row>
-    <row r="438" spans="9:9" ht="15.75" customHeight="1">
+    <row r="438" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I438" s="13"/>
     </row>
-    <row r="439" spans="9:9" ht="15.75" customHeight="1">
+    <row r="439" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I439" s="13"/>
     </row>
-    <row r="440" spans="9:9" ht="15.75" customHeight="1">
+    <row r="440" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I440" s="13"/>
     </row>
-    <row r="441" spans="9:9" ht="15.75" customHeight="1">
+    <row r="441" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I441" s="13"/>
     </row>
-    <row r="442" spans="9:9" ht="15.75" customHeight="1">
+    <row r="442" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I442" s="13"/>
     </row>
-    <row r="443" spans="9:9" ht="15.75" customHeight="1">
+    <row r="443" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I443" s="13"/>
     </row>
-    <row r="444" spans="9:9" ht="15.75" customHeight="1">
+    <row r="444" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I444" s="13"/>
     </row>
-    <row r="445" spans="9:9" ht="15.75" customHeight="1">
+    <row r="445" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I445" s="13"/>
     </row>
-    <row r="446" spans="9:9" ht="15.75" customHeight="1">
+    <row r="446" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I446" s="13"/>
     </row>
-    <row r="447" spans="9:9" ht="15.75" customHeight="1">
+    <row r="447" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I447" s="13"/>
     </row>
-    <row r="448" spans="9:9" ht="15.75" customHeight="1">
+    <row r="448" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I448" s="13"/>
     </row>
-    <row r="449" spans="9:9" ht="15.75" customHeight="1">
+    <row r="449" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I449" s="13"/>
     </row>
-    <row r="450" spans="9:9" ht="15.75" customHeight="1">
+    <row r="450" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I450" s="13"/>
     </row>
-    <row r="451" spans="9:9" ht="15.75" customHeight="1">
+    <row r="451" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I451" s="13"/>
     </row>
-    <row r="452" spans="9:9" ht="15.75" customHeight="1">
+    <row r="452" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I452" s="13"/>
     </row>
-    <row r="453" spans="9:9" ht="15.75" customHeight="1">
+    <row r="453" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I453" s="13"/>
     </row>
-    <row r="454" spans="9:9" ht="15.75" customHeight="1">
+    <row r="454" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I454" s="13"/>
     </row>
-    <row r="455" spans="9:9" ht="15.75" customHeight="1">
+    <row r="455" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I455" s="13"/>
     </row>
-    <row r="456" spans="9:9" ht="15.75" customHeight="1">
+    <row r="456" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I456" s="13"/>
     </row>
-    <row r="457" spans="9:9" ht="15.75" customHeight="1">
+    <row r="457" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I457" s="13"/>
     </row>
-    <row r="458" spans="9:9" ht="15.75" customHeight="1">
+    <row r="458" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I458" s="13"/>
     </row>
-    <row r="459" spans="9:9" ht="15.75" customHeight="1">
+    <row r="459" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I459" s="13"/>
     </row>
-    <row r="460" spans="9:9" ht="15.75" customHeight="1">
+    <row r="460" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I460" s="13"/>
     </row>
-    <row r="461" spans="9:9" ht="15.75" customHeight="1">
+    <row r="461" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I461" s="13"/>
     </row>
-    <row r="462" spans="9:9" ht="15.75" customHeight="1">
+    <row r="462" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I462" s="13"/>
     </row>
-    <row r="463" spans="9:9" ht="15.75" customHeight="1">
+    <row r="463" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I463" s="13"/>
     </row>
-    <row r="464" spans="9:9" ht="15.75" customHeight="1">
+    <row r="464" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I464" s="13"/>
     </row>
-    <row r="465" spans="9:9" ht="15.75" customHeight="1">
+    <row r="465" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I465" s="13"/>
     </row>
-    <row r="466" spans="9:9" ht="15.75" customHeight="1">
+    <row r="466" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I466" s="13"/>
     </row>
-    <row r="467" spans="9:9" ht="15.75" customHeight="1">
+    <row r="467" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I467" s="13"/>
     </row>
-    <row r="468" spans="9:9" ht="15.75" customHeight="1">
+    <row r="468" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I468" s="13"/>
     </row>
-    <row r="469" spans="9:9" ht="15.75" customHeight="1">
+    <row r="469" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I469" s="13"/>
     </row>
-    <row r="470" spans="9:9" ht="15.75" customHeight="1">
+    <row r="470" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I470" s="13"/>
     </row>
-    <row r="471" spans="9:9" ht="15.75" customHeight="1">
+    <row r="471" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I471" s="13"/>
     </row>
-    <row r="472" spans="9:9" ht="15.75" customHeight="1">
+    <row r="472" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I472" s="13"/>
     </row>
-    <row r="473" spans="9:9" ht="15.75" customHeight="1">
+    <row r="473" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I473" s="13"/>
     </row>
-    <row r="474" spans="9:9" ht="15.75" customHeight="1">
+    <row r="474" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I474" s="13"/>
     </row>
-    <row r="475" spans="9:9" ht="15.75" customHeight="1">
+    <row r="475" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I475" s="13"/>
     </row>
-    <row r="476" spans="9:9" ht="15.75" customHeight="1">
+    <row r="476" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I476" s="13"/>
     </row>
-    <row r="477" spans="9:9" ht="15.75" customHeight="1">
+    <row r="477" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I477" s="13"/>
     </row>
-    <row r="478" spans="9:9" ht="15.75" customHeight="1">
+    <row r="478" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I478" s="13"/>
     </row>
-    <row r="479" spans="9:9" ht="15.75" customHeight="1">
+    <row r="479" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I479" s="13"/>
     </row>
-    <row r="480" spans="9:9" ht="15.75" customHeight="1">
+    <row r="480" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I480" s="13"/>
     </row>
-    <row r="481" spans="9:9" ht="15.75" customHeight="1">
+    <row r="481" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I481" s="13"/>
     </row>
-    <row r="482" spans="9:9" ht="15.75" customHeight="1">
+    <row r="482" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I482" s="13"/>
     </row>
-    <row r="483" spans="9:9" ht="15.75" customHeight="1">
+    <row r="483" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I483" s="13"/>
     </row>
-    <row r="484" spans="9:9" ht="15.75" customHeight="1">
+    <row r="484" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I484" s="13"/>
     </row>
-    <row r="485" spans="9:9" ht="15.75" customHeight="1">
+    <row r="485" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I485" s="13"/>
     </row>
-    <row r="486" spans="9:9" ht="15.75" customHeight="1">
+    <row r="486" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I486" s="13"/>
     </row>
-    <row r="487" spans="9:9" ht="15.75" customHeight="1">
+    <row r="487" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I487" s="13"/>
     </row>
-    <row r="488" spans="9:9" ht="15.75" customHeight="1">
+    <row r="488" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I488" s="13"/>
     </row>
-    <row r="489" spans="9:9" ht="15.75" customHeight="1">
+    <row r="489" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I489" s="13"/>
     </row>
-    <row r="490" spans="9:9" ht="15.75" customHeight="1">
+    <row r="490" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I490" s="13"/>
     </row>
-    <row r="491" spans="9:9" ht="15.75" customHeight="1">
+    <row r="491" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I491" s="13"/>
     </row>
-    <row r="492" spans="9:9" ht="15.75" customHeight="1">
+    <row r="492" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I492" s="13"/>
     </row>
-    <row r="493" spans="9:9" ht="15.75" customHeight="1">
+    <row r="493" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I493" s="13"/>
     </row>
-    <row r="494" spans="9:9" ht="15.75" customHeight="1">
+    <row r="494" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I494" s="13"/>
     </row>
-    <row r="495" spans="9:9" ht="15.75" customHeight="1">
+    <row r="495" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I495" s="13"/>
     </row>
-    <row r="496" spans="9:9" ht="15.75" customHeight="1">
+    <row r="496" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I496" s="13"/>
     </row>
-    <row r="497" spans="9:9" ht="15.75" customHeight="1">
+    <row r="497" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I497" s="13"/>
     </row>
-    <row r="498" spans="9:9" ht="15.75" customHeight="1">
+    <row r="498" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I498" s="13"/>
     </row>
-    <row r="499" spans="9:9" ht="15.75" customHeight="1">
+    <row r="499" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I499" s="13"/>
     </row>
-    <row r="500" spans="9:9" ht="15.75" customHeight="1">
+    <row r="500" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I500" s="13"/>
     </row>
-    <row r="501" spans="9:9" ht="15.75" customHeight="1">
+    <row r="501" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I501" s="13"/>
     </row>
-    <row r="502" spans="9:9" ht="15.75" customHeight="1">
+    <row r="502" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I502" s="13"/>
     </row>
-    <row r="503" spans="9:9" ht="15.75" customHeight="1">
+    <row r="503" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I503" s="13"/>
     </row>
-    <row r="504" spans="9:9" ht="15.75" customHeight="1">
+    <row r="504" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I504" s="13"/>
     </row>
-    <row r="505" spans="9:9" ht="15.75" customHeight="1">
+    <row r="505" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I505" s="13"/>
     </row>
-    <row r="506" spans="9:9" ht="15.75" customHeight="1">
+    <row r="506" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I506" s="13"/>
     </row>
-    <row r="507" spans="9:9" ht="15.75" customHeight="1">
+    <row r="507" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I507" s="13"/>
     </row>
-    <row r="508" spans="9:9" ht="15.75" customHeight="1">
+    <row r="508" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I508" s="13"/>
     </row>
-    <row r="509" spans="9:9" ht="15.75" customHeight="1">
+    <row r="509" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I509" s="13"/>
     </row>
-    <row r="510" spans="9:9" ht="15.75" customHeight="1">
+    <row r="510" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I510" s="13"/>
     </row>
-    <row r="511" spans="9:9" ht="15.75" customHeight="1">
+    <row r="511" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I511" s="13"/>
     </row>
-    <row r="512" spans="9:9" ht="15.75" customHeight="1">
+    <row r="512" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I512" s="13"/>
     </row>
-    <row r="513" spans="9:9" ht="15.75" customHeight="1">
+    <row r="513" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I513" s="13"/>
     </row>
-    <row r="514" spans="9:9" ht="15.75" customHeight="1">
+    <row r="514" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I514" s="13"/>
     </row>
-    <row r="515" spans="9:9" ht="15.75" customHeight="1">
+    <row r="515" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I515" s="13"/>
     </row>
-    <row r="516" spans="9:9" ht="15.75" customHeight="1">
+    <row r="516" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I516" s="13"/>
     </row>
-    <row r="517" spans="9:9" ht="15.75" customHeight="1">
+    <row r="517" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I517" s="13"/>
     </row>
-    <row r="518" spans="9:9" ht="15.75" customHeight="1">
+    <row r="518" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I518" s="13"/>
     </row>
-    <row r="519" spans="9:9" ht="15.75" customHeight="1">
+    <row r="519" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I519" s="13"/>
     </row>
-    <row r="520" spans="9:9" ht="15.75" customHeight="1">
+    <row r="520" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I520" s="13"/>
     </row>
-    <row r="521" spans="9:9" ht="15.75" customHeight="1">
+    <row r="521" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I521" s="13"/>
     </row>
-    <row r="522" spans="9:9" ht="15.75" customHeight="1">
+    <row r="522" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I522" s="13"/>
     </row>
-    <row r="523" spans="9:9" ht="15.75" customHeight="1">
+    <row r="523" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I523" s="13"/>
     </row>
-    <row r="524" spans="9:9" ht="15.75" customHeight="1">
+    <row r="524" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I524" s="13"/>
     </row>
-    <row r="525" spans="9:9" ht="15.75" customHeight="1">
+    <row r="525" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I525" s="13"/>
     </row>
-    <row r="526" spans="9:9" ht="15.75" customHeight="1">
+    <row r="526" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I526" s="13"/>
     </row>
-    <row r="527" spans="9:9" ht="15.75" customHeight="1">
+    <row r="527" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I527" s="13"/>
     </row>
-    <row r="528" spans="9:9" ht="15.75" customHeight="1">
+    <row r="528" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I528" s="13"/>
     </row>
-    <row r="529" spans="9:9" ht="15.75" customHeight="1">
+    <row r="529" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I529" s="13"/>
     </row>
-    <row r="530" spans="9:9" ht="15.75" customHeight="1">
+    <row r="530" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I530" s="13"/>
     </row>
-    <row r="531" spans="9:9" ht="15.75" customHeight="1">
+    <row r="531" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I531" s="13"/>
     </row>
-    <row r="532" spans="9:9" ht="15.75" customHeight="1">
+    <row r="532" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I532" s="13"/>
     </row>
-    <row r="533" spans="9:9" ht="15.75" customHeight="1">
+    <row r="533" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I533" s="13"/>
     </row>
-    <row r="534" spans="9:9" ht="15.75" customHeight="1">
+    <row r="534" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I534" s="13"/>
     </row>
-    <row r="535" spans="9:9" ht="15.75" customHeight="1">
+    <row r="535" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I535" s="13"/>
     </row>
-    <row r="536" spans="9:9" ht="15.75" customHeight="1">
+    <row r="536" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I536" s="13"/>
     </row>
-    <row r="537" spans="9:9" ht="15.75" customHeight="1">
+    <row r="537" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I537" s="13"/>
     </row>
-    <row r="538" spans="9:9" ht="15.75" customHeight="1">
+    <row r="538" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I538" s="13"/>
     </row>
-    <row r="539" spans="9:9" ht="15.75" customHeight="1">
+    <row r="539" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I539" s="13"/>
     </row>
-    <row r="540" spans="9:9" ht="15.75" customHeight="1">
+    <row r="540" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I540" s="13"/>
     </row>
-    <row r="541" spans="9:9" ht="15.75" customHeight="1">
+    <row r="541" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I541" s="13"/>
     </row>
-    <row r="542" spans="9:9" ht="15.75" customHeight="1">
+    <row r="542" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I542" s="13"/>
     </row>
-    <row r="543" spans="9:9" ht="15.75" customHeight="1">
+    <row r="543" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I543" s="13"/>
     </row>
-    <row r="544" spans="9:9" ht="15.75" customHeight="1">
+    <row r="544" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I544" s="13"/>
     </row>
-    <row r="545" spans="9:9" ht="15.75" customHeight="1">
+    <row r="545" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I545" s="13"/>
     </row>
-    <row r="546" spans="9:9" ht="15.75" customHeight="1">
+    <row r="546" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I546" s="13"/>
     </row>
-    <row r="547" spans="9:9" ht="15.75" customHeight="1">
+    <row r="547" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I547" s="13"/>
     </row>
-    <row r="548" spans="9:9" ht="15.75" customHeight="1">
+    <row r="548" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I548" s="13"/>
     </row>
-    <row r="549" spans="9:9" ht="15.75" customHeight="1">
+    <row r="549" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I549" s="13"/>
     </row>
-    <row r="550" spans="9:9" ht="15.75" customHeight="1">
+    <row r="550" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I550" s="13"/>
     </row>
-    <row r="551" spans="9:9" ht="15.75" customHeight="1">
+    <row r="551" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I551" s="13"/>
     </row>
-    <row r="552" spans="9:9" ht="15.75" customHeight="1">
+    <row r="552" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I552" s="13"/>
     </row>
-    <row r="553" spans="9:9" ht="15.75" customHeight="1">
+    <row r="553" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I553" s="13"/>
     </row>
-    <row r="554" spans="9:9" ht="15.75" customHeight="1">
+    <row r="554" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I554" s="13"/>
     </row>
-    <row r="555" spans="9:9" ht="15.75" customHeight="1">
+    <row r="555" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I555" s="13"/>
     </row>
-    <row r="556" spans="9:9" ht="15.75" customHeight="1">
+    <row r="556" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I556" s="13"/>
     </row>
-    <row r="557" spans="9:9" ht="15.75" customHeight="1">
+    <row r="557" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I557" s="13"/>
     </row>
-    <row r="558" spans="9:9" ht="15.75" customHeight="1">
+    <row r="558" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I558" s="13"/>
     </row>
-    <row r="559" spans="9:9" ht="15.75" customHeight="1">
+    <row r="559" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I559" s="13"/>
     </row>
-    <row r="560" spans="9:9" ht="15.75" customHeight="1">
+    <row r="560" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I560" s="13"/>
     </row>
-    <row r="561" spans="9:9" ht="15.75" customHeight="1">
+    <row r="561" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I561" s="13"/>
     </row>
-    <row r="562" spans="9:9" ht="15.75" customHeight="1">
+    <row r="562" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I562" s="13"/>
     </row>
-    <row r="563" spans="9:9" ht="15.75" customHeight="1">
+    <row r="563" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I563" s="13"/>
     </row>
-    <row r="564" spans="9:9" ht="15.75" customHeight="1">
+    <row r="564" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I564" s="13"/>
     </row>
-    <row r="565" spans="9:9" ht="15.75" customHeight="1">
+    <row r="565" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I565" s="13"/>
     </row>
-    <row r="566" spans="9:9" ht="15.75" customHeight="1">
+    <row r="566" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I566" s="13"/>
     </row>
-    <row r="567" spans="9:9" ht="15.75" customHeight="1">
+    <row r="567" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I567" s="13"/>
     </row>
-    <row r="568" spans="9:9" ht="15.75" customHeight="1">
+    <row r="568" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I568" s="13"/>
     </row>
-    <row r="569" spans="9:9" ht="15.75" customHeight="1">
+    <row r="569" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I569" s="13"/>
     </row>
-    <row r="570" spans="9:9" ht="15.75" customHeight="1">
+    <row r="570" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I570" s="13"/>
     </row>
-    <row r="571" spans="9:9" ht="15.75" customHeight="1">
+    <row r="571" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I571" s="13"/>
     </row>
-    <row r="572" spans="9:9" ht="15.75" customHeight="1">
+    <row r="572" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I572" s="13"/>
     </row>
-    <row r="573" spans="9:9" ht="15.75" customHeight="1">
+    <row r="573" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I573" s="13"/>
     </row>
-    <row r="574" spans="9:9" ht="15.75" customHeight="1">
+    <row r="574" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I574" s="13"/>
     </row>
-    <row r="575" spans="9:9" ht="15.75" customHeight="1">
+    <row r="575" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I575" s="13"/>
     </row>
-    <row r="576" spans="9:9" ht="15.75" customHeight="1">
+    <row r="576" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I576" s="13"/>
     </row>
-    <row r="577" spans="9:9" ht="15.75" customHeight="1">
+    <row r="577" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I577" s="13"/>
     </row>
-    <row r="578" spans="9:9" ht="15.75" customHeight="1">
+    <row r="578" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I578" s="13"/>
     </row>
-    <row r="579" spans="9:9" ht="15.75" customHeight="1">
+    <row r="579" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I579" s="13"/>
     </row>
-    <row r="580" spans="9:9" ht="15.75" customHeight="1">
+    <row r="580" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I580" s="13"/>
     </row>
-    <row r="581" spans="9:9" ht="15.75" customHeight="1">
+    <row r="581" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I581" s="13"/>
     </row>
-    <row r="582" spans="9:9" ht="15.75" customHeight="1">
+    <row r="582" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I582" s="13"/>
     </row>
-    <row r="583" spans="9:9" ht="15.75" customHeight="1">
+    <row r="583" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I583" s="13"/>
     </row>
-    <row r="584" spans="9:9" ht="15.75" customHeight="1">
+    <row r="584" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I584" s="13"/>
     </row>
-    <row r="585" spans="9:9" ht="15.75" customHeight="1">
+    <row r="585" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I585" s="13"/>
     </row>
-    <row r="586" spans="9:9" ht="15.75" customHeight="1">
+    <row r="586" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I586" s="13"/>
     </row>
-    <row r="587" spans="9:9" ht="15.75" customHeight="1">
+    <row r="587" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I587" s="13"/>
     </row>
-    <row r="588" spans="9:9" ht="15.75" customHeight="1">
+    <row r="588" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I588" s="13"/>
     </row>
-    <row r="589" spans="9:9" ht="15.75" customHeight="1">
+    <row r="589" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I589" s="13"/>
     </row>
-    <row r="590" spans="9:9" ht="15.75" customHeight="1">
+    <row r="590" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I590" s="13"/>
     </row>
-    <row r="591" spans="9:9" ht="15.75" customHeight="1">
+    <row r="591" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I591" s="13"/>
     </row>
-    <row r="592" spans="9:9" ht="15.75" customHeight="1">
+    <row r="592" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I592" s="13"/>
     </row>
-    <row r="593" spans="9:9" ht="15.75" customHeight="1">
+    <row r="593" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I593" s="13"/>
     </row>
-    <row r="594" spans="9:9" ht="15.75" customHeight="1">
+    <row r="594" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I594" s="13"/>
     </row>
-    <row r="595" spans="9:9" ht="15.75" customHeight="1">
+    <row r="595" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I595" s="13"/>
     </row>
-    <row r="596" spans="9:9" ht="15.75" customHeight="1">
+    <row r="596" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I596" s="13"/>
     </row>
-    <row r="597" spans="9:9" ht="15.75" customHeight="1">
+    <row r="597" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I597" s="13"/>
     </row>
-    <row r="598" spans="9:9" ht="15.75" customHeight="1">
+    <row r="598" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I598" s="13"/>
     </row>
-    <row r="599" spans="9:9" ht="15.75" customHeight="1">
+    <row r="599" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I599" s="13"/>
     </row>
-    <row r="600" spans="9:9" ht="15.75" customHeight="1">
+    <row r="600" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I600" s="13"/>
     </row>
-    <row r="601" spans="9:9" ht="15.75" customHeight="1">
+    <row r="601" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I601" s="13"/>
     </row>
-    <row r="602" spans="9:9" ht="15.75" customHeight="1">
+    <row r="602" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I602" s="13"/>
     </row>
-    <row r="603" spans="9:9" ht="15.75" customHeight="1">
+    <row r="603" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I603" s="13"/>
     </row>
-    <row r="604" spans="9:9" ht="15.75" customHeight="1">
+    <row r="604" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I604" s="13"/>
     </row>
-    <row r="605" spans="9:9" ht="15.75" customHeight="1">
+    <row r="605" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I605" s="13"/>
     </row>
-    <row r="606" spans="9:9" ht="15.75" customHeight="1">
+    <row r="606" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I606" s="13"/>
     </row>
-    <row r="607" spans="9:9" ht="15.75" customHeight="1">
+    <row r="607" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I607" s="13"/>
     </row>
-    <row r="608" spans="9:9" ht="15.75" customHeight="1">
+    <row r="608" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I608" s="13"/>
     </row>
-    <row r="609" spans="9:9" ht="15.75" customHeight="1">
+    <row r="609" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I609" s="13"/>
     </row>
-    <row r="610" spans="9:9" ht="15.75" customHeight="1">
+    <row r="610" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I610" s="13"/>
     </row>
-    <row r="611" spans="9:9" ht="15.75" customHeight="1">
+    <row r="611" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I611" s="13"/>
     </row>
-    <row r="612" spans="9:9" ht="15.75" customHeight="1">
+    <row r="612" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I612" s="13"/>
     </row>
-    <row r="613" spans="9:9" ht="15.75" customHeight="1">
+    <row r="613" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I613" s="13"/>
     </row>
-    <row r="614" spans="9:9" ht="15.75" customHeight="1">
+    <row r="614" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I614" s="13"/>
     </row>
-    <row r="615" spans="9:9" ht="15.75" customHeight="1">
+    <row r="615" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I615" s="13"/>
     </row>
-    <row r="616" spans="9:9" ht="15.75" customHeight="1">
+    <row r="616" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I616" s="13"/>
     </row>
-    <row r="617" spans="9:9" ht="15.75" customHeight="1">
+    <row r="617" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I617" s="13"/>
     </row>
-    <row r="618" spans="9:9" ht="15.75" customHeight="1">
+    <row r="618" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I618" s="13"/>
     </row>
-    <row r="619" spans="9:9" ht="15.75" customHeight="1">
+    <row r="619" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I619" s="13"/>
     </row>
-    <row r="620" spans="9:9" ht="15.75" customHeight="1">
+    <row r="620" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I620" s="13"/>
     </row>
-    <row r="621" spans="9:9" ht="15.75" customHeight="1">
+    <row r="621" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I621" s="13"/>
     </row>
-    <row r="622" spans="9:9" ht="15.75" customHeight="1">
+    <row r="622" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I622" s="13"/>
     </row>
-    <row r="623" spans="9:9" ht="15.75" customHeight="1">
+    <row r="623" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I623" s="13"/>
     </row>
-    <row r="624" spans="9:9" ht="15.75" customHeight="1">
+    <row r="624" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I624" s="13"/>
     </row>
-    <row r="625" spans="9:9" ht="15.75" customHeight="1">
+    <row r="625" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I625" s="13"/>
     </row>
-    <row r="626" spans="9:9" ht="15.75" customHeight="1">
+    <row r="626" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I626" s="13"/>
     </row>
-    <row r="627" spans="9:9" ht="15.75" customHeight="1">
+    <row r="627" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I627" s="13"/>
     </row>
-    <row r="628" spans="9:9" ht="15.75" customHeight="1">
+    <row r="628" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I628" s="13"/>
     </row>
-    <row r="629" spans="9:9" ht="15.75" customHeight="1">
+    <row r="629" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I629" s="13"/>
     </row>
-    <row r="630" spans="9:9" ht="15.75" customHeight="1">
+    <row r="630" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I630" s="13"/>
     </row>
-    <row r="631" spans="9:9" ht="15.75" customHeight="1">
+    <row r="631" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I631" s="13"/>
     </row>
-    <row r="632" spans="9:9" ht="15.75" customHeight="1">
+    <row r="632" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I632" s="13"/>
     </row>
-    <row r="633" spans="9:9" ht="15.75" customHeight="1">
+    <row r="633" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I633" s="13"/>
     </row>
-    <row r="634" spans="9:9" ht="15.75" customHeight="1">
+    <row r="634" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I634" s="13"/>
     </row>
-    <row r="635" spans="9:9" ht="15.75" customHeight="1">
+    <row r="635" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I635" s="13"/>
     </row>
-    <row r="636" spans="9:9" ht="15.75" customHeight="1">
+    <row r="636" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I636" s="13"/>
     </row>
-    <row r="637" spans="9:9" ht="15.75" customHeight="1">
+    <row r="637" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I637" s="13"/>
     </row>
-    <row r="638" spans="9:9" ht="15.75" customHeight="1">
+    <row r="638" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I638" s="13"/>
     </row>
-    <row r="639" spans="9:9" ht="15.75" customHeight="1">
+    <row r="639" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I639" s="13"/>
     </row>
-    <row r="640" spans="9:9" ht="15.75" customHeight="1">
+    <row r="640" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I640" s="13"/>
     </row>
-    <row r="641" spans="9:9" ht="15.75" customHeight="1">
+    <row r="641" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I641" s="13"/>
     </row>
-    <row r="642" spans="9:9" ht="15.75" customHeight="1">
+    <row r="642" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I642" s="13"/>
     </row>
-    <row r="643" spans="9:9" ht="15.75" customHeight="1">
+    <row r="643" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I643" s="13"/>
     </row>
-    <row r="644" spans="9:9" ht="15.75" customHeight="1">
+    <row r="644" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I644" s="13"/>
     </row>
-    <row r="645" spans="9:9" ht="15.75" customHeight="1">
+    <row r="645" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I645" s="13"/>
     </row>
-    <row r="646" spans="9:9" ht="15.75" customHeight="1">
+    <row r="646" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I646" s="13"/>
     </row>
-    <row r="647" spans="9:9" ht="15.75" customHeight="1">
+    <row r="647" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I647" s="13"/>
     </row>
-    <row r="648" spans="9:9" ht="15.75" customHeight="1">
+    <row r="648" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I648" s="13"/>
     </row>
-    <row r="649" spans="9:9" ht="15.75" customHeight="1">
+    <row r="649" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I649" s="13"/>
     </row>
-    <row r="650" spans="9:9" ht="15.75" customHeight="1">
+    <row r="650" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I650" s="13"/>
     </row>
-    <row r="651" spans="9:9" ht="15.75" customHeight="1">
+    <row r="651" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I651" s="13"/>
     </row>
-    <row r="652" spans="9:9" ht="15.75" customHeight="1">
+    <row r="652" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I652" s="13"/>
     </row>
-    <row r="653" spans="9:9" ht="15.75" customHeight="1">
+    <row r="653" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I653" s="13"/>
     </row>
-    <row r="654" spans="9:9" ht="15.75" customHeight="1">
+    <row r="654" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I654" s="13"/>
     </row>
-    <row r="655" spans="9:9" ht="15.75" customHeight="1">
+    <row r="655" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I655" s="13"/>
     </row>
-    <row r="656" spans="9:9" ht="15.75" customHeight="1">
+    <row r="656" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I656" s="13"/>
     </row>
-    <row r="657" spans="9:9" ht="15.75" customHeight="1">
+    <row r="657" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I657" s="13"/>
     </row>
-    <row r="658" spans="9:9" ht="15.75" customHeight="1">
+    <row r="658" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I658" s="13"/>
     </row>
-    <row r="659" spans="9:9" ht="15.75" customHeight="1">
+    <row r="659" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I659" s="13"/>
     </row>
-    <row r="660" spans="9:9" ht="15.75" customHeight="1">
+    <row r="660" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I660" s="13"/>
     </row>
-    <row r="661" spans="9:9" ht="15.75" customHeight="1">
+    <row r="661" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I661" s="13"/>
     </row>
-    <row r="662" spans="9:9" ht="15.75" customHeight="1">
+    <row r="662" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I662" s="13"/>
     </row>
-    <row r="663" spans="9:9" ht="15.75" customHeight="1">
+    <row r="663" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I663" s="13"/>
     </row>
-    <row r="664" spans="9:9" ht="15.75" customHeight="1">
+    <row r="664" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I664" s="13"/>
     </row>
-    <row r="665" spans="9:9" ht="15.75" customHeight="1">
+    <row r="665" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I665" s="13"/>
     </row>
-    <row r="666" spans="9:9" ht="15.75" customHeight="1">
+    <row r="666" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I666" s="13"/>
     </row>
-    <row r="667" spans="9:9" ht="15.75" customHeight="1">
+    <row r="667" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I667" s="13"/>
     </row>
-    <row r="668" spans="9:9" ht="15.75" customHeight="1">
+    <row r="668" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I668" s="13"/>
     </row>
-    <row r="669" spans="9:9" ht="15.75" customHeight="1">
+    <row r="669" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I669" s="13"/>
     </row>
-    <row r="670" spans="9:9" ht="15.75" customHeight="1">
+    <row r="670" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I670" s="13"/>
     </row>
-    <row r="671" spans="9:9" ht="15.75" customHeight="1">
+    <row r="671" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I671" s="13"/>
     </row>
-    <row r="672" spans="9:9" ht="15.75" customHeight="1">
+    <row r="672" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I672" s="13"/>
     </row>
-    <row r="673" spans="9:9" ht="15.75" customHeight="1">
+    <row r="673" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I673" s="13"/>
     </row>
-    <row r="674" spans="9:9" ht="15.75" customHeight="1">
+    <row r="674" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I674" s="13"/>
     </row>
-    <row r="675" spans="9:9" ht="15.75" customHeight="1">
+    <row r="675" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I675" s="13"/>
     </row>
-    <row r="676" spans="9:9" ht="15.75" customHeight="1">
+    <row r="676" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I676" s="13"/>
     </row>
-    <row r="677" spans="9:9" ht="15.75" customHeight="1">
+    <row r="677" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I677" s="13"/>
     </row>
-    <row r="678" spans="9:9" ht="15.75" customHeight="1">
+    <row r="678" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I678" s="13"/>
     </row>
-    <row r="679" spans="9:9" ht="15.75" customHeight="1">
+    <row r="679" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I679" s="13"/>
     </row>
-    <row r="680" spans="9:9" ht="15.75" customHeight="1">
+    <row r="680" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I680" s="13"/>
     </row>
-    <row r="681" spans="9:9" ht="15.75" customHeight="1">
+    <row r="681" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I681" s="13"/>
     </row>
-    <row r="682" spans="9:9" ht="15.75" customHeight="1">
+    <row r="682" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I682" s="13"/>
     </row>
-    <row r="683" spans="9:9" ht="15.75" customHeight="1">
+    <row r="683" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I683" s="13"/>
     </row>
-    <row r="684" spans="9:9" ht="15.75" customHeight="1">
+    <row r="684" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I684" s="13"/>
     </row>
-    <row r="685" spans="9:9" ht="15.75" customHeight="1">
+    <row r="685" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I685" s="13"/>
     </row>
-    <row r="686" spans="9:9" ht="15.75" customHeight="1">
+    <row r="686" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I686" s="13"/>
     </row>
-    <row r="687" spans="9:9" ht="15.75" customHeight="1">
+    <row r="687" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I687" s="13"/>
     </row>
-    <row r="688" spans="9:9" ht="15.75" customHeight="1">
+    <row r="688" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I688" s="13"/>
     </row>
-    <row r="689" spans="9:9" ht="15.75" customHeight="1">
+    <row r="689" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I689" s="13"/>
     </row>
-    <row r="690" spans="9:9" ht="15.75" customHeight="1">
+    <row r="690" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I690" s="13"/>
     </row>
-    <row r="691" spans="9:9" ht="15.75" customHeight="1">
+    <row r="691" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I691" s="13"/>
     </row>
-    <row r="692" spans="9:9" ht="15.75" customHeight="1">
+    <row r="692" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I692" s="13"/>
     </row>
-    <row r="693" spans="9:9" ht="15.75" customHeight="1">
+    <row r="693" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I693" s="13"/>
     </row>
-    <row r="694" spans="9:9" ht="15.75" customHeight="1">
+    <row r="694" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I694" s="13"/>
     </row>
-    <row r="695" spans="9:9" ht="15.75" customHeight="1">
+    <row r="695" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I695" s="13"/>
     </row>
-    <row r="696" spans="9:9" ht="15.75" customHeight="1">
+    <row r="696" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I696" s="13"/>
     </row>
-    <row r="697" spans="9:9" ht="15.75" customHeight="1">
+    <row r="697" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I697" s="13"/>
     </row>
-    <row r="698" spans="9:9" ht="15.75" customHeight="1">
+    <row r="698" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I698" s="13"/>
     </row>
-    <row r="699" spans="9:9" ht="15.75" customHeight="1">
+    <row r="699" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I699" s="13"/>
     </row>
-    <row r="700" spans="9:9" ht="15.75" customHeight="1">
+    <row r="700" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I700" s="13"/>
     </row>
-    <row r="701" spans="9:9" ht="15.75" customHeight="1">
+    <row r="701" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I701" s="13"/>
     </row>
-    <row r="702" spans="9:9" ht="15.75" customHeight="1">
+    <row r="702" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I702" s="13"/>
     </row>
-    <row r="703" spans="9:9" ht="15.75" customHeight="1">
+    <row r="703" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I703" s="13"/>
     </row>
-    <row r="704" spans="9:9" ht="15.75" customHeight="1">
+    <row r="704" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I704" s="13"/>
     </row>
-    <row r="705" spans="9:9" ht="15.75" customHeight="1">
+    <row r="705" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I705" s="13"/>
     </row>
-    <row r="706" spans="9:9" ht="15.75" customHeight="1">
+    <row r="706" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I706" s="13"/>
     </row>
-    <row r="707" spans="9:9" ht="15.75" customHeight="1">
+    <row r="707" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I707" s="13"/>
     </row>
-    <row r="708" spans="9:9" ht="15.75" customHeight="1">
+    <row r="708" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I708" s="13"/>
     </row>
-    <row r="709" spans="9:9" ht="15.75" customHeight="1">
+    <row r="709" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I709" s="13"/>
     </row>
-    <row r="710" spans="9:9" ht="15.75" customHeight="1">
+    <row r="710" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I710" s="13"/>
     </row>
-    <row r="711" spans="9:9" ht="15.75" customHeight="1">
+    <row r="711" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I711" s="13"/>
     </row>
-    <row r="712" spans="9:9" ht="15.75" customHeight="1">
+    <row r="712" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I712" s="13"/>
     </row>
-    <row r="713" spans="9:9" ht="15.75" customHeight="1">
+    <row r="713" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I713" s="13"/>
     </row>
-    <row r="714" spans="9:9" ht="15.75" customHeight="1">
+    <row r="714" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I714" s="13"/>
     </row>
-    <row r="715" spans="9:9" ht="15.75" customHeight="1">
+    <row r="715" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I715" s="13"/>
     </row>
-    <row r="716" spans="9:9" ht="15.75" customHeight="1">
+    <row r="716" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I716" s="13"/>
     </row>
-    <row r="717" spans="9:9" ht="15.75" customHeight="1">
+    <row r="717" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I717" s="13"/>
     </row>
-    <row r="718" spans="9:9" ht="15.75" customHeight="1">
+    <row r="718" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I718" s="13"/>
     </row>
-    <row r="719" spans="9:9" ht="15.75" customHeight="1">
+    <row r="719" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I719" s="13"/>
     </row>
-    <row r="720" spans="9:9" ht="15.75" customHeight="1">
+    <row r="720" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I720" s="13"/>
     </row>
-    <row r="721" spans="9:9" ht="15.75" customHeight="1">
+    <row r="721" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I721" s="13"/>
     </row>
-    <row r="722" spans="9:9" ht="15.75" customHeight="1">
+    <row r="722" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I722" s="13"/>
     </row>
-    <row r="723" spans="9:9" ht="15.75" customHeight="1">
+    <row r="723" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I723" s="13"/>
     </row>
-    <row r="724" spans="9:9" ht="15.75" customHeight="1">
+    <row r="724" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I724" s="13"/>
     </row>
-    <row r="725" spans="9:9" ht="15.75" customHeight="1">
+    <row r="725" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I725" s="13"/>
     </row>
-    <row r="726" spans="9:9" ht="15.75" customHeight="1">
+    <row r="726" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I726" s="13"/>
     </row>
-    <row r="727" spans="9:9" ht="15.75" customHeight="1">
+    <row r="727" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I727" s="13"/>
     </row>
-    <row r="728" spans="9:9" ht="15.75" customHeight="1">
+    <row r="728" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I728" s="13"/>
     </row>
-    <row r="729" spans="9:9" ht="15.75" customHeight="1">
+    <row r="729" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I729" s="13"/>
     </row>
-    <row r="730" spans="9:9" ht="15.75" customHeight="1">
+    <row r="730" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I730" s="13"/>
     </row>
-    <row r="731" spans="9:9" ht="15.75" customHeight="1">
+    <row r="731" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I731" s="13"/>
     </row>
-    <row r="732" spans="9:9" ht="15.75" customHeight="1">
+    <row r="732" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I732" s="13"/>
     </row>
-    <row r="733" spans="9:9" ht="15.75" customHeight="1">
+    <row r="733" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I733" s="13"/>
     </row>
-    <row r="734" spans="9:9" ht="15.75" customHeight="1">
+    <row r="734" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I734" s="13"/>
     </row>
-    <row r="735" spans="9:9" ht="15.75" customHeight="1">
+    <row r="735" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I735" s="13"/>
     </row>
-    <row r="736" spans="9:9" ht="15.75" customHeight="1">
+    <row r="736" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I736" s="13"/>
     </row>
-    <row r="737" spans="9:9" ht="15.75" customHeight="1">
+    <row r="737" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I737" s="13"/>
     </row>
-    <row r="738" spans="9:9" ht="15.75" customHeight="1">
+    <row r="738" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I738" s="13"/>
     </row>
-    <row r="739" spans="9:9" ht="15.75" customHeight="1">
+    <row r="739" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I739" s="13"/>
     </row>
-    <row r="740" spans="9:9" ht="15.75" customHeight="1">
+    <row r="740" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I740" s="13"/>
     </row>
-    <row r="741" spans="9:9" ht="15.75" customHeight="1">
+    <row r="741" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I741" s="13"/>
     </row>
-    <row r="742" spans="9:9" ht="15.75" customHeight="1">
+    <row r="742" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I742" s="13"/>
     </row>
-    <row r="743" spans="9:9" ht="15.75" customHeight="1">
+    <row r="743" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I743" s="13"/>
     </row>
-    <row r="744" spans="9:9" ht="15.75" customHeight="1">
+    <row r="744" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I744" s="13"/>
     </row>
-    <row r="745" spans="9:9" ht="15.75" customHeight="1">
+    <row r="745" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I745" s="13"/>
     </row>
-    <row r="746" spans="9:9" ht="15.75" customHeight="1">
+    <row r="746" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I746" s="13"/>
     </row>
-    <row r="747" spans="9:9" ht="15.75" customHeight="1">
+    <row r="747" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I747" s="13"/>
     </row>
-    <row r="748" spans="9:9" ht="15.75" customHeight="1">
+    <row r="748" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I748" s="13"/>
     </row>
-    <row r="749" spans="9:9" ht="15.75" customHeight="1">
+    <row r="749" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I749" s="13"/>
     </row>
-    <row r="750" spans="9:9" ht="15.75" customHeight="1">
+    <row r="750" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I750" s="13"/>
     </row>
-    <row r="751" spans="9:9" ht="15.75" customHeight="1">
+    <row r="751" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I751" s="13"/>
     </row>
-    <row r="752" spans="9:9" ht="15.75" customHeight="1">
+    <row r="752" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I752" s="13"/>
     </row>
-    <row r="753" spans="9:9" ht="15.75" customHeight="1">
+    <row r="753" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I753" s="13"/>
     </row>
-    <row r="754" spans="9:9" ht="15.75" customHeight="1">
+    <row r="754" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I754" s="13"/>
     </row>
-    <row r="755" spans="9:9" ht="15.75" customHeight="1">
+    <row r="755" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I755" s="13"/>
     </row>
-    <row r="756" spans="9:9" ht="15.75" customHeight="1">
+    <row r="756" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I756" s="13"/>
     </row>
-    <row r="757" spans="9:9" ht="15.75" customHeight="1">
+    <row r="757" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I757" s="13"/>
     </row>
-    <row r="758" spans="9:9" ht="15.75" customHeight="1">
+    <row r="758" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I758" s="13"/>
     </row>
-    <row r="759" spans="9:9" ht="15.75" customHeight="1">
+    <row r="759" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I759" s="13"/>
     </row>
-    <row r="760" spans="9:9" ht="15.75" customHeight="1">
+    <row r="760" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I760" s="13"/>
     </row>
-    <row r="761" spans="9:9" ht="15.75" customHeight="1">
+    <row r="761" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I761" s="13"/>
     </row>
-    <row r="762" spans="9:9" ht="15.75" customHeight="1">
+    <row r="762" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I762" s="13"/>
     </row>
-    <row r="763" spans="9:9" ht="15.75" customHeight="1">
+    <row r="763" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I763" s="13"/>
     </row>
-    <row r="764" spans="9:9" ht="15.75" customHeight="1">
+    <row r="764" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I764" s="13"/>
     </row>
-    <row r="765" spans="9:9" ht="15.75" customHeight="1">
+    <row r="765" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I765" s="13"/>
     </row>
-    <row r="766" spans="9:9" ht="15.75" customHeight="1">
+    <row r="766" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I766" s="13"/>
     </row>
-    <row r="767" spans="9:9" ht="15.75" customHeight="1">
+    <row r="767" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I767" s="13"/>
     </row>
-    <row r="768" spans="9:9" ht="15.75" customHeight="1">
+    <row r="768" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I768" s="13"/>
     </row>
-    <row r="769" spans="9:9" ht="15.75" customHeight="1">
+    <row r="769" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I769" s="13"/>
     </row>
-    <row r="770" spans="9:9" ht="15.75" customHeight="1">
+    <row r="770" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I770" s="13"/>
     </row>
-    <row r="771" spans="9:9" ht="15.75" customHeight="1">
+    <row r="771" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I771" s="13"/>
     </row>
-    <row r="772" spans="9:9" ht="15.75" customHeight="1">
+    <row r="772" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I772" s="13"/>
     </row>
-    <row r="773" spans="9:9" ht="15.75" customHeight="1">
+    <row r="773" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I773" s="13"/>
     </row>
-    <row r="774" spans="9:9" ht="15.75" customHeight="1">
+    <row r="774" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I774" s="13"/>
     </row>
-    <row r="775" spans="9:9" ht="15.75" customHeight="1">
+    <row r="775" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I775" s="13"/>
     </row>
-    <row r="776" spans="9:9" ht="15.75" customHeight="1">
+    <row r="776" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I776" s="13"/>
     </row>
-    <row r="777" spans="9:9" ht="15.75" customHeight="1">
+    <row r="777" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I777" s="13"/>
     </row>
-    <row r="778" spans="9:9" ht="15.75" customHeight="1">
+    <row r="778" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I778" s="13"/>
     </row>
-    <row r="779" spans="9:9" ht="15.75" customHeight="1">
+    <row r="779" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I779" s="13"/>
     </row>
-    <row r="780" spans="9:9" ht="15.75" customHeight="1">
+    <row r="780" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I780" s="13"/>
     </row>
-    <row r="781" spans="9:9" ht="15.75" customHeight="1">
+    <row r="781" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I781" s="13"/>
     </row>
-    <row r="782" spans="9:9" ht="15.75" customHeight="1">
+    <row r="782" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I782" s="13"/>
     </row>
-    <row r="783" spans="9:9" ht="15.75" customHeight="1">
+    <row r="783" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I783" s="13"/>
     </row>
-    <row r="784" spans="9:9" ht="15.75" customHeight="1">
+    <row r="784" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I784" s="13"/>
     </row>
-    <row r="785" spans="9:9" ht="15.75" customHeight="1">
+    <row r="785" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I785" s="13"/>
     </row>
-    <row r="786" spans="9:9" ht="15.75" customHeight="1">
+    <row r="786" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I786" s="13"/>
     </row>
-    <row r="787" spans="9:9" ht="15.75" customHeight="1">
+    <row r="787" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I787" s="13"/>
     </row>
-    <row r="788" spans="9:9" ht="15.75" customHeight="1">
+    <row r="788" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I788" s="13"/>
     </row>
-    <row r="789" spans="9:9" ht="15.75" customHeight="1">
+    <row r="789" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I789" s="13"/>
     </row>
-    <row r="790" spans="9:9" ht="15.75" customHeight="1">
+    <row r="790" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I790" s="13"/>
     </row>
-    <row r="791" spans="9:9" ht="15.75" customHeight="1">
+    <row r="791" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I791" s="13"/>
     </row>
-    <row r="792" spans="9:9" ht="15.75" customHeight="1">
+    <row r="792" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I792" s="13"/>
     </row>
-    <row r="793" spans="9:9" ht="15.75" customHeight="1">
+    <row r="793" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I793" s="13"/>
     </row>
-    <row r="794" spans="9:9" ht="15.75" customHeight="1">
+    <row r="794" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I794" s="13"/>
     </row>
-    <row r="795" spans="9:9" ht="15.75" customHeight="1">
+    <row r="795" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I795" s="13"/>
     </row>
-    <row r="796" spans="9:9" ht="15.75" customHeight="1">
+    <row r="796" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I796" s="13"/>
     </row>
-    <row r="797" spans="9:9" ht="15.75" customHeight="1">
+    <row r="797" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I797" s="13"/>
     </row>
-    <row r="798" spans="9:9" ht="15.75" customHeight="1">
+    <row r="798" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I798" s="13"/>
     </row>
-    <row r="799" spans="9:9" ht="15.75" customHeight="1">
+    <row r="799" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I799" s="13"/>
     </row>
-    <row r="800" spans="9:9" ht="15.75" customHeight="1">
+    <row r="800" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I800" s="13"/>
     </row>
-    <row r="801" spans="9:9" ht="15.75" customHeight="1">
+    <row r="801" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I801" s="13"/>
     </row>
-    <row r="802" spans="9:9" ht="15.75" customHeight="1">
+    <row r="802" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I802" s="13"/>
     </row>
-    <row r="803" spans="9:9" ht="15.75" customHeight="1">
+    <row r="803" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I803" s="13"/>
     </row>
-    <row r="804" spans="9:9" ht="15.75" customHeight="1">
+    <row r="804" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I804" s="13"/>
     </row>
-    <row r="805" spans="9:9" ht="15.75" customHeight="1">
+    <row r="805" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I805" s="13"/>
     </row>
-    <row r="806" spans="9:9" ht="15.75" customHeight="1">
+    <row r="806" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I806" s="13"/>
     </row>
-    <row r="807" spans="9:9" ht="15.75" customHeight="1">
+    <row r="807" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I807" s="13"/>
     </row>
-    <row r="808" spans="9:9" ht="15.75" customHeight="1">
+    <row r="808" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I808" s="13"/>
     </row>
-    <row r="809" spans="9:9" ht="15.75" customHeight="1">
+    <row r="809" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I809" s="13"/>
     </row>
-    <row r="810" spans="9:9" ht="15.75" customHeight="1">
+    <row r="810" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I810" s="13"/>
     </row>
-    <row r="811" spans="9:9" ht="15.75" customHeight="1">
+    <row r="811" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I811" s="13"/>
     </row>
-    <row r="812" spans="9:9" ht="15.75" customHeight="1">
+    <row r="812" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I812" s="13"/>
     </row>
-    <row r="813" spans="9:9" ht="15.75" customHeight="1">
+    <row r="813" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I813" s="13"/>
     </row>
-    <row r="814" spans="9:9" ht="15.75" customHeight="1">
+    <row r="814" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I814" s="13"/>
     </row>
-    <row r="815" spans="9:9" ht="15.75" customHeight="1">
+    <row r="815" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I815" s="13"/>
     </row>
-    <row r="816" spans="9:9" ht="15.75" customHeight="1">
+    <row r="816" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I816" s="13"/>
     </row>
-    <row r="817" spans="9:9" ht="15.75" customHeight="1">
+    <row r="817" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I817" s="13"/>
     </row>
-    <row r="818" spans="9:9" ht="15.75" customHeight="1">
+    <row r="818" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I818" s="13"/>
     </row>
-    <row r="819" spans="9:9" ht="15.75" customHeight="1">
+    <row r="819" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I819" s="13"/>
     </row>
-    <row r="820" spans="9:9" ht="15.75" customHeight="1">
+    <row r="820" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I820" s="13"/>
     </row>
-    <row r="821" spans="9:9" ht="15.75" customHeight="1">
+    <row r="821" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I821" s="13"/>
     </row>
-    <row r="822" spans="9:9" ht="15.75" customHeight="1">
+    <row r="822" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I822" s="13"/>
     </row>
-    <row r="823" spans="9:9" ht="15.75" customHeight="1">
+    <row r="823" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I823" s="13"/>
     </row>
-    <row r="824" spans="9:9" ht="15.75" customHeight="1">
+    <row r="824" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I824" s="13"/>
     </row>
-    <row r="825" spans="9:9" ht="15.75" customHeight="1">
+    <row r="825" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I825" s="13"/>
     </row>
-    <row r="826" spans="9:9" ht="15.75" customHeight="1">
+    <row r="826" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I826" s="13"/>
     </row>
-    <row r="827" spans="9:9" ht="15.75" customHeight="1">
+    <row r="827" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I827" s="13"/>
     </row>
-    <row r="828" spans="9:9" ht="15.75" customHeight="1">
+    <row r="828" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I828" s="13"/>
     </row>
-    <row r="829" spans="9:9" ht="15.75" customHeight="1">
+    <row r="829" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I829" s="13"/>
     </row>
-    <row r="830" spans="9:9" ht="15.75" customHeight="1">
+    <row r="830" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I830" s="13"/>
     </row>
-    <row r="831" spans="9:9" ht="15.75" customHeight="1">
+    <row r="831" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I831" s="13"/>
     </row>
-    <row r="832" spans="9:9" ht="15.75" customHeight="1">
+    <row r="832" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I832" s="13"/>
     </row>
-    <row r="833" spans="9:9" ht="15.75" customHeight="1">
+    <row r="833" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I833" s="13"/>
     </row>
-    <row r="834" spans="9:9" ht="15.75" customHeight="1">
+    <row r="834" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I834" s="13"/>
     </row>
-    <row r="835" spans="9:9" ht="15.75" customHeight="1">
+    <row r="835" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I835" s="13"/>
     </row>
-    <row r="836" spans="9:9" ht="15.75" customHeight="1">
+    <row r="836" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I836" s="13"/>
     </row>
-    <row r="837" spans="9:9" ht="15.75" customHeight="1">
+    <row r="837" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I837" s="13"/>
     </row>
-    <row r="838" spans="9:9" ht="15.75" customHeight="1">
+    <row r="838" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I838" s="13"/>
     </row>
-    <row r="839" spans="9:9" ht="15.75" customHeight="1">
+    <row r="839" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I839" s="13"/>
     </row>
-    <row r="840" spans="9:9" ht="15.75" customHeight="1">
+    <row r="840" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I840" s="13"/>
     </row>
-    <row r="841" spans="9:9" ht="15.75" customHeight="1">
+    <row r="841" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I841" s="13"/>
     </row>
-    <row r="842" spans="9:9" ht="15.75" customHeight="1">
+    <row r="842" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I842" s="13"/>
     </row>
-    <row r="843" spans="9:9" ht="15.75" customHeight="1">
+    <row r="843" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I843" s="13"/>
     </row>
-    <row r="844" spans="9:9" ht="15.75" customHeight="1">
+    <row r="844" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I844" s="13"/>
     </row>
-    <row r="845" spans="9:9" ht="15.75" customHeight="1">
+    <row r="845" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I845" s="13"/>
     </row>
-    <row r="846" spans="9:9" ht="15.75" customHeight="1">
+    <row r="846" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I846" s="13"/>
     </row>
-    <row r="847" spans="9:9" ht="15.75" customHeight="1">
+    <row r="847" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I847" s="13"/>
     </row>
-    <row r="848" spans="9:9" ht="15.75" customHeight="1">
+    <row r="848" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I848" s="13"/>
     </row>
-    <row r="849" spans="9:9" ht="15.75" customHeight="1">
+    <row r="849" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I849" s="13"/>
     </row>
-    <row r="850" spans="9:9" ht="15.75" customHeight="1">
+    <row r="850" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I850" s="13"/>
     </row>
-    <row r="851" spans="9:9" ht="15.75" customHeight="1">
+    <row r="851" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I851" s="13"/>
     </row>
-    <row r="852" spans="9:9" ht="15.75" customHeight="1">
+    <row r="852" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I852" s="13"/>
     </row>
-    <row r="853" spans="9:9" ht="15.75" customHeight="1">
+    <row r="853" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I853" s="13"/>
     </row>
-    <row r="854" spans="9:9" ht="15.75" customHeight="1">
+    <row r="854" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I854" s="13"/>
     </row>
-    <row r="855" spans="9:9" ht="15.75" customHeight="1">
+    <row r="855" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I855" s="13"/>
     </row>
-    <row r="856" spans="9:9" ht="15.75" customHeight="1">
+    <row r="856" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I856" s="13"/>
     </row>
-    <row r="857" spans="9:9" ht="15.75" customHeight="1">
+    <row r="857" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I857" s="13"/>
     </row>
-    <row r="858" spans="9:9" ht="15.75" customHeight="1">
+    <row r="858" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I858" s="13"/>
     </row>
-    <row r="859" spans="9:9" ht="15.75" customHeight="1">
+    <row r="859" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I859" s="13"/>
     </row>
-    <row r="860" spans="9:9" ht="15.75" customHeight="1">
+    <row r="860" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I860" s="13"/>
     </row>
-    <row r="861" spans="9:9" ht="15.75" customHeight="1">
+    <row r="861" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I861" s="13"/>
     </row>
-    <row r="862" spans="9:9" ht="15.75" customHeight="1">
+    <row r="862" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I862" s="13"/>
     </row>
-    <row r="863" spans="9:9" ht="15.75" customHeight="1">
+    <row r="863" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I863" s="13"/>
     </row>
-    <row r="864" spans="9:9" ht="15.75" customHeight="1">
+    <row r="864" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I864" s="13"/>
     </row>
-    <row r="865" spans="9:9" ht="15.75" customHeight="1">
+    <row r="865" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I865" s="13"/>
     </row>
-    <row r="866" spans="9:9" ht="15.75" customHeight="1">
+    <row r="866" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I866" s="13"/>
     </row>
-    <row r="867" spans="9:9" ht="15.75" customHeight="1">
+    <row r="867" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I867" s="13"/>
     </row>
-    <row r="868" spans="9:9" ht="15.75" customHeight="1">
+    <row r="868" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I868" s="13"/>
     </row>
-    <row r="869" spans="9:9" ht="15.75" customHeight="1">
+    <row r="869" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I869" s="13"/>
     </row>
-    <row r="870" spans="9:9" ht="15.75" customHeight="1">
+    <row r="870" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I870" s="13"/>
     </row>
-    <row r="871" spans="9:9" ht="15.75" customHeight="1">
+    <row r="871" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I871" s="13"/>
     </row>
-    <row r="872" spans="9:9" ht="15.75" customHeight="1">
+    <row r="872" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I872" s="13"/>
     </row>
-    <row r="873" spans="9:9" ht="15.75" customHeight="1">
+    <row r="873" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I873" s="13"/>
     </row>
-    <row r="874" spans="9:9" ht="15.75" customHeight="1">
+    <row r="874" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I874" s="13"/>
     </row>
-    <row r="875" spans="9:9" ht="15.75" customHeight="1">
+    <row r="875" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I875" s="13"/>
     </row>
-    <row r="876" spans="9:9" ht="15.75" customHeight="1">
+    <row r="876" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I876" s="13"/>
     </row>
-    <row r="877" spans="9:9" ht="15.75" customHeight="1">
+    <row r="877" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I877" s="13"/>
     </row>
-    <row r="878" spans="9:9" ht="15.75" customHeight="1">
+    <row r="878" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I878" s="13"/>
     </row>
-    <row r="879" spans="9:9" ht="15.75" customHeight="1">
+    <row r="879" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I879" s="13"/>
     </row>
-    <row r="880" spans="9:9" ht="15.75" customHeight="1">
+    <row r="880" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I880" s="13"/>
     </row>
-    <row r="881" spans="9:9" ht="15.75" customHeight="1">
+    <row r="881" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I881" s="13"/>
     </row>
-    <row r="882" spans="9:9" ht="15.75" customHeight="1">
+    <row r="882" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I882" s="13"/>
     </row>
-    <row r="883" spans="9:9" ht="15.75" customHeight="1">
+    <row r="883" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I883" s="13"/>
     </row>
-    <row r="884" spans="9:9" ht="15.75" customHeight="1">
+    <row r="884" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I884" s="13"/>
     </row>
-    <row r="885" spans="9:9" ht="15.75" customHeight="1">
+    <row r="885" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I885" s="13"/>
     </row>
-    <row r="886" spans="9:9" ht="15.75" customHeight="1">
+    <row r="886" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I886" s="13"/>
     </row>
-    <row r="887" spans="9:9" ht="15.75" customHeight="1">
+    <row r="887" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I887" s="13"/>
     </row>
-    <row r="888" spans="9:9" ht="15.75" customHeight="1">
+    <row r="888" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I888" s="13"/>
     </row>
-    <row r="889" spans="9:9" ht="15.75" customHeight="1">
+    <row r="889" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I889" s="13"/>
     </row>
-    <row r="890" spans="9:9" ht="15.75" customHeight="1">
+    <row r="890" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I890" s="13"/>
     </row>
-    <row r="891" spans="9:9" ht="15.75" customHeight="1">
+    <row r="891" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I891" s="13"/>
     </row>
-    <row r="892" spans="9:9" ht="15.75" customHeight="1">
+    <row r="892" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I892" s="13"/>
     </row>
-    <row r="893" spans="9:9" ht="15.75" customHeight="1">
+    <row r="893" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I893" s="13"/>
     </row>
-    <row r="894" spans="9:9" ht="15.75" customHeight="1">
+    <row r="894" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I894" s="13"/>
     </row>
-    <row r="895" spans="9:9" ht="15.75" customHeight="1">
+    <row r="895" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I895" s="13"/>
     </row>
-    <row r="896" spans="9:9" ht="15.75" customHeight="1">
+    <row r="896" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I896" s="13"/>
     </row>
-    <row r="897" spans="9:9" ht="15.75" customHeight="1">
+    <row r="897" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I897" s="13"/>
     </row>
-    <row r="898" spans="9:9" ht="15.75" customHeight="1">
+    <row r="898" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I898" s="13"/>
     </row>
-    <row r="899" spans="9:9" ht="15.75" customHeight="1">
+    <row r="899" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I899" s="13"/>
     </row>
-    <row r="900" spans="9:9" ht="15.75" customHeight="1">
+    <row r="900" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I900" s="13"/>
     </row>
-    <row r="901" spans="9:9" ht="15.75" customHeight="1">
+    <row r="901" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I901" s="13"/>
     </row>
-    <row r="902" spans="9:9" ht="15.75" customHeight="1">
+    <row r="902" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I902" s="13"/>
     </row>
-    <row r="903" spans="9:9" ht="15.75" customHeight="1">
+    <row r="903" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I903" s="13"/>
     </row>
-    <row r="904" spans="9:9" ht="15.75" customHeight="1">
+    <row r="904" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I904" s="13"/>
     </row>
-    <row r="905" spans="9:9" ht="15.75" customHeight="1">
+    <row r="905" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I905" s="13"/>
     </row>
-    <row r="906" spans="9:9" ht="15.75" customHeight="1">
+    <row r="906" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I906" s="13"/>
     </row>
-    <row r="907" spans="9:9" ht="15.75" customHeight="1">
+    <row r="907" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I907" s="13"/>
     </row>
-    <row r="908" spans="9:9" ht="15.75" customHeight="1">
+    <row r="908" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I908" s="13"/>
     </row>
-    <row r="909" spans="9:9" ht="15.75" customHeight="1">
+    <row r="909" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I909" s="13"/>
     </row>
-    <row r="910" spans="9:9" ht="15.75" customHeight="1">
+    <row r="910" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I910" s="13"/>
     </row>
-    <row r="911" spans="9:9" ht="15.75" customHeight="1">
+    <row r="911" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I911" s="13"/>
     </row>
-    <row r="912" spans="9:9" ht="15.75" customHeight="1">
+    <row r="912" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I912" s="13"/>
     </row>
-    <row r="913" spans="9:9" ht="15.75" customHeight="1">
+    <row r="913" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I913" s="13"/>
     </row>
-    <row r="914" spans="9:9" ht="15.75" customHeight="1">
+    <row r="914" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I914" s="13"/>
     </row>
-    <row r="915" spans="9:9" ht="15.75" customHeight="1">
+    <row r="915" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I915" s="13"/>
     </row>
-    <row r="916" spans="9:9" ht="15.75" customHeight="1">
+    <row r="916" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I916" s="13"/>
     </row>
-    <row r="917" spans="9:9" ht="15.75" customHeight="1">
+    <row r="917" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I917" s="13"/>
     </row>
-    <row r="918" spans="9:9" ht="15.75" customHeight="1">
+    <row r="918" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I918" s="13"/>
     </row>
-    <row r="919" spans="9:9" ht="15.75" customHeight="1">
+    <row r="919" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I919" s="13"/>
     </row>
-    <row r="920" spans="9:9" ht="15.75" customHeight="1">
+    <row r="920" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I920" s="13"/>
     </row>
-    <row r="921" spans="9:9" ht="15.75" customHeight="1">
+    <row r="921" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I921" s="13"/>
     </row>
-    <row r="922" spans="9:9" ht="15.75" customHeight="1">
+    <row r="922" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I922" s="13"/>
     </row>
-    <row r="923" spans="9:9" ht="15.75" customHeight="1">
+    <row r="923" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I923" s="13"/>
     </row>
-    <row r="924" spans="9:9" ht="15.75" customHeight="1">
+    <row r="924" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I924" s="13"/>
     </row>
-    <row r="925" spans="9:9" ht="15.75" customHeight="1">
+    <row r="925" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I925" s="13"/>
     </row>
-    <row r="926" spans="9:9" ht="15.75" customHeight="1">
+    <row r="926" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I926" s="13"/>
     </row>
-    <row r="927" spans="9:9" ht="15.75" customHeight="1">
+    <row r="927" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I927" s="13"/>
     </row>
-    <row r="928" spans="9:9" ht="15.75" customHeight="1">
+    <row r="928" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I928" s="13"/>
     </row>
-    <row r="929" spans="9:9" ht="15.75" customHeight="1">
+    <row r="929" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I929" s="13"/>
     </row>
-    <row r="930" spans="9:9" ht="15.75" customHeight="1">
+    <row r="930" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I930" s="13"/>
     </row>
-    <row r="931" spans="9:9" ht="15.75" customHeight="1">
+    <row r="931" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I931" s="13"/>
     </row>
-    <row r="932" spans="9:9" ht="15.75" customHeight="1">
+    <row r="932" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I932" s="13"/>
     </row>
-    <row r="933" spans="9:9" ht="15.75" customHeight="1">
+    <row r="933" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I933" s="13"/>
     </row>
-    <row r="934" spans="9:9" ht="15.75" customHeight="1">
+    <row r="934" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I934" s="13"/>
     </row>
-    <row r="935" spans="9:9" ht="15.75" customHeight="1">
+    <row r="935" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I935" s="13"/>
     </row>
-    <row r="936" spans="9:9" ht="15.75" customHeight="1">
+    <row r="936" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I936" s="13"/>
     </row>
-    <row r="937" spans="9:9" ht="15.75" customHeight="1">
+    <row r="937" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I937" s="13"/>
     </row>
-    <row r="938" spans="9:9" ht="15.75" customHeight="1">
+    <row r="938" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I938" s="13"/>
     </row>
-    <row r="939" spans="9:9" ht="15.75" customHeight="1">
+    <row r="939" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I939" s="13"/>
     </row>
-    <row r="940" spans="9:9" ht="15.75" customHeight="1">
+    <row r="940" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I940" s="13"/>
     </row>
-    <row r="941" spans="9:9" ht="15.75" customHeight="1">
+    <row r="941" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I941" s="13"/>
     </row>
-    <row r="942" spans="9:9" ht="15.75" customHeight="1">
+    <row r="942" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I942" s="13"/>
     </row>
-    <row r="943" spans="9:9" ht="15.75" customHeight="1">
+    <row r="943" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I943" s="13"/>
     </row>
-    <row r="944" spans="9:9" ht="15.75" customHeight="1">
+    <row r="944" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I944" s="13"/>
     </row>
-    <row r="945" spans="9:9" ht="15.75" customHeight="1">
+    <row r="945" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I945" s="13"/>
     </row>
-    <row r="946" spans="9:9" ht="15.75" customHeight="1">
+    <row r="946" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I946" s="13"/>
     </row>
-    <row r="947" spans="9:9" ht="15.75" customHeight="1">
+    <row r="947" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I947" s="13"/>
     </row>
-    <row r="948" spans="9:9" ht="15.75" customHeight="1">
+    <row r="948" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I948" s="13"/>
     </row>
-    <row r="949" spans="9:9" ht="15.75" customHeight="1">
+    <row r="949" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I949" s="13"/>
     </row>
-    <row r="950" spans="9:9" ht="15.75" customHeight="1">
+    <row r="950" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I950" s="13"/>
     </row>
-    <row r="951" spans="9:9" ht="15.75" customHeight="1">
+    <row r="951" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I951" s="13"/>
     </row>
-    <row r="952" spans="9:9" ht="15.75" customHeight="1">
+    <row r="952" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I952" s="13"/>
     </row>
-    <row r="953" spans="9:9" ht="15.75" customHeight="1">
+    <row r="953" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I953" s="13"/>
     </row>
-    <row r="954" spans="9:9" ht="15.75" customHeight="1">
+    <row r="954" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I954" s="13"/>
     </row>
-    <row r="955" spans="9:9" ht="15.75" customHeight="1">
+    <row r="955" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I955" s="13"/>
     </row>
-    <row r="956" spans="9:9" ht="15.75" customHeight="1">
+    <row r="956" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I956" s="13"/>
     </row>
-    <row r="957" spans="9:9" ht="15.75" customHeight="1">
+    <row r="957" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I957" s="13"/>
     </row>
-    <row r="958" spans="9:9" ht="15.75" customHeight="1">
+    <row r="958" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I958" s="13"/>
     </row>
-    <row r="959" spans="9:9" ht="15.75" customHeight="1">
+    <row r="959" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I959" s="13"/>
     </row>
-    <row r="960" spans="9:9" ht="15.75" customHeight="1">
+    <row r="960" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I960" s="13"/>
     </row>
-    <row r="961" spans="9:9" ht="15.75" customHeight="1">
+    <row r="961" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I961" s="13"/>
     </row>
-    <row r="962" spans="9:9" ht="15.75" customHeight="1">
+    <row r="962" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I962" s="13"/>
     </row>
-    <row r="963" spans="9:9" ht="15.75" customHeight="1">
+    <row r="963" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I963" s="13"/>
     </row>
-    <row r="964" spans="9:9" ht="15.75" customHeight="1">
+    <row r="964" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I964" s="13"/>
     </row>
-    <row r="965" spans="9:9" ht="15.75" customHeight="1">
+    <row r="965" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I965" s="13"/>
     </row>
-    <row r="966" spans="9:9" ht="15.75" customHeight="1">
+    <row r="966" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I966" s="13"/>
     </row>
-    <row r="967" spans="9:9" ht="15.75" customHeight="1">
+    <row r="967" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I967" s="13"/>
     </row>
-    <row r="968" spans="9:9" ht="15.75" customHeight="1">
+    <row r="968" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I968" s="13"/>
     </row>
-    <row r="969" spans="9:9" ht="15.75" customHeight="1">
+    <row r="969" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I969" s="13"/>
     </row>
-    <row r="970" spans="9:9" ht="15.75" customHeight="1">
+    <row r="970" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I970" s="13"/>
     </row>
-    <row r="971" spans="9:9" ht="15.75" customHeight="1">
+    <row r="971" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I971" s="13"/>
     </row>
-    <row r="972" spans="9:9" ht="15.75" customHeight="1">
+    <row r="972" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I972" s="13"/>
     </row>
-    <row r="973" spans="9:9" ht="15.75" customHeight="1">
+    <row r="973" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I973" s="13"/>
     </row>
-    <row r="974" spans="9:9" ht="15.75" customHeight="1">
+    <row r="974" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I974" s="13"/>
     </row>
-    <row r="975" spans="9:9" ht="15.75" customHeight="1">
+    <row r="975" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I975" s="13"/>
     </row>
-    <row r="976" spans="9:9" ht="15.75" customHeight="1">
+    <row r="976" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I976" s="13"/>
     </row>
-    <row r="977" spans="9:9" ht="15.75" customHeight="1">
+    <row r="977" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I977" s="13"/>
     </row>
-    <row r="978" spans="9:9" ht="15.75" customHeight="1">
+    <row r="978" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I978" s="13"/>
     </row>
-    <row r="979" spans="9:9" ht="15.75" customHeight="1">
+    <row r="979" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I979" s="13"/>
     </row>
-    <row r="980" spans="9:9" ht="15.75" customHeight="1">
+    <row r="980" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I980" s="13"/>
     </row>
-    <row r="981" spans="9:9" ht="15.75" customHeight="1">
+    <row r="981" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I981" s="13"/>
     </row>
-    <row r="982" spans="9:9" ht="15.75" customHeight="1">
+    <row r="982" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I982" s="13"/>
     </row>
-    <row r="983" spans="9:9" ht="15.75" customHeight="1">
+    <row r="983" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I983" s="13"/>
     </row>
-    <row r="984" spans="9:9" ht="15.75" customHeight="1">
+    <row r="984" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I984" s="13"/>
     </row>
-    <row r="985" spans="9:9" ht="15.75" customHeight="1">
+    <row r="985" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I985" s="13"/>
     </row>
-    <row r="986" spans="9:9" ht="15.75" customHeight="1">
+    <row r="986" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I986" s="13"/>
     </row>
-    <row r="987" spans="9:9" ht="15.75" customHeight="1">
+    <row r="987" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I987" s="13"/>
     </row>
-    <row r="988" spans="9:9" ht="15.75" customHeight="1">
+    <row r="988" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I988" s="13"/>
     </row>
-    <row r="989" spans="9:9" ht="15.75" customHeight="1">
+    <row r="989" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I989" s="13"/>
     </row>
-    <row r="990" spans="9:9" ht="15.75" customHeight="1">
+    <row r="990" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I990" s="13"/>
     </row>
-    <row r="991" spans="9:9" ht="15.75" customHeight="1">
+    <row r="991" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I991" s="13"/>
     </row>
-    <row r="992" spans="9:9" ht="15.75" customHeight="1">
+    <row r="992" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I992" s="13"/>
     </row>
-    <row r="993" spans="9:9" ht="15.75" customHeight="1">
+    <row r="993" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I993" s="13"/>
     </row>
-    <row r="994" spans="9:9" ht="15.75" customHeight="1">
+    <row r="994" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I994" s="13"/>
     </row>
-    <row r="995" spans="9:9" ht="15.75" customHeight="1">
+    <row r="995" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I995" s="13"/>
     </row>
-    <row r="996" spans="9:9" ht="15.75" customHeight="1">
+    <row r="996" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I996" s="13"/>
     </row>
-    <row r="997" spans="9:9" ht="15.75" customHeight="1">
+    <row r="997" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I997" s="13"/>
     </row>
-    <row r="998" spans="9:9" ht="15.75" customHeight="1">
+    <row r="998" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I998" s="13"/>
     </row>
-    <row r="999" spans="9:9" ht="15.75" customHeight="1">
+    <row r="999" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I999" s="13"/>
     </row>
-    <row r="1000" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1000" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1000" s="13"/>
     </row>
-    <row r="1001" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1001" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1001" s="13"/>
     </row>
-    <row r="1002" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1002" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1002" s="13"/>
     </row>
-    <row r="1003" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1003" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1003" s="13"/>
     </row>
-    <row r="1004" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1004" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1004" s="13"/>
     </row>
-    <row r="1005" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1005" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1005" s="13"/>
     </row>
-    <row r="1006" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1006" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1006" s="13"/>
     </row>
-    <row r="1007" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1007" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1007" s="13"/>
     </row>
-    <row r="1008" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1008" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1008" s="13"/>
     </row>
-    <row r="1009" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1009" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1009" s="13"/>
     </row>
-    <row r="1010" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1010" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1010" s="13"/>
     </row>
-    <row r="1011" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1011" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1011" s="13"/>
     </row>
-    <row r="1012" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1012" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1012" s="13"/>
     </row>
-    <row r="1013" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1013" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1013" s="13"/>
     </row>
-    <row r="1014" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1014" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1014" s="13"/>
     </row>
-    <row r="1015" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1015" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1015" s="13"/>
     </row>
-    <row r="1016" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1016" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1016" s="13"/>
     </row>
-    <row r="1017" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1017" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1017" s="13"/>
     </row>
-    <row r="1018" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1018" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1018" s="13"/>
     </row>
-    <row r="1019" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1019" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1019" s="13"/>
     </row>
-    <row r="1020" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1020" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1020" s="13"/>
     </row>
-    <row r="1021" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1021" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1021" s="13"/>
     </row>
-    <row r="1022" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1022" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1022" s="13"/>
     </row>
-    <row r="1023" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1023" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1023" s="13"/>
     </row>
-    <row r="1024" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1024" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1024" s="13"/>
     </row>
-    <row r="1025" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1025" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1025" s="13"/>
     </row>
-    <row r="1026" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1026" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1026" s="13"/>
     </row>
-    <row r="1027" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1027" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1027" s="13"/>
     </row>
-    <row r="1028" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1028" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1028" s="13"/>
     </row>
-    <row r="1029" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1029" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1029" s="13"/>
     </row>
-    <row r="1030" spans="9:9" ht="15.75" customHeight="1">
+    <row r="1030" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1030" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionado index de pergunta negócio + arrumado colunas
algumas colunas estavam com o tipo não batendo com valor maximo e minimo mencionado, alem de que um indice de uma das tabelas foi colocado como clustered quando já tinha o do PK
</commit_message>
<xml_diff>
--- a/dicionario_tabelas/dicionario.xlsx
+++ b/dicionario_tabelas/dicionario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC do Brunooo\Documents\Github\Sistema-de-Manutencao-de-Veiculos\dicionario_tabelas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\APENAS MEU\Faculdade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFCC2F6-402B-44B6-AFCA-559A00B687F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C6C75C-B636-4E8F-A97B-B7C470E3F0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="186">
   <si>
     <t>Tabela</t>
   </si>
@@ -563,17 +563,39 @@
   </si>
   <si>
     <t>0,01 – 999,99</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>idx_manutencoes_cd_alas</t>
+  </si>
+  <si>
+    <t>idx_manutencoes_cd_status_seguro</t>
+  </si>
+  <si>
+    <t>cd_status_seguro</t>
+  </si>
+  <si>
+    <t>idx_seguros_nm_seguradora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -877,268 +899,284 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1356,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1034"/>
+  <dimension ref="A1:Q1037"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A116" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2104,40 +2142,47 @@
       <c r="Q26" s="67"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="61" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" s="100"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27" s="46"/>
+      <c r="F27" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="101"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="104"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="105"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="103"/>
+      <c r="P27" s="103"/>
+      <c r="Q27" s="103"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="B27" s="62"/>
-      <c r="C27" s="44" t="s">
+      <c r="B28" s="62"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E28" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="63" t="s">
+      <c r="F28" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G27" s="64"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="85"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="62"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2148,14 +2193,14 @@
       <c r="P28" s="4"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="86"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="86"/>
-      <c r="H29" s="86"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="85"/>
+      <c r="E29" s="85"/>
+      <c r="F29" s="85"/>
+      <c r="G29" s="85"/>
+      <c r="H29" s="85"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2184,14 +2229,14 @@
       <c r="P30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="87"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="87"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -2202,38 +2247,29 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="87"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="80" t="s">
+      <c r="B33" s="80" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="K32" s="75" t="s">
-        <v>133</v>
-      </c>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="77"/>
-    </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="80" t="s">
-        <v>42</v>
       </c>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
@@ -2243,10 +2279,10 @@
       <c r="H33" s="60"/>
       <c r="I33" s="2"/>
       <c r="J33" s="29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="75" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="L33" s="76"/>
       <c r="M33" s="76"/>
@@ -2255,268 +2291,258 @@
       <c r="P33" s="76"/>
       <c r="Q33" s="77"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="54"/>
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>42</v>
+      </c>
       <c r="C34" s="54"/>
       <c r="D34" s="54"/>
       <c r="E34" s="54"/>
       <c r="F34" s="54"/>
       <c r="G34" s="54"/>
       <c r="H34" s="60"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="90" t="s">
+      <c r="I34" s="2"/>
+      <c r="J34" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" s="75" t="s">
+        <v>43</v>
+      </c>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="77"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="K34" s="91"/>
-      <c r="L34" s="91"/>
-      <c r="M34" s="91"/>
-      <c r="N34" s="91"/>
-      <c r="O34" s="91"/>
-      <c r="P34" s="91"/>
-      <c r="Q34" s="91"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="91"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="91"/>
+      <c r="P35" s="91"/>
+      <c r="Q35" s="91"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="60"/>
-      <c r="C35" s="33" t="s">
+      <c r="B36" s="60"/>
+      <c r="C36" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H36" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="1" t="s">
+      <c r="I36" s="2"/>
+      <c r="J36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O35" s="29" t="s">
+      <c r="O36" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="P35" s="78" t="s">
+      <c r="P36" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="Q35" s="79"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="96" t="s">
+      <c r="Q36" s="79"/>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="96" t="s">
         <v>44</v>
-      </c>
-      <c r="B36" s="60"/>
-      <c r="C36" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L36" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O36" s="18"/>
-      <c r="P36" s="75" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q36" s="77"/>
-    </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="80" t="s">
-        <v>47</v>
       </c>
       <c r="B37" s="60"/>
       <c r="C37" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="I37" s="2"/>
       <c r="J37" s="5" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>176</v>
+        <v>164</v>
+      </c>
+      <c r="L37" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="M37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N37" s="5"/>
+      <c r="N37" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="O37" s="18"/>
       <c r="P37" s="75" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="Q37" s="77"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="80" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B38" s="60"/>
       <c r="C38" s="10" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="57"/>
+        <v>50</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N38" s="5"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" s="77"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="80" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B39" s="60"/>
       <c r="C39" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="K39" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L39" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="M39" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N39" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="O39" s="98"/>
-      <c r="P39" s="98"/>
-      <c r="Q39" s="98"/>
+      <c r="H39" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="K39" s="55"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="57"/>
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="80" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="B40" s="60"/>
       <c r="C40" s="10" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
-      <c r="H40" s="10" t="s">
-        <v>58</v>
+      <c r="H40" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="43" t="s">
-        <v>150</v>
-      </c>
-      <c r="K40" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L40" s="43"/>
-      <c r="M40" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="N40" s="97" t="s">
-        <v>134</v>
-      </c>
-      <c r="O40" s="97"/>
-      <c r="P40" s="97"/>
-      <c r="Q40" s="97"/>
+      <c r="J40" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L40" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N40" s="98" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40" s="98"/>
+      <c r="P40" s="98"/>
+      <c r="Q40" s="98"/>
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="80" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B41" s="60"/>
       <c r="C41" s="10" t="s">
@@ -2526,24 +2552,26 @@
         <v>57</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43" t="s">
+        <v>150</v>
+      </c>
+      <c r="K41" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="M41" s="50"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="50" t="s">
+        <v>14</v>
+      </c>
       <c r="N41" s="97" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="O41" s="97"/>
       <c r="P41" s="97"/>
@@ -2551,7 +2579,7 @@
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="80" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B42" s="60"/>
       <c r="C42" s="10" t="s">
@@ -2561,91 +2589,106 @@
         <v>57</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I42" s="14"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
+        <v>60</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="K42" s="43"/>
+      <c r="L42" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" s="50"/>
+      <c r="N42" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="O42" s="97"/>
+      <c r="P42" s="97"/>
+      <c r="Q42" s="97"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="80" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B43" s="60"/>
       <c r="C43" s="10" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="I43" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="I43" s="14"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="9"/>
       <c r="M43" s="8"/>
-      <c r="N43" s="31"/>
+      <c r="N43" s="8"/>
       <c r="O43" s="8"/>
       <c r="P43" s="8"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="80" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B44" s="60"/>
       <c r="C44" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>165</v>
+        <v>64</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="G44" s="5"/>
       <c r="H44" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
       <c r="L44" s="9"/>
       <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
+      <c r="N44" s="31"/>
       <c r="O44" s="8"/>
       <c r="P44" s="8"/>
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="54"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="60"/>
+      <c r="A45" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="60"/>
+      <c r="C45" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>66</v>
+      </c>
       <c r="I45" s="2"/>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
@@ -2657,21 +2700,13 @@
     </row>
     <row r="46" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B46" s="60"/>
-      <c r="C46" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="53" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
       <c r="G46" s="54"/>
       <c r="H46" s="60"/>
       <c r="I46" s="2"/>
@@ -2684,22 +2719,24 @@
       <c r="P46" s="8"/>
     </row>
     <row r="47" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="61" t="s">
-        <v>142</v>
-      </c>
-      <c r="B47" s="62"/>
-      <c r="C47" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="F47" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="G47" s="64"/>
-      <c r="H47" s="62"/>
+      <c r="A47" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="60"/>
+      <c r="C47" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="54"/>
+      <c r="H47" s="60"/>
       <c r="I47" s="2"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
@@ -2711,16 +2748,18 @@
     </row>
     <row r="48" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="61" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B48" s="62"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="45" t="s">
+      <c r="C48" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="46"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="46" t="s">
+        <v>14</v>
+      </c>
       <c r="F48" s="63" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G48" s="64"/>
       <c r="H48" s="62"/>
@@ -2734,32 +2773,38 @@
       <c r="P48" s="8"/>
     </row>
     <row r="49" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
+      <c r="A49" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="62"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="46"/>
+      <c r="F49" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="G49" s="64"/>
+      <c r="H49" s="62"/>
       <c r="I49" s="2"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
       <c r="O49" s="8"/>
       <c r="P49" s="8"/>
     </row>
     <row r="50" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="86"/>
-      <c r="B50" s="86"/>
-      <c r="C50" s="86"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86"/>
-      <c r="G50" s="86"/>
-      <c r="H50" s="86"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="85"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="85"/>
+      <c r="F50" s="85"/>
+      <c r="G50" s="85"/>
+      <c r="H50" s="85"/>
       <c r="I50" s="2"/>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
@@ -2788,14 +2833,14 @@
       <c r="P51" s="8"/>
     </row>
     <row r="52" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="87"/>
-      <c r="B52" s="87"/>
-      <c r="C52" s="87"/>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="87"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="86"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="86"/>
       <c r="I52" s="2"/>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
@@ -2806,38 +2851,29 @@
       <c r="P52" s="8"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B53" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="60"/>
+      <c r="A53" s="87"/>
+      <c r="B53" s="87"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
+      <c r="H53" s="87"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="K53" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="L53" s="65"/>
-      <c r="M53" s="65"/>
-      <c r="N53" s="65"/>
-      <c r="O53" s="65"/>
-      <c r="P53" s="65"/>
-      <c r="Q53" s="65"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" s="80" t="s">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="C54" s="54"/>
       <c r="D54" s="54"/>
@@ -2847,10 +2883,10 @@
       <c r="H54" s="60"/>
       <c r="I54" s="2"/>
       <c r="J54" s="20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54" s="65" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="L54" s="65"/>
       <c r="M54" s="65"/>
@@ -2860,10 +2896,12 @@
       <c r="Q54" s="65"/>
     </row>
     <row r="55" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="54"/>
+      <c r="A55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="80" t="s">
+        <v>67</v>
+      </c>
       <c r="C55" s="54"/>
       <c r="D55" s="54"/>
       <c r="E55" s="54"/>
@@ -2871,149 +2909,135 @@
       <c r="G55" s="54"/>
       <c r="H55" s="60"/>
       <c r="I55" s="2"/>
-      <c r="J55" s="74" t="s">
+      <c r="J55" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="K55" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="L55" s="65"/>
+      <c r="M55" s="65"/>
+      <c r="N55" s="65"/>
+      <c r="O55" s="65"/>
+      <c r="P55" s="65"/>
+      <c r="Q55" s="65"/>
+    </row>
+    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="K55" s="74"/>
-      <c r="L55" s="74"/>
-      <c r="M55" s="74"/>
-      <c r="N55" s="74"/>
-      <c r="O55" s="74"/>
-      <c r="P55" s="74"/>
-      <c r="Q55" s="74"/>
-    </row>
-    <row r="56" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="53" t="s">
+      <c r="B56" s="54"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="K56" s="74"/>
+      <c r="L56" s="74"/>
+      <c r="M56" s="74"/>
+      <c r="N56" s="74"/>
+      <c r="O56" s="74"/>
+      <c r="P56" s="74"/>
+      <c r="Q56" s="74"/>
+    </row>
+    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="60"/>
-      <c r="C56" s="33" t="s">
+      <c r="B57" s="60"/>
+      <c r="C57" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="33" t="s">
+      <c r="H57" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I56" s="2"/>
-      <c r="J56" s="20" t="s">
+      <c r="I57" s="2"/>
+      <c r="J57" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K56" s="20" t="s">
+      <c r="K57" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="L56" s="20" t="s">
+      <c r="L57" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M56" s="20" t="s">
+      <c r="M57" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="N56" s="20" t="s">
+      <c r="N57" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="O56" s="20" t="s">
+      <c r="O57" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="P56" s="68" t="s">
+      <c r="P57" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="Q56" s="68"/>
-    </row>
-    <row r="57" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="B57" s="60"/>
-      <c r="C57" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G57" s="5"/>
-      <c r="H57" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="I57" s="2"/>
-      <c r="J57" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="K57" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="L57" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="M57" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N57" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O57" s="21"/>
-      <c r="P57" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q57" s="65"/>
+      <c r="Q57" s="68"/>
     </row>
     <row r="58" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="80" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B58" s="60"/>
       <c r="C58" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G58" s="5"/>
       <c r="H58" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I58" s="3"/>
-      <c r="J58" s="21" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="28" t="s">
+        <v>71</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="L58" s="23" t="s">
-        <v>27</v>
+        <v>164</v>
+      </c>
+      <c r="L58" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="M58" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N58" s="21"/>
+      <c r="N58" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="O58" s="21"/>
       <c r="P58" s="65" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="Q58" s="65"/>
     </row>
     <row r="59" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="80" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B59" s="60"/>
       <c r="C59" s="10" t="s">
@@ -3028,30 +3052,38 @@
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="K59" s="55"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="55"/>
-      <c r="N59" s="55"/>
-      <c r="O59" s="55"/>
-      <c r="P59" s="56"/>
-      <c r="Q59" s="57"/>
+        <v>73</v>
+      </c>
+      <c r="I59" s="3"/>
+      <c r="J59" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K59" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L59" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q59" s="65"/>
     </row>
     <row r="60" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="89" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="59"/>
+      <c r="A60" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="60"/>
       <c r="C60" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>178</v>
+        <v>40</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>13</v>
@@ -3059,107 +3091,108 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I60" s="2"/>
-      <c r="J60" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="K60" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="L60" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="M60" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="N60" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="O60" s="98"/>
-      <c r="P60" s="98"/>
-      <c r="Q60" s="98"/>
+        <v>75</v>
+      </c>
+      <c r="I60" s="4"/>
+      <c r="J60" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="K60" s="55"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="55"/>
+      <c r="N60" s="55"/>
+      <c r="O60" s="55"/>
+      <c r="P60" s="56"/>
+      <c r="Q60" s="57"/>
     </row>
     <row r="61" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" s="60"/>
+      <c r="A61" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61" s="59"/>
       <c r="C61" s="10" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>13</v>
       </c>
       <c r="F61" s="5"/>
-      <c r="G61" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="G61" s="5"/>
       <c r="H61" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I61" s="2"/>
-      <c r="J61" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="K61" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="L61" s="43"/>
-      <c r="M61" s="50" t="s">
-        <v>14</v>
-      </c>
-      <c r="N61" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="O61" s="97"/>
-      <c r="P61" s="97"/>
-      <c r="Q61" s="97"/>
+      <c r="J61" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="K61" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="L61" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="M61" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N61" s="98" t="s">
+        <v>34</v>
+      </c>
+      <c r="O61" s="98"/>
+      <c r="P61" s="98"/>
+      <c r="Q61" s="98"/>
     </row>
     <row r="62" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="88" t="s">
-        <v>80</v>
+      <c r="A62" s="80" t="s">
+        <v>44</v>
       </c>
       <c r="B62" s="60"/>
-      <c r="C62" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>118</v>
+      <c r="C62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="13"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H62" s="13" t="s">
-        <v>82</v>
+      <c r="H62" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="I62" s="2"/>
-      <c r="J62" s="16"/>
-      <c r="K62" s="16"/>
-      <c r="L62" s="16"/>
-      <c r="M62" s="16"/>
-      <c r="N62" s="16"/>
-      <c r="O62" s="16"/>
-      <c r="P62" s="16"/>
+      <c r="J62" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="K62" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L62" s="43"/>
+      <c r="M62" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="N62" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="O62" s="97"/>
+      <c r="P62" s="97"/>
+      <c r="Q62" s="97"/>
     </row>
     <row r="63" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="88" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B63" s="60"/>
-      <c r="C63" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>167</v>
+      <c r="C63" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>13</v>
@@ -3169,7 +3202,7 @@
         <v>14</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="16"/>
@@ -3181,15 +3214,15 @@
       <c r="P63" s="16"/>
     </row>
     <row r="64" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="80" t="s">
-        <v>71</v>
+      <c r="A64" s="88" t="s">
+        <v>83</v>
       </c>
       <c r="B64" s="60"/>
-      <c r="C64" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D64" s="26" t="s">
-        <v>165</v>
+      <c r="C64" s="102" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>13</v>
@@ -3199,9 +3232,9 @@
         <v>14</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I64" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="I64" s="2"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
       <c r="L64" s="16"/>
@@ -3211,16 +3244,26 @@
       <c r="P64" s="16"/>
     </row>
     <row r="65" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" s="54"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="60"/>
+      <c r="A65" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" s="60"/>
+      <c r="C65" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="13"/>
+      <c r="G65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="I65" s="11"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
@@ -3232,21 +3275,13 @@
     </row>
     <row r="66" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B66" s="60"/>
-      <c r="C66" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F66" s="53" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B66" s="54"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="54"/>
+      <c r="F66" s="54"/>
       <c r="G66" s="54"/>
       <c r="H66" s="60"/>
       <c r="I66" s="11"/>
@@ -3259,40 +3294,50 @@
       <c r="P66" s="16"/>
     </row>
     <row r="67" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="63" t="s">
+      <c r="A67" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" s="60"/>
+      <c r="C67" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="54"/>
+      <c r="H67" s="60"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="16"/>
+      <c r="N67" s="16"/>
+      <c r="O67" s="16"/>
+      <c r="P67" s="16"/>
+    </row>
+    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="B67" s="62"/>
-      <c r="C67" s="44" t="s">
+      <c r="B68" s="62"/>
+      <c r="C68" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45" t="s">
+      <c r="D68" s="45"/>
+      <c r="E68" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="63" t="s">
+      <c r="F68" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="G67" s="64"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="36"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
-      <c r="P67" s="15"/>
-    </row>
-    <row r="68" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="85"/>
-      <c r="B68" s="85"/>
-      <c r="C68" s="85"/>
-      <c r="D68" s="85"/>
-      <c r="E68" s="85"/>
-      <c r="F68" s="85"/>
-      <c r="G68" s="85"/>
-      <c r="H68" s="85"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="62"/>
       <c r="I68" s="11"/>
       <c r="J68" s="15"/>
       <c r="K68" s="15"/>
@@ -3303,18 +3348,18 @@
       <c r="P68" s="15"/>
     </row>
     <row r="69" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="86"/>
-      <c r="B69" s="86"/>
-      <c r="C69" s="86"/>
-      <c r="D69" s="86"/>
-      <c r="E69" s="86"/>
-      <c r="F69" s="86"/>
-      <c r="G69" s="86"/>
-      <c r="H69" s="86"/>
+      <c r="A69" s="85"/>
+      <c r="B69" s="85"/>
+      <c r="C69" s="85"/>
+      <c r="D69" s="85"/>
+      <c r="E69" s="85"/>
+      <c r="F69" s="85"/>
+      <c r="G69" s="85"/>
+      <c r="H69" s="85"/>
       <c r="I69" s="11"/>
       <c r="J69" s="15"/>
       <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
+      <c r="L69" s="36"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
       <c r="O69" s="15"/>
@@ -3339,51 +3384,47 @@
       <c r="P70" s="15"/>
     </row>
     <row r="71" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="87"/>
-      <c r="B71" s="87"/>
-      <c r="C71" s="87"/>
-      <c r="D71" s="87"/>
-      <c r="E71" s="87"/>
-      <c r="F71" s="87"/>
-      <c r="G71" s="87"/>
-      <c r="H71" s="87"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="12"/>
-      <c r="K71" s="12"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="12"/>
+      <c r="A71" s="86"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
+      <c r="G71" s="86"/>
+      <c r="H71" s="86"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
     </row>
     <row r="72" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="80" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="60"/>
+      <c r="A72" s="87"/>
+      <c r="B72" s="87"/>
+      <c r="C72" s="87"/>
+      <c r="D72" s="87"/>
+      <c r="E72" s="87"/>
+      <c r="F72" s="87"/>
+      <c r="G72" s="87"/>
+      <c r="H72" s="87"/>
       <c r="I72" s="14"/>
-      <c r="J72" s="2"/>
-      <c r="K72" s="2"/>
-      <c r="L72" s="2"/>
-      <c r="M72" s="2"/>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" s="2"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
     </row>
     <row r="73" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B73" s="80" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C73" s="54"/>
       <c r="D73" s="54"/>
@@ -3401,107 +3442,101 @@
       <c r="P73" s="2"/>
     </row>
     <row r="74" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="54"/>
+      <c r="A74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="80" t="s">
+        <v>86</v>
+      </c>
       <c r="C74" s="54"/>
       <c r="D74" s="54"/>
       <c r="E74" s="54"/>
       <c r="F74" s="54"/>
       <c r="G74" s="54"/>
       <c r="H74" s="60"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="3"/>
-      <c r="P74" s="3"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+      <c r="N74" s="2"/>
+      <c r="O74" s="2"/>
+      <c r="P74" s="2"/>
     </row>
     <row r="75" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="53" t="s">
+      <c r="A75" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="60"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+    </row>
+    <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B75" s="60"/>
-      <c r="C75" s="33" t="s">
+      <c r="B76" s="60"/>
+      <c r="C76" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H75" s="33" t="s">
+      <c r="H76" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I75" s="2"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="32"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-    </row>
-    <row r="76" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B76" s="60"/>
-      <c r="C76" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G76" s="5"/>
-      <c r="H76" s="10" t="s">
-        <v>88</v>
-      </c>
       <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
-      <c r="K76" s="2"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2"/>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="32"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
     </row>
     <row r="77" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="80" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B77" s="60"/>
       <c r="C77" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>18</v>
+        <v>164</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G77" s="5"/>
-      <c r="H77" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="I77" s="3"/>
+      <c r="H77" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -3512,24 +3547,24 @@
     </row>
     <row r="78" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="80" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="B78" s="60"/>
       <c r="C78" s="10" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
-      <c r="H78" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="I78" s="4"/>
+      <c r="H78" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="I78" s="3"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
@@ -3539,42 +3574,42 @@
       <c r="P78" s="2"/>
     </row>
     <row r="79" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B79" s="54"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54"/>
-      <c r="F79" s="54"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="60"/>
-      <c r="I79" s="2"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
+      <c r="A79" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79" s="60"/>
+      <c r="C79" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="I79" s="4"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
     </row>
     <row r="80" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B80" s="60"/>
-      <c r="C80" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F80" s="53" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B80" s="54"/>
+      <c r="C80" s="54"/>
+      <c r="D80" s="54"/>
+      <c r="E80" s="54"/>
+      <c r="F80" s="54"/>
       <c r="G80" s="54"/>
       <c r="H80" s="60"/>
       <c r="I80" s="2"/>
@@ -3587,22 +3622,24 @@
       <c r="P80" s="4"/>
     </row>
     <row r="81" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="B81" s="62"/>
-      <c r="C81" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G81" s="64"/>
-      <c r="H81" s="62"/>
+      <c r="A81" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B81" s="60"/>
+      <c r="C81" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F81" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G81" s="54"/>
+      <c r="H81" s="60"/>
       <c r="I81" s="2"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
@@ -3613,32 +3650,40 @@
       <c r="P81" s="4"/>
     </row>
     <row r="82" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="85"/>
-      <c r="B82" s="85"/>
-      <c r="C82" s="85"/>
-      <c r="D82" s="85"/>
-      <c r="E82" s="85"/>
-      <c r="F82" s="85"/>
-      <c r="G82" s="85"/>
-      <c r="H82" s="85"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
+      <c r="A82" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="62"/>
+      <c r="C82" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="G82" s="64"/>
+      <c r="H82" s="62"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="4"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
     </row>
     <row r="83" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="86"/>
-      <c r="B83" s="86"/>
-      <c r="C83" s="86"/>
-      <c r="D83" s="86"/>
-      <c r="E83" s="86"/>
-      <c r="F83" s="86"/>
-      <c r="G83" s="86"/>
-      <c r="H83" s="86"/>
+      <c r="A83" s="85"/>
+      <c r="B83" s="85"/>
+      <c r="C83" s="85"/>
+      <c r="D83" s="85"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="85"/>
+      <c r="H83" s="85"/>
       <c r="I83" s="4"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -3667,56 +3712,47 @@
       <c r="P84" s="2"/>
     </row>
     <row r="85" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="87"/>
-      <c r="B85" s="87"/>
-      <c r="C85" s="87"/>
-      <c r="D85" s="87"/>
-      <c r="E85" s="87"/>
-      <c r="F85" s="87"/>
-      <c r="G85" s="87"/>
-      <c r="H85" s="87"/>
+      <c r="A85" s="86"/>
+      <c r="B85" s="86"/>
+      <c r="C85" s="86"/>
+      <c r="D85" s="86"/>
+      <c r="E85" s="86"/>
+      <c r="F85" s="86"/>
+      <c r="G85" s="86"/>
+      <c r="H85" s="86"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="12"/>
-      <c r="K85" s="12"/>
-      <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
-      <c r="O85" s="12"/>
-      <c r="P85" s="12"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2"/>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" s="2"/>
     </row>
     <row r="86" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="C86" s="54"/>
-      <c r="D86" s="54"/>
-      <c r="E86" s="54"/>
-      <c r="F86" s="54"/>
-      <c r="G86" s="54"/>
-      <c r="H86" s="60"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="K86" s="70" t="s">
-        <v>136</v>
-      </c>
-      <c r="L86" s="70"/>
-      <c r="M86" s="70"/>
-      <c r="N86" s="70"/>
-      <c r="O86" s="70"/>
-      <c r="P86" s="70"/>
-      <c r="Q86" s="70"/>
+      <c r="A86" s="87"/>
+      <c r="B86" s="87"/>
+      <c r="C86" s="87"/>
+      <c r="D86" s="87"/>
+      <c r="E86" s="87"/>
+      <c r="F86" s="87"/>
+      <c r="G86" s="87"/>
+      <c r="H86" s="87"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="12"/>
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="12"/>
+      <c r="P86" s="12"/>
     </row>
     <row r="87" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B87" s="80" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C87" s="54"/>
       <c r="D87" s="54"/>
@@ -3726,10 +3762,10 @@
       <c r="H87" s="60"/>
       <c r="I87" s="2"/>
       <c r="J87" s="25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K87" s="70" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="L87" s="70"/>
       <c r="M87" s="70"/>
@@ -3739,169 +3775,155 @@
       <c r="Q87" s="70"/>
     </row>
     <row r="88" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88" s="54"/>
+      <c r="A88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="80" t="s">
+        <v>91</v>
+      </c>
       <c r="C88" s="54"/>
       <c r="D88" s="54"/>
       <c r="E88" s="54"/>
       <c r="F88" s="54"/>
       <c r="G88" s="54"/>
       <c r="H88" s="60"/>
-      <c r="I88" s="12"/>
-      <c r="J88" s="71" t="s">
+      <c r="I88" s="2"/>
+      <c r="J88" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K88" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="L88" s="70"/>
+      <c r="M88" s="70"/>
+      <c r="N88" s="70"/>
+      <c r="O88" s="70"/>
+      <c r="P88" s="70"/>
+      <c r="Q88" s="70"/>
+    </row>
+    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="K88" s="71"/>
-      <c r="L88" s="71"/>
-      <c r="M88" s="71"/>
-      <c r="N88" s="71"/>
-      <c r="O88" s="71"/>
-      <c r="P88" s="71"/>
-      <c r="Q88" s="71"/>
-    </row>
-    <row r="89" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="53" t="s">
+      <c r="B89" s="54"/>
+      <c r="C89" s="54"/>
+      <c r="D89" s="54"/>
+      <c r="E89" s="54"/>
+      <c r="F89" s="54"/>
+      <c r="G89" s="54"/>
+      <c r="H89" s="60"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="K89" s="71"/>
+      <c r="L89" s="71"/>
+      <c r="M89" s="71"/>
+      <c r="N89" s="71"/>
+      <c r="O89" s="71"/>
+      <c r="P89" s="71"/>
+      <c r="Q89" s="71"/>
+    </row>
+    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B89" s="60"/>
-      <c r="C89" s="33" t="s">
+      <c r="B90" s="60"/>
+      <c r="C90" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G89" s="1" t="s">
+      <c r="G90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H89" s="33" t="s">
+      <c r="H90" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="I89" s="2"/>
-      <c r="J89" s="25" t="s">
+      <c r="I90" s="2"/>
+      <c r="J90" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K89" s="25" t="s">
+      <c r="K90" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="L89" s="25" t="s">
+      <c r="L90" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M89" s="25" t="s">
+      <c r="M90" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N89" s="25" t="s">
+      <c r="N90" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="O89" s="25" t="s">
+      <c r="O90" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="P89" s="83" t="s">
+      <c r="P90" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="Q89" s="83"/>
-    </row>
-    <row r="90" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="B90" s="60"/>
-      <c r="C90" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G90" s="5"/>
-      <c r="H90" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="I90" s="2"/>
-      <c r="J90" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="K90" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="L90" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="M90" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="N90" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="O90" s="26"/>
-      <c r="P90" s="84" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q90" s="84"/>
+      <c r="Q90" s="83"/>
     </row>
     <row r="91" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="80" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B91" s="60"/>
       <c r="C91" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>118</v>
+        <v>11</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F91" s="5"/>
-      <c r="G91" s="5" t="s">
+      <c r="F91" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H91" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I91" s="3"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="I91" s="2"/>
       <c r="J91" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K91" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="L91" s="27" t="s">
-        <v>168</v>
+        <v>137</v>
+      </c>
+      <c r="K91" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="L91" s="26" t="s">
+        <v>165</v>
       </c>
       <c r="M91" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="N91" s="26"/>
+      <c r="N91" s="26" t="s">
+        <v>14</v>
+      </c>
       <c r="O91" s="26"/>
       <c r="P91" s="84" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="Q91" s="84"/>
     </row>
     <row r="92" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="80" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B92" s="60"/>
       <c r="C92" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>12</v>
+        <v>81</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>13</v>
@@ -3910,31 +3932,39 @@
       <c r="G92" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H92" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I92" s="4"/>
-      <c r="J92" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="K92" s="54"/>
-      <c r="L92" s="54"/>
-      <c r="M92" s="54"/>
-      <c r="N92" s="55"/>
-      <c r="O92" s="55"/>
-      <c r="P92" s="56"/>
-      <c r="Q92" s="57"/>
+      <c r="H92" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K92" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="L92" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="M92" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="N92" s="26"/>
+      <c r="O92" s="26"/>
+      <c r="P92" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q92" s="84"/>
     </row>
     <row r="93" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="80" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="B93" s="60"/>
-      <c r="C93" s="10" t="s">
-        <v>139</v>
+      <c r="C93" s="42" t="s">
+        <v>11</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>167</v>
+        <v>12</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>13</v>
@@ -3944,38 +3974,30 @@
         <v>14</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I93" s="2"/>
-      <c r="J93" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M93" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="N93" s="98" t="s">
-        <v>34</v>
-      </c>
-      <c r="O93" s="98"/>
-      <c r="P93" s="98"/>
-      <c r="Q93" s="98"/>
+        <v>45</v>
+      </c>
+      <c r="I93" s="4"/>
+      <c r="J93" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="K93" s="54"/>
+      <c r="L93" s="54"/>
+      <c r="M93" s="54"/>
+      <c r="N93" s="55"/>
+      <c r="O93" s="55"/>
+      <c r="P93" s="56"/>
+      <c r="Q93" s="57"/>
     </row>
     <row r="94" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="80" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B94" s="60"/>
       <c r="C94" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D94" s="26" t="s">
-        <v>165</v>
+        <v>139</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>13</v>
@@ -3985,74 +4007,85 @@
         <v>14</v>
       </c>
       <c r="H94" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I94" s="2"/>
+      <c r="J94" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L94" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M94" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N94" s="98" t="s">
+        <v>34</v>
+      </c>
+      <c r="O94" s="98"/>
+      <c r="P94" s="98"/>
+      <c r="Q94" s="98"/>
+    </row>
+    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" s="60"/>
+      <c r="C95" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H95" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="I94" s="2"/>
-      <c r="J94" s="47" t="s">
+      <c r="I95" s="2"/>
+      <c r="J95" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="K94" s="45" t="s">
+      <c r="K95" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="L94" s="45"/>
-      <c r="M94" s="47" t="s">
+      <c r="L95" s="45"/>
+      <c r="M95" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="N94" s="97" t="s">
+      <c r="N95" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="O94" s="97"/>
-      <c r="P94" s="97"/>
-      <c r="Q94" s="97"/>
-    </row>
-    <row r="95" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="18" t="s">
+      <c r="O95" s="97"/>
+      <c r="P95" s="97"/>
+      <c r="Q95" s="97"/>
+    </row>
+    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B95" s="17"/>
-      <c r="C95" s="10" t="s">
+      <c r="B96" s="17"/>
+      <c r="C96" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D96" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F95" s="5"/>
-      <c r="G95" s="5"/>
-      <c r="H95" s="10" t="s">
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="10" t="s">
         <v>125</v>
-      </c>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
-      <c r="M95" s="2"/>
-      <c r="N95" s="2"/>
-      <c r="O95" s="2"/>
-      <c r="P95" s="2"/>
-    </row>
-    <row r="96" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B96" s="60"/>
-      <c r="C96" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="D96" s="26" t="s">
-        <v>165</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H96" s="10" t="s">
-        <v>126</v>
       </c>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
@@ -4063,685 +4096,740 @@
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
     </row>
-    <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="53" t="s">
+    <row r="97" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B97" s="60"/>
+      <c r="C97" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D97" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="2"/>
+      <c r="P97" s="2"/>
+    </row>
+    <row r="98" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B97" s="54"/>
-      <c r="C97" s="54"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="54"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="60"/>
-      <c r="I97" s="2"/>
-    </row>
-    <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B98" s="60"/>
-      <c r="C98" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F98" s="53" t="s">
-        <v>34</v>
-      </c>
+      <c r="B98" s="54"/>
+      <c r="C98" s="54"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="54"/>
+      <c r="F98" s="54"/>
       <c r="G98" s="54"/>
       <c r="H98" s="60"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="63" t="s">
+    <row r="99" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B99" s="60"/>
+      <c r="C99" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F99" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G99" s="54"/>
+      <c r="H99" s="60"/>
+      <c r="I99" s="2"/>
+    </row>
+    <row r="100" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="B99" s="62"/>
-      <c r="C99" s="44" t="s">
+      <c r="B100" s="62"/>
+      <c r="C100" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D99" s="45"/>
-      <c r="E99" s="45" t="s">
+      <c r="D100" s="45"/>
+      <c r="E100" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F99" s="63" t="s">
+      <c r="F100" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="G99" s="64"/>
-      <c r="H99" s="62"/>
-      <c r="I99" s="2"/>
-    </row>
-    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="81" t="s">
+      <c r="G100" s="64"/>
+      <c r="H100" s="62"/>
+      <c r="I100" s="2"/>
+    </row>
+    <row r="101" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="B101" s="100"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E101" s="45"/>
+      <c r="F101" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="G101" s="101"/>
+      <c r="H101" s="100"/>
+      <c r="I101" s="2"/>
+    </row>
+    <row r="102" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B102" s="100"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="E102" s="45"/>
+      <c r="F102" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="G102" s="101"/>
+      <c r="H102" s="100"/>
+      <c r="I102" s="2"/>
+    </row>
+    <row r="103" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="81" t="s">
         <v>153</v>
       </c>
-      <c r="B100" s="60"/>
-      <c r="C100" s="37"/>
-      <c r="D100" s="7" t="s">
+      <c r="B103" s="60"/>
+      <c r="C103" s="37"/>
+      <c r="D103" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E100" s="7"/>
-      <c r="F100" s="81" t="s">
+      <c r="E103" s="7"/>
+      <c r="F103" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="G100" s="54"/>
-      <c r="H100" s="60"/>
-      <c r="I100" s="2"/>
-    </row>
-    <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="81" t="s">
+      <c r="G103" s="54"/>
+      <c r="H103" s="60"/>
+      <c r="I103" s="2"/>
+    </row>
+    <row r="104" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="B101" s="60"/>
-      <c r="C101" s="37"/>
-      <c r="D101" s="7" t="s">
+      <c r="B104" s="60"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="7"/>
-      <c r="F101" s="81" t="s">
+      <c r="E104" s="7"/>
+      <c r="F104" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="G101" s="54"/>
-      <c r="H101" s="60"/>
-      <c r="I101" s="2"/>
-    </row>
-    <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="81" t="s">
+      <c r="G104" s="54"/>
+      <c r="H104" s="60"/>
+      <c r="I104" s="2"/>
+    </row>
+    <row r="105" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="81" t="s">
         <v>155</v>
       </c>
-      <c r="B102" s="60"/>
-      <c r="C102" s="37"/>
-      <c r="D102" s="7" t="s">
+      <c r="B105" s="60"/>
+      <c r="C105" s="37"/>
+      <c r="D105" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E102" s="7"/>
-      <c r="F102" s="81" t="s">
+      <c r="E105" s="7"/>
+      <c r="F105" s="81" t="s">
         <v>124</v>
       </c>
-      <c r="G102" s="54"/>
-      <c r="H102" s="60"/>
-      <c r="I102" s="4"/>
-    </row>
-    <row r="103" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="92"/>
-      <c r="B103" s="85"/>
-      <c r="C103" s="85"/>
-      <c r="D103" s="85"/>
-      <c r="E103" s="85"/>
-      <c r="F103" s="85"/>
-      <c r="G103" s="85"/>
-      <c r="H103" s="85"/>
-      <c r="I103" s="4"/>
-    </row>
-    <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="93"/>
-      <c r="B104" s="86"/>
-      <c r="C104" s="86"/>
-      <c r="D104" s="86"/>
-      <c r="E104" s="86"/>
-      <c r="F104" s="86"/>
-      <c r="G104" s="86"/>
-      <c r="H104" s="86"/>
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="93"/>
-      <c r="B105" s="86"/>
-      <c r="C105" s="86"/>
-      <c r="D105" s="86"/>
-      <c r="E105" s="86"/>
-      <c r="F105" s="86"/>
-      <c r="G105" s="86"/>
-      <c r="H105" s="86"/>
+      <c r="G105" s="54"/>
+      <c r="H105" s="60"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="94"/>
-      <c r="B106" s="87"/>
-      <c r="C106" s="87"/>
-      <c r="D106" s="87"/>
-      <c r="E106" s="87"/>
-      <c r="F106" s="87"/>
-      <c r="G106" s="87"/>
-      <c r="H106" s="87"/>
+    <row r="106" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="92"/>
+      <c r="B106" s="85"/>
+      <c r="C106" s="85"/>
+      <c r="D106" s="85"/>
+      <c r="E106" s="85"/>
+      <c r="F106" s="85"/>
+      <c r="G106" s="85"/>
+      <c r="H106" s="85"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="93"/>
+      <c r="B107" s="86"/>
+      <c r="C107" s="86"/>
+      <c r="D107" s="86"/>
+      <c r="E107" s="86"/>
+      <c r="F107" s="86"/>
+      <c r="G107" s="86"/>
+      <c r="H107" s="86"/>
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="93"/>
+      <c r="B108" s="86"/>
+      <c r="C108" s="86"/>
+      <c r="D108" s="86"/>
+      <c r="E108" s="86"/>
+      <c r="F108" s="86"/>
+      <c r="G108" s="86"/>
+      <c r="H108" s="86"/>
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="94"/>
+      <c r="B109" s="87"/>
+      <c r="C109" s="87"/>
+      <c r="D109" s="87"/>
+      <c r="E109" s="87"/>
+      <c r="F109" s="87"/>
+      <c r="G109" s="87"/>
+      <c r="H109" s="87"/>
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B107" s="80" t="s">
+      <c r="B110" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C107" s="54"/>
-      <c r="D107" s="54"/>
-      <c r="E107" s="54"/>
-      <c r="F107" s="54"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="60"/>
-      <c r="I107" s="2"/>
-    </row>
-    <row r="108" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="C110" s="54"/>
+      <c r="D110" s="54"/>
+      <c r="E110" s="54"/>
+      <c r="F110" s="54"/>
+      <c r="G110" s="54"/>
+      <c r="H110" s="60"/>
+      <c r="I110" s="2"/>
+    </row>
+    <row r="111" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B108" s="80" t="s">
+      <c r="B111" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="C108" s="54"/>
-      <c r="D108" s="54"/>
-      <c r="E108" s="54"/>
-      <c r="F108" s="54"/>
-      <c r="G108" s="54"/>
-      <c r="H108" s="60"/>
-      <c r="I108" s="2"/>
-    </row>
-    <row r="109" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="82" t="s">
+      <c r="C111" s="54"/>
+      <c r="D111" s="54"/>
+      <c r="E111" s="54"/>
+      <c r="F111" s="54"/>
+      <c r="G111" s="54"/>
+      <c r="H111" s="60"/>
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B109" s="54"/>
-      <c r="C109" s="54"/>
-      <c r="D109" s="54"/>
-      <c r="E109" s="54"/>
-      <c r="F109" s="54"/>
-      <c r="G109" s="54"/>
-      <c r="H109" s="60"/>
-      <c r="I109" s="2"/>
-    </row>
-    <row r="110" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="B110" s="60"/>
-      <c r="C110" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H110" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="I110" s="2"/>
-    </row>
-    <row r="111" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="B111" s="60"/>
-      <c r="C111" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G111" s="5"/>
-      <c r="H111" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="I111" s="2"/>
-    </row>
-    <row r="112" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="B112" s="60"/>
-      <c r="C112" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
-      <c r="H112" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="I112" s="3"/>
+      <c r="B112" s="54"/>
+      <c r="C112" s="54"/>
+      <c r="D112" s="54"/>
+      <c r="E112" s="54"/>
+      <c r="F112" s="54"/>
+      <c r="G112" s="54"/>
+      <c r="H112" s="60"/>
+      <c r="I112" s="2"/>
     </row>
     <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113" s="60"/>
+      <c r="C113" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H113" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I113" s="2"/>
+    </row>
+    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="80" t="s">
+        <v>93</v>
+      </c>
+      <c r="B114" s="60"/>
+      <c r="C114" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G114" s="5"/>
+      <c r="H114" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I114" s="2"/>
+    </row>
+    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B115" s="60"/>
+      <c r="C115" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I115" s="3"/>
+    </row>
+    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B113" s="54"/>
-      <c r="C113" s="54"/>
-      <c r="D113" s="54"/>
-      <c r="E113" s="54"/>
-      <c r="F113" s="54"/>
-      <c r="G113" s="54"/>
-      <c r="H113" s="60"/>
-      <c r="I113" s="4"/>
-      <c r="J113" s="19"/>
-      <c r="K113" s="19"/>
-    </row>
-    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B114" s="60"/>
-      <c r="C114" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F114" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="G114" s="54"/>
-      <c r="H114" s="60"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="19"/>
-      <c r="K114" s="19"/>
-    </row>
-    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="63" t="s">
-        <v>146</v>
-      </c>
-      <c r="B115" s="62"/>
-      <c r="C115" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" s="45"/>
-      <c r="E115" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="F115" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="G115" s="64"/>
-      <c r="H115" s="62"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="19"/>
-      <c r="K115" s="19"/>
-    </row>
-    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="63" t="s">
-        <v>147</v>
-      </c>
-      <c r="B116" s="62"/>
-      <c r="C116" s="44"/>
-      <c r="D116" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="E116" s="45"/>
-      <c r="F116" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="G116" s="64"/>
-      <c r="H116" s="62"/>
+      <c r="B116" s="54"/>
+      <c r="C116" s="54"/>
+      <c r="D116" s="54"/>
+      <c r="E116" s="54"/>
+      <c r="F116" s="54"/>
+      <c r="G116" s="54"/>
+      <c r="H116" s="60"/>
       <c r="I116" s="4"/>
       <c r="J116" s="19"/>
       <c r="K116" s="19"/>
     </row>
     <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="85"/>
-      <c r="B117" s="85"/>
-      <c r="C117" s="85"/>
-      <c r="D117" s="85"/>
-      <c r="E117" s="85"/>
-      <c r="F117" s="85"/>
-      <c r="G117" s="85"/>
-      <c r="H117" s="85"/>
-      <c r="I117" s="4"/>
+      <c r="A117" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B117" s="60"/>
+      <c r="C117" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F117" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G117" s="54"/>
+      <c r="H117" s="60"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="19"/>
     </row>
     <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="86"/>
-      <c r="B118" s="86"/>
-      <c r="C118" s="86"/>
-      <c r="D118" s="86"/>
-      <c r="E118" s="86"/>
-      <c r="F118" s="86"/>
-      <c r="G118" s="86"/>
-      <c r="H118" s="86"/>
-      <c r="I118" s="4"/>
+      <c r="A118" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118" s="62"/>
+      <c r="C118" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="45"/>
+      <c r="E118" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="G118" s="64"/>
+      <c r="H118" s="62"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="19"/>
     </row>
     <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="86"/>
-      <c r="B119" s="86"/>
-      <c r="C119" s="86"/>
-      <c r="D119" s="86"/>
-      <c r="E119" s="86"/>
-      <c r="F119" s="86"/>
-      <c r="G119" s="86"/>
-      <c r="H119" s="86"/>
+      <c r="A119" s="63" t="s">
+        <v>147</v>
+      </c>
+      <c r="B119" s="62"/>
+      <c r="C119" s="44"/>
+      <c r="D119" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E119" s="45"/>
+      <c r="F119" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="G119" s="64"/>
+      <c r="H119" s="62"/>
       <c r="I119" s="4"/>
+      <c r="J119" s="19"/>
+      <c r="K119" s="19"/>
     </row>
     <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="95"/>
-      <c r="B120" s="95"/>
-      <c r="C120" s="95"/>
-      <c r="D120" s="95"/>
-      <c r="E120" s="95"/>
-      <c r="F120" s="95"/>
-      <c r="G120" s="95"/>
-      <c r="H120" s="95"/>
+      <c r="A120" s="85"/>
+      <c r="B120" s="85"/>
+      <c r="C120" s="85"/>
+      <c r="D120" s="85"/>
+      <c r="E120" s="85"/>
+      <c r="F120" s="85"/>
+      <c r="G120" s="85"/>
+      <c r="H120" s="85"/>
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="20" t="s">
+      <c r="A121" s="86"/>
+      <c r="B121" s="86"/>
+      <c r="C121" s="86"/>
+      <c r="D121" s="86"/>
+      <c r="E121" s="86"/>
+      <c r="F121" s="86"/>
+      <c r="G121" s="86"/>
+      <c r="H121" s="86"/>
+      <c r="I121" s="4"/>
+    </row>
+    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="86"/>
+      <c r="B122" s="86"/>
+      <c r="C122" s="86"/>
+      <c r="D122" s="86"/>
+      <c r="E122" s="86"/>
+      <c r="F122" s="86"/>
+      <c r="G122" s="86"/>
+      <c r="H122" s="86"/>
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="95"/>
+      <c r="B123" s="95"/>
+      <c r="C123" s="95"/>
+      <c r="D123" s="95"/>
+      <c r="E123" s="95"/>
+      <c r="F123" s="95"/>
+      <c r="G123" s="95"/>
+      <c r="H123" s="95"/>
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B121" s="65" t="s">
+      <c r="B124" s="65" t="s">
         <v>122</v>
       </c>
-      <c r="C121" s="66" t="s">
+      <c r="C124" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="D121" s="66"/>
-      <c r="E121" s="66"/>
-      <c r="F121" s="66"/>
-      <c r="G121" s="66"/>
-      <c r="H121" s="66"/>
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
+      <c r="D124" s="66"/>
+      <c r="E124" s="66"/>
+      <c r="F124" s="66"/>
+      <c r="G124" s="66"/>
+      <c r="H124" s="66"/>
+      <c r="I124" s="2"/>
+    </row>
+    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B122" s="65" t="s">
+      <c r="B125" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="C122" s="66"/>
-      <c r="D122" s="66"/>
-      <c r="E122" s="66"/>
-      <c r="F122" s="66"/>
-      <c r="G122" s="66"/>
-      <c r="H122" s="66"/>
-      <c r="I122" s="2"/>
-      <c r="K122" s="40"/>
-    </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="74" t="s">
+      <c r="C125" s="66"/>
+      <c r="D125" s="66"/>
+      <c r="E125" s="66"/>
+      <c r="F125" s="66"/>
+      <c r="G125" s="66"/>
+      <c r="H125" s="66"/>
+      <c r="I125" s="2"/>
+      <c r="K125" s="40"/>
+    </row>
+    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B123" s="66"/>
-      <c r="C123" s="66"/>
-      <c r="D123" s="66"/>
-      <c r="E123" s="66"/>
-      <c r="F123" s="66"/>
-      <c r="G123" s="66"/>
-      <c r="H123" s="66"/>
-      <c r="I123" s="12"/>
-    </row>
-    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="68" t="s">
+      <c r="B126" s="66"/>
+      <c r="C126" s="66"/>
+      <c r="D126" s="66"/>
+      <c r="E126" s="66"/>
+      <c r="F126" s="66"/>
+      <c r="G126" s="66"/>
+      <c r="H126" s="66"/>
+      <c r="I126" s="12"/>
+    </row>
+    <row r="127" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="B124" s="66"/>
-      <c r="C124" s="34" t="s">
+      <c r="B127" s="66"/>
+      <c r="C127" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D124" s="20" t="s">
+      <c r="D127" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E124" s="20" t="s">
+      <c r="E127" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F124" s="20" t="s">
+      <c r="F127" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G124" s="20" t="s">
+      <c r="G127" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H124" s="34" t="s">
+      <c r="H127" s="34" t="s">
         <v>1</v>
-      </c>
-      <c r="I124" s="19"/>
-    </row>
-    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="B125" s="66"/>
-      <c r="C125" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D125" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="E125" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F125" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G125" s="21"/>
-      <c r="H125" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="I125" s="19"/>
-    </row>
-    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="B126" s="66"/>
-      <c r="C126" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D126" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E126" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F126" s="21"/>
-      <c r="G126" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="H126" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="I126" s="19"/>
-    </row>
-    <row r="127" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="B127" s="66"/>
-      <c r="C127" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D127" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E127" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F127" s="21"/>
-      <c r="G127" s="21"/>
-      <c r="H127" s="35" t="s">
-        <v>112</v>
       </c>
       <c r="I127" s="19"/>
     </row>
     <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="65" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B128" s="66"/>
       <c r="C128" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D128" s="23" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="D128" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="E128" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F128" s="21"/>
+      <c r="F128" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="G128" s="21"/>
       <c r="H128" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I128" s="19"/>
+    </row>
+    <row r="129" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" s="66"/>
+      <c r="C129" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E129" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" s="21"/>
+      <c r="G129" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H129" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="I129" s="19"/>
+    </row>
+    <row r="130" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="B130" s="66"/>
+      <c r="C130" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D130" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E130" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F130" s="21"/>
+      <c r="G130" s="21"/>
+      <c r="H130" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="I130" s="19"/>
+    </row>
+    <row r="131" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="B131" s="66"/>
+      <c r="C131" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D131" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E131" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F131" s="21"/>
+      <c r="G131" s="21"/>
+      <c r="H131" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="I128" s="19"/>
-    </row>
-    <row r="129" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="67" t="s">
+      <c r="I131" s="19"/>
+    </row>
+    <row r="132" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="67" t="s">
         <v>108</v>
       </c>
-      <c r="B129" s="66"/>
-      <c r="C129" s="39" t="s">
+      <c r="B132" s="66"/>
+      <c r="C132" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="D129" s="24" t="s">
+      <c r="D132" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E129" s="24" t="s">
+      <c r="E132" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F129" s="21"/>
-      <c r="G129" s="21"/>
-      <c r="H129" s="35" t="s">
+      <c r="F132" s="21"/>
+      <c r="G132" s="21"/>
+      <c r="H132" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="I129" s="19"/>
-    </row>
-    <row r="130" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="67" t="s">
+      <c r="I132" s="19"/>
+    </row>
+    <row r="133" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="B130" s="66"/>
-      <c r="C130" s="39" t="s">
+      <c r="B133" s="66"/>
+      <c r="C133" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D130" s="24" t="s">
+      <c r="D133" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E130" s="24" t="s">
+      <c r="E133" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F130" s="24"/>
-      <c r="G130" s="22" t="s">
+      <c r="F133" s="24"/>
+      <c r="G133" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H130" s="22" t="s">
+      <c r="H133" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="I130" s="19"/>
-    </row>
-    <row r="131" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="53" t="s">
+      <c r="I133" s="19"/>
+    </row>
+    <row r="134" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B131" s="54"/>
-      <c r="C131" s="54"/>
-      <c r="D131" s="54"/>
-      <c r="E131" s="54"/>
-      <c r="F131" s="54"/>
-      <c r="G131" s="58"/>
-      <c r="H131" s="59"/>
-      <c r="I131" s="19"/>
-    </row>
-    <row r="132" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="53" t="s">
+      <c r="B134" s="54"/>
+      <c r="C134" s="54"/>
+      <c r="D134" s="54"/>
+      <c r="E134" s="54"/>
+      <c r="F134" s="54"/>
+      <c r="G134" s="58"/>
+      <c r="H134" s="59"/>
+      <c r="I134" s="19"/>
+    </row>
+    <row r="135" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B132" s="60"/>
-      <c r="C132" s="1" t="s">
+      <c r="B135" s="60"/>
+      <c r="C135" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E132" s="1" t="s">
+      <c r="E135" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F132" s="53" t="s">
+      <c r="F135" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G132" s="54"/>
-      <c r="H132" s="60"/>
-      <c r="I132" s="19"/>
-    </row>
-    <row r="133" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="61" t="s">
+      <c r="G135" s="54"/>
+      <c r="H135" s="60"/>
+      <c r="I135" s="19"/>
+    </row>
+    <row r="136" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="61" t="s">
         <v>148</v>
       </c>
-      <c r="B133" s="62"/>
-      <c r="C133" s="45" t="s">
+      <c r="B136" s="62"/>
+      <c r="C136" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D133" s="45"/>
-      <c r="E133" s="46" t="s">
+      <c r="D136" s="45"/>
+      <c r="E136" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F133" s="63" t="s">
+      <c r="F136" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="G133" s="64"/>
-      <c r="H133" s="62"/>
-      <c r="I133" s="19"/>
-    </row>
-    <row r="134" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="61" t="s">
+      <c r="G136" s="64"/>
+      <c r="H136" s="62"/>
+      <c r="I136" s="19"/>
+    </row>
+    <row r="137" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="B134" s="62"/>
-      <c r="C134" s="45"/>
-      <c r="D134" s="45" t="s">
+      <c r="B137" s="62"/>
+      <c r="C137" s="45"/>
+      <c r="D137" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E134" s="46"/>
-      <c r="F134" s="63" t="s">
+      <c r="E137" s="46"/>
+      <c r="F137" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G134" s="64"/>
-      <c r="H134" s="62"/>
-      <c r="I134" s="12"/>
-    </row>
-    <row r="135" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="61" t="s">
+      <c r="G137" s="64"/>
+      <c r="H137" s="62"/>
+      <c r="I137" s="12"/>
+    </row>
+    <row r="138" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="B135" s="62"/>
-      <c r="C135" s="45"/>
-      <c r="D135" s="45" t="s">
+      <c r="B138" s="62"/>
+      <c r="C138" s="45"/>
+      <c r="D138" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E135" s="46"/>
-      <c r="F135" s="63" t="s">
+      <c r="E138" s="46"/>
+      <c r="F138" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="G135" s="64"/>
-      <c r="H135" s="62"/>
-      <c r="I135" s="12"/>
-    </row>
-    <row r="136" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I136" s="12"/>
-    </row>
-    <row r="137" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I137" s="12"/>
-    </row>
-    <row r="138" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G138" s="64"/>
+      <c r="H138" s="62"/>
       <c r="I138" s="12"/>
     </row>
     <row r="139" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -7432,52 +7520,65 @@
     <row r="1034" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I1034" s="12"/>
     </row>
+    <row r="1035" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1035" s="12"/>
+    </row>
+    <row r="1036" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1036" s="12"/>
+    </row>
+    <row r="1037" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1037" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="176">
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="F48:H48"/>
-    <mergeCell ref="N41:Q41"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="F27:H27"/>
+  <mergeCells count="182">
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="F28:H28"/>
     <mergeCell ref="N26:Q26"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="F137:H137"/>
     <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="N60:Q60"/>
+    <mergeCell ref="N41:Q41"/>
     <mergeCell ref="N61:Q61"/>
-    <mergeCell ref="N93:Q93"/>
+    <mergeCell ref="N62:Q62"/>
     <mergeCell ref="N94:Q94"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="N95:Q95"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="F105:H105"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:H97"/>
-    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:H98"/>
     <mergeCell ref="A99:B99"/>
-    <mergeCell ref="B122:H122"/>
-    <mergeCell ref="B121:H121"/>
-    <mergeCell ref="A103:H106"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A117:H120"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="B125:H125"/>
+    <mergeCell ref="B124:H124"/>
+    <mergeCell ref="A106:H109"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A120:H123"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
@@ -7486,17 +7587,19 @@
     <mergeCell ref="A13:H16"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="B18:H18"/>
-    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:H35"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A28:H31"/>
+    <mergeCell ref="A29:H32"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="B32:H32"/>
     <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="F27:H27"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
@@ -7506,75 +7609,75 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="A49:H52"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="F48:H48"/>
+    <mergeCell ref="A50:H53"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="B55:H55"/>
+    <mergeCell ref="A56:H56"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="B72:H72"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="B73:H73"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B74:H74"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:B59"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A66:H66"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="F67:H67"/>
-    <mergeCell ref="A68:H71"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="A69:H72"/>
+    <mergeCell ref="A91:B91"/>
     <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A74:H74"/>
-    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A75:H75"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:H80"/>
     <mergeCell ref="F81:H81"/>
-    <mergeCell ref="B86:H86"/>
-    <mergeCell ref="A82:H85"/>
-    <mergeCell ref="K86:Q86"/>
-    <mergeCell ref="B108:H108"/>
-    <mergeCell ref="B107:H107"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="B87:H87"/>
+    <mergeCell ref="A83:H86"/>
+    <mergeCell ref="K87:Q87"/>
+    <mergeCell ref="B111:H111"/>
+    <mergeCell ref="B110:H110"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A116:H116"/>
     <mergeCell ref="A115:B115"/>
-    <mergeCell ref="F114:H114"/>
     <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A113:H113"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A109:H109"/>
-    <mergeCell ref="K87:Q87"/>
-    <mergeCell ref="J88:Q88"/>
-    <mergeCell ref="P89:Q89"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A112:H112"/>
+    <mergeCell ref="K88:Q88"/>
+    <mergeCell ref="J89:Q89"/>
     <mergeCell ref="P90:Q90"/>
     <mergeCell ref="P91:Q91"/>
-    <mergeCell ref="B87:H87"/>
-    <mergeCell ref="A88:H88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="B88:H88"/>
+    <mergeCell ref="A89:H89"/>
+    <mergeCell ref="A90:B90"/>
     <mergeCell ref="P57:Q57"/>
     <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="J59:Q59"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="J60:Q60"/>
     <mergeCell ref="K17:Q17"/>
     <mergeCell ref="K18:Q18"/>
     <mergeCell ref="J19:Q19"/>
@@ -7584,34 +7687,34 @@
     <mergeCell ref="J23:Q23"/>
     <mergeCell ref="N24:Q24"/>
     <mergeCell ref="N25:Q25"/>
-    <mergeCell ref="K32:Q32"/>
-    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="K33:Q33"/>
     <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="K33:Q33"/>
-    <mergeCell ref="J38:Q38"/>
-    <mergeCell ref="J34:Q34"/>
     <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="K34:Q34"/>
+    <mergeCell ref="J39:Q39"/>
+    <mergeCell ref="J35:Q35"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="J56:Q56"/>
     <mergeCell ref="K54:Q54"/>
-    <mergeCell ref="J55:Q55"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="J92:Q92"/>
-    <mergeCell ref="A131:H131"/>
+    <mergeCell ref="J93:Q93"/>
+    <mergeCell ref="A134:H134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="A131:B131"/>
     <mergeCell ref="A132:B132"/>
-    <mergeCell ref="F132:H132"/>
     <mergeCell ref="A133:B133"/>
-    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="A127:B127"/>
     <mergeCell ref="A128:B128"/>
     <mergeCell ref="A129:B129"/>
     <mergeCell ref="A130:B130"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A123:H123"/>
+    <mergeCell ref="A126:H126"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>